<commit_message>
Katalog guncellendi - Sal 04.11.2025 16:54:46,88
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\SIVAL_GIYIM_KATALOG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF10C62-1DAC-4222-8BB7-BF557832F18D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -85,7 +85,7 @@
     <t>4616.png</t>
   </si>
   <si>
-    <t>çilek</t>
+    <t>çilek2</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Katalog guncellendi - Sal 04.11.2025 17:07:33,46
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\SIVAL_GIYIM_KATALOG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1493D8A0-A25E-496E-930D-CB16FBA30229}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>urun_adi</t>
   </si>
@@ -86,6 +86,21 @@
   </si>
   <si>
     <t>çilek2</t>
+  </si>
+  <si>
+    <t>Baggy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">350 TL </t>
+  </si>
+  <si>
+    <t>Jeans</t>
+  </si>
+  <si>
+    <t>BAG1.jpg</t>
+  </si>
+  <si>
+    <t>100% Pamuk</t>
   </si>
 </sst>
 </file>
@@ -458,7 +473,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,6 +562,26 @@
         <v>15</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E8" s="2"/>
     </row>

</xml_diff>

<commit_message>
Katalog guncellendi - Çar 05.11.2025  8:33:03,75
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1493D8A0-A25E-496E-930D-CB16FBA30229}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3DA050E-F739-4B53-8048-A7FB2AC8DD5A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>urun_adi</t>
   </si>
@@ -40,57 +40,9 @@
     <t>stok</t>
   </si>
   <si>
-    <t>450 TL</t>
-  </si>
-  <si>
-    <t>Takı</t>
-  </si>
-  <si>
-    <t>14 ayar altın kolye</t>
-  </si>
-  <si>
     <t>Var</t>
   </si>
   <si>
-    <t>180 TL</t>
-  </si>
-  <si>
-    <t>925 ayar gümüş küpe</t>
-  </si>
-  <si>
-    <t>120 TL</t>
-  </si>
-  <si>
-    <t>Kozmetik</t>
-  </si>
-  <si>
-    <t>5'li mat ruj seti</t>
-  </si>
-  <si>
-    <t>Yok</t>
-  </si>
-  <si>
-    <t>elma</t>
-  </si>
-  <si>
-    <t>armut</t>
-  </si>
-  <si>
-    <t>4602.png</t>
-  </si>
-  <si>
-    <t>4609.png</t>
-  </si>
-  <si>
-    <t>4616.png</t>
-  </si>
-  <si>
-    <t>çilek2</t>
-  </si>
-  <si>
-    <t>Baggy</t>
-  </si>
-  <si>
     <t xml:space="preserve">350 TL </t>
   </si>
   <si>
@@ -101,6 +53,15 @@
   </si>
   <si>
     <t>100% Pamuk</t>
+  </si>
+  <si>
+    <t>BAG2.jpg</t>
+  </si>
+  <si>
+    <t>Baggy Mavi</t>
+  </si>
+  <si>
+    <t>Baggy Gri</t>
   </si>
 </sst>
 </file>
@@ -473,7 +434,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,82 +465,42 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
       <c r="F3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Katalog guncellendi - Çar 05.11.2025  8:39:19,12
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3DA050E-F739-4B53-8048-A7FB2AC8DD5A}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB4036AC-5CCD-454D-B95A-E2AE8FE89B72}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>urun_adi</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Var</t>
   </si>
   <si>
-    <t xml:space="preserve">350 TL </t>
-  </si>
-  <si>
     <t>Jeans</t>
   </si>
   <si>
@@ -62,6 +59,18 @@
   </si>
   <si>
     <t>Baggy Gri</t>
+  </si>
+  <si>
+    <t>Baggy Siyah</t>
+  </si>
+  <si>
+    <t>300 TL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">300 TL </t>
+  </si>
+  <si>
+    <t>BAG6.jpg</t>
   </si>
 </sst>
 </file>
@@ -434,7 +443,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,19 +474,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
@@ -485,21 +494,41 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Katalog guncellendi - Sal 11.11.2025 11:12:12,43
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB4036AC-5CCD-454D-B95A-E2AE8FE89B72}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC712864-80F3-4978-AF94-3784A0920830}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>urun_adi</t>
   </si>
@@ -49,9 +49,6 @@
     <t>BAG1.jpg</t>
   </si>
   <si>
-    <t>100% Pamuk</t>
-  </si>
-  <si>
     <t>BAG2.jpg</t>
   </si>
   <si>
@@ -71,6 +68,18 @@
   </si>
   <si>
     <t>BAG6.jpg</t>
+  </si>
+  <si>
+    <t>Baggy Füme</t>
+  </si>
+  <si>
+    <t>300 tl</t>
+  </si>
+  <si>
+    <t>BAG3.jpg</t>
+  </si>
+  <si>
+    <t>Erkek baggy pantolon, bol ve rahat kesimiyle öne çıkan, modern sokak stilinin vazgeçilmez parçasıdır. Kalçadan paçaya kadar geniş formu sayesinde hareket özgürlüğü sunar.Ürün içeriği 100% Pamuk. Rahatlığından ödün vermeden tarzını yansıtmak isteyen erkekler için ideal bir seçimdir.29-38 Beden beden seçeneği mevcuttur.</t>
   </si>
 </sst>
 </file>
@@ -443,13 +452,14 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.28515625" customWidth="1"/>
     <col min="4" max="4" width="25.28515625" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -474,10 +484,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -486,7 +496,7 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
@@ -494,19 +504,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
@@ -514,21 +524,41 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Katalog guncellendi - Sal 11.11.2025 11:30:27,18
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC712864-80F3-4978-AF94-3784A0920830}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03479F0E-0CB9-401F-8D1B-126B4ED6D1F9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,7 +79,7 @@
     <t>BAG3.jpg</t>
   </si>
   <si>
-    <t>Erkek baggy pantolon, bol ve rahat kesimiyle öne çıkan, modern sokak stilinin vazgeçilmez parçasıdır. Kalçadan paçaya kadar geniş formu sayesinde hareket özgürlüğü sunar.Ürün içeriği 100% Pamuk. Rahatlığından ödün vermeden tarzını yansıtmak isteyen erkekler için ideal bir seçimdir.29-38 Beden beden seçeneği mevcuttur.</t>
+    <t>Erkek baggy pantolon, bol ve rahat kesimiyle öne çıkan, modern sokak stilinin vazgeçilmez parçasıdır. Kalçadan paçaya kadar geniş formu sayesinde hareket özgürlüğü sunar.Ürün içeriği 100% Pamuk. Rahatlığından ödün vermeden tarzını yansıtmak isteyen erkekler için ideal bir seçimdir.29-38  beden seçeneği mevcuttur.</t>
   </si>
 </sst>
 </file>
@@ -452,7 +452,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Katalog guncellendi - Sal 11.11.2025 11:33:04,76
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03479F0E-0CB9-401F-8D1B-126B4ED6D1F9}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40C3D814-216C-4B01-A01C-5B6A16C4C6F7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -452,7 +452,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Katalog guncellendi - Çar 12.11.2025 15:56:14,56
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40C3D814-216C-4B01-A01C-5B6A16C4C6F7}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6B770FB-BE58-4FD0-A3EC-30ECC6790D2F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>urun_adi</t>
   </si>
@@ -73,13 +73,19 @@
     <t>Baggy Füme</t>
   </si>
   <si>
-    <t>300 tl</t>
-  </si>
-  <si>
     <t>BAG3.jpg</t>
   </si>
   <si>
-    <t>Erkek baggy pantolon, bol ve rahat kesimiyle öne çıkan, modern sokak stilinin vazgeçilmez parçasıdır. Kalçadan paçaya kadar geniş formu sayesinde hareket özgürlüğü sunar.Ürün içeriği 100% Pamuk. Rahatlığından ödün vermeden tarzını yansıtmak isteyen erkekler için ideal bir seçimdir.29-38  beden seçeneği mevcuttur.</t>
+    <t>Baggy Kar Yıkama</t>
+  </si>
+  <si>
+    <t>300 Tl</t>
+  </si>
+  <si>
+    <t>BAG4.jpg</t>
+  </si>
+  <si>
+    <t>Erkek baggy pantolon, bol ve rahat kesimiyle öne çıkan, modern sokak stilinin vazgeçilmez parçasıdır. Kalçadan paçaya kadar geniş formu sayesinde hareket özgürlüğü sunar.Ürün içeriği 100% Pamuk.29-38  beden seçeneği mevcuttur.</t>
   </si>
 </sst>
 </file>
@@ -452,14 +458,14 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.28515625" customWidth="1"/>
     <col min="4" max="4" width="25.28515625" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -496,7 +502,7 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
@@ -516,7 +522,7 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
@@ -536,7 +542,7 @@
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
         <v>6</v>
@@ -547,18 +553,38 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
+      <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="F5" t="s">
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Katalog guncellendi - Cum 14.11.2025  9:48:30,89
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6B770FB-BE58-4FD0-A3EC-30ECC6790D2F}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC9D9DAD-53E0-4319-AC52-884F8E248526}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
   <si>
     <t>urun_adi</t>
   </si>
@@ -86,6 +86,12 @@
   </si>
   <si>
     <t>Erkek baggy pantolon, bol ve rahat kesimiyle öne çıkan, modern sokak stilinin vazgeçilmez parçasıdır. Kalçadan paçaya kadar geniş formu sayesinde hareket özgürlüğü sunar.Ürün içeriği 100% Pamuk.29-38  beden seçeneği mevcuttur.</t>
+  </si>
+  <si>
+    <t>Baggy Koyu Mavi</t>
+  </si>
+  <si>
+    <t>BAG5.jpg</t>
   </si>
 </sst>
 </file>
@@ -458,7 +464,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,6 +594,26 @@
         <v>6</v>
       </c>
     </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E8" s="2"/>
     </row>

</xml_diff>

<commit_message>
Katalog guncellendi - Cum 14.11.2025 10:30:35,36
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC9D9DAD-53E0-4319-AC52-884F8E248526}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0A9B3D6-AD4C-43B6-A691-A92087D1D128}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
   <si>
     <t>urun_adi</t>
   </si>
@@ -92,6 +92,18 @@
   </si>
   <si>
     <t>BAG5.jpg</t>
+  </si>
+  <si>
+    <t>Bel Paça Lastik  Pantolon</t>
+  </si>
+  <si>
+    <t>350 Tl</t>
+  </si>
+  <si>
+    <t>ANTRASİT.jpg</t>
+  </si>
+  <si>
+    <t>%98 pamuk içeriği ile nefes alabilen yapıda, cildinize nazik dokunuşlar sunar.Bağcıklı kapama şekliyle kişisel zevke göre ayarlama imkanı taşır.Lastikli bel detayı sayesinde  rahatlığından ödün vermez.34-46 Beden aralığı mevcuttur.</t>
   </si>
 </sst>
 </file>
@@ -463,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,7 +627,21 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E8" s="2"/>
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Katalog guncellendi - Cum 14.11.2025 10:40:31,95
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0A9B3D6-AD4C-43B6-A691-A92087D1D128}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{099BBEA2-22B3-4BC8-9F58-63BB1617CFCE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
   <si>
     <t>urun_adi</t>
   </si>
@@ -94,9 +94,6 @@
     <t>BAG5.jpg</t>
   </si>
   <si>
-    <t>Bel Paça Lastik  Pantolon</t>
-  </si>
-  <si>
     <t>350 Tl</t>
   </si>
   <si>
@@ -104,6 +101,21 @@
   </si>
   <si>
     <t>%98 pamuk içeriği ile nefes alabilen yapıda, cildinize nazik dokunuşlar sunar.Bağcıklı kapama şekliyle kişisel zevke göre ayarlama imkanı taşır.Lastikli bel detayı sayesinde  rahatlığından ödün vermez.34-46 Beden aralığı mevcuttur.</t>
+  </si>
+  <si>
+    <t>Bel Paça Lastik  Pantolon Antrasit</t>
+  </si>
+  <si>
+    <t>Bel Paça Lastik  Pantolon Gri</t>
+  </si>
+  <si>
+    <t>Bel Paça Lastik  Pantolon Füme</t>
+  </si>
+  <si>
+    <t>GRİ.jpg</t>
+  </si>
+  <si>
+    <t>MAVİİ.jpg</t>
   </si>
 </sst>
 </file>
@@ -473,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,19 +640,53 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
         <v>24</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
         <v>25</v>
       </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>27</v>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Katalog guncellendi - Cum 14.11.2025 10:45:01,80
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="92" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{099BBEA2-22B3-4BC8-9F58-63BB1617CFCE}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{614C7311-2985-4B4D-B93E-153BB0A14516}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -97,9 +97,6 @@
     <t>350 Tl</t>
   </si>
   <si>
-    <t>ANTRASİT.jpg</t>
-  </si>
-  <si>
     <t>%98 pamuk içeriği ile nefes alabilen yapıda, cildinize nazik dokunuşlar sunar.Bağcıklı kapama şekliyle kişisel zevke göre ayarlama imkanı taşır.Lastikli bel detayı sayesinde  rahatlığından ödün vermez.34-46 Beden aralığı mevcuttur.</t>
   </si>
   <si>
@@ -116,6 +113,9 @@
   </si>
   <si>
     <t>MAVİİ.jpg</t>
+  </si>
+  <si>
+    <t>ANRASİT.jpg</t>
   </si>
 </sst>
 </file>
@@ -488,7 +488,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,7 +640,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
         <v>24</v>
@@ -649,15 +649,15 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
         <v>24</v>
@@ -666,15 +666,15 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
         <v>24</v>
@@ -683,10 +683,10 @@
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Katalog guncellendi - Cum 14.11.2025 10:47:42,04
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="94" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{614C7311-2985-4B4D-B93E-153BB0A14516}"/>
+  <xr:revisionPtr revIDLastSave="95" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0C7C894-A500-43DC-B3D2-5BCBA15EE170}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5325" yWindow="3720" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -106,9 +106,6 @@
     <t>Bel Paça Lastik  Pantolon Gri</t>
   </si>
   <si>
-    <t>Bel Paça Lastik  Pantolon Füme</t>
-  </si>
-  <si>
     <t>GRİ.jpg</t>
   </si>
   <si>
@@ -116,6 +113,9 @@
   </si>
   <si>
     <t>ANRASİT.jpg</t>
+  </si>
+  <si>
+    <t>Bel Paça Lastik  Pantolon Mavi</t>
   </si>
 </sst>
 </file>
@@ -488,7 +488,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,7 +649,7 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>25</v>
@@ -666,7 +666,7 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
         <v>25</v>
@@ -674,7 +674,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
         <v>24</v>
@@ -683,7 +683,7 @@
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Katalog guncellendi - Cum 14.11.2025 11:27:17,39
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="95" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0C7C894-A500-43DC-B3D2-5BCBA15EE170}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26092B41-C976-446D-80B7-D26ACA716CB2}"/>
   <bookViews>
     <workbookView xWindow="5325" yWindow="3720" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="79">
   <si>
     <t>urun_adi</t>
   </si>
@@ -116,13 +116,154 @@
   </si>
   <si>
     <t>Bel Paça Lastik  Pantolon Mavi</t>
+  </si>
+  <si>
+    <t>Gömlek</t>
+  </si>
+  <si>
+    <t>BEJ.jpg</t>
+  </si>
+  <si>
+    <t>%85 pamuk, %12 polyester ve %3 spandex karışımından oluşan materyali ile konforlu bir deneyim sağlar.S-M-L-XL-2XL Beden seçeneği mevcuttur.</t>
+  </si>
+  <si>
+    <t>Kot Gömlek Bej</t>
+  </si>
+  <si>
+    <t>Kot Gömlek Bordo</t>
+  </si>
+  <si>
+    <t>BORDOKOTGMLK.jpg</t>
+  </si>
+  <si>
+    <t>var</t>
+  </si>
+  <si>
+    <t>Kot Gömlek Denim Blue</t>
+  </si>
+  <si>
+    <t>DENİMBLUEKOTGMLK.jpg</t>
+  </si>
+  <si>
+    <t>Kot Gömlek Fıstık Yeşili</t>
+  </si>
+  <si>
+    <t>FISTIKYEŞİLİ.jpg</t>
+  </si>
+  <si>
+    <t>Kot Gömlek Füme</t>
+  </si>
+  <si>
+    <t>FÜMEKOTGMLK.jpg</t>
+  </si>
+  <si>
+    <t>Kot Gömlek Kahverengi</t>
+  </si>
+  <si>
+    <t>KAHVERENGİ.jpg</t>
+  </si>
+  <si>
+    <t>Kot Gömlek Kraliyet Mavisi</t>
+  </si>
+  <si>
+    <t>KRALİYET MAVİSİ.jpg</t>
+  </si>
+  <si>
+    <t>Kot Gömlek Peygamber Çiçeği</t>
+  </si>
+  <si>
+    <t>PEYGAMBERÇİÇEĞİ.jpg</t>
+  </si>
+  <si>
+    <t>Kot Gömlek Siyah</t>
+  </si>
+  <si>
+    <t>SİYAHKOTGMLK.jpg</t>
+  </si>
+  <si>
+    <t>Kot Gömlek Mavi</t>
+  </si>
+  <si>
+    <t>MAVİKOTGMLK.jpg</t>
+  </si>
+  <si>
+    <t>Kot Gömlek Taş</t>
+  </si>
+  <si>
+    <t>TAŞ.jpg</t>
+  </si>
+  <si>
+    <t>YEŞİLİN51.TONU.jpg</t>
+  </si>
+  <si>
+    <t>Kot Gömlek Yeşilin 51. Tonu</t>
+  </si>
+  <si>
+    <t>GÖMLEK CEKETDENİMBLUE.jpg</t>
+  </si>
+  <si>
+    <t>Kot Gömlek Ceket Denim Blue</t>
+  </si>
+  <si>
+    <t>%100 pamuk materyali ile üretilmiş, Çıt çıt kapama şekliyle güvenli bir kullanım sağlar.İki tarz tek parçada;Hem gömlek hem ceket.XS-S /  M-L /  XL-2XL Beden seçeneği Mevcuttur.</t>
+  </si>
+  <si>
+    <t>400 Tl</t>
+  </si>
+  <si>
+    <t>Kot Gömlek Ceket Mavi</t>
+  </si>
+  <si>
+    <t>GÖMLEK CEKETMAVİ.jpg</t>
+  </si>
+  <si>
+    <t>Kot Gömlek Ceket Kar Yıkama</t>
+  </si>
+  <si>
+    <t>GÖMLEKCEKETBUZMAVİSİ.jpg</t>
+  </si>
+  <si>
+    <t>EŞREFAÇIKMAVİ.jpg</t>
+  </si>
+  <si>
+    <t>Eşref Gömlek Açık Mavi</t>
+  </si>
+  <si>
+    <t>260 Tl</t>
+  </si>
+  <si>
+    <t>Polyester materyali sayesinde hafifliğiyle konforlu bir kullanım sunarken dayanıklılığından da taviz vermez.Uzun kollu oluşu soğuk havalarda ekstra koruma sağlarken çizgili deseniyle trendleri takip eder.S-M-L-XL-2XL Beden seçeneği mevcuttur.</t>
+  </si>
+  <si>
+    <t>Eşref Gömlek Bej</t>
+  </si>
+  <si>
+    <t>EŞREFBEJ.jpg</t>
+  </si>
+  <si>
+    <t>Eşref Gömlek Beyaz</t>
+  </si>
+  <si>
+    <t>EŞREFBEYAZ.jpg</t>
+  </si>
+  <si>
+    <t>Eşref Gömlek Koyu Mavi</t>
+  </si>
+  <si>
+    <t>EŞREFKOYUMAVİ.jpg</t>
+  </si>
+  <si>
+    <t>EŞREFSİYAH.jpg</t>
+  </si>
+  <si>
+    <t>Eşref Gömlek Siyah</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,6 +281,19 @@
       <color rgb="FF666666"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF666666"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
     </font>
   </fonts>
   <fills count="2">
@@ -177,12 +331,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,6 +809,9 @@
       <c r="E8" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="F8" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -671,6 +829,9 @@
       <c r="E9" t="s">
         <v>25</v>
       </c>
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -688,8 +849,412 @@
       <c r="E10" t="s">
         <v>25</v>
       </c>
+      <c r="F10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" t="s">
+        <v>61</v>
+      </c>
+      <c r="F24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" t="s">
+        <v>67</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" t="s">
+        <v>74</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>78</v>
+      </c>
+      <c r="B30" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" t="s">
+        <v>77</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F30" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Katalog guncellendi - Cum 14.11.2025 11:32:48,27
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26092B41-C976-446D-80B7-D26ACA716CB2}"/>
+  <xr:revisionPtr revIDLastSave="116" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E235233-3577-47F3-86FB-3E228D889202}"/>
   <bookViews>
     <workbookView xWindow="5325" yWindow="3720" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -124,9 +124,6 @@
     <t>BEJ.jpg</t>
   </si>
   <si>
-    <t>%85 pamuk, %12 polyester ve %3 spandex karışımından oluşan materyali ile konforlu bir deneyim sağlar.S-M-L-XL-2XL Beden seçeneği mevcuttur.</t>
-  </si>
-  <si>
     <t>Kot Gömlek Bej</t>
   </si>
   <si>
@@ -205,9 +202,6 @@
     <t>Kot Gömlek Ceket Denim Blue</t>
   </si>
   <si>
-    <t>%100 pamuk materyali ile üretilmiş, Çıt çıt kapama şekliyle güvenli bir kullanım sağlar.İki tarz tek parçada;Hem gömlek hem ceket.XS-S /  M-L /  XL-2XL Beden seçeneği Mevcuttur.</t>
-  </si>
-  <si>
     <t>400 Tl</t>
   </si>
   <si>
@@ -232,9 +226,6 @@
     <t>260 Tl</t>
   </si>
   <si>
-    <t>Polyester materyali sayesinde hafifliğiyle konforlu bir kullanım sunarken dayanıklılığından da taviz vermez.Uzun kollu oluşu soğuk havalarda ekstra koruma sağlarken çizgili deseniyle trendleri takip eder.S-M-L-XL-2XL Beden seçeneği mevcuttur.</t>
-  </si>
-  <si>
     <t>Eşref Gömlek Bej</t>
   </si>
   <si>
@@ -257,6 +248,15 @@
   </si>
   <si>
     <t>Eşref Gömlek Siyah</t>
+  </si>
+  <si>
+    <t>Polyester materyali sayesinde hafifliğiyle konforlu bir kullanım sunarken dayanıklılığından da taviz vermez.Uzun kollu oluşu soğuk havalarda ekstra koruma sağlarken çizgili deseniyle trendleri takip eder.S-M-L-XL-2XL Beden seçeneği mevcuttur.Ürünümüz serili olarak satılmaktadır.</t>
+  </si>
+  <si>
+    <t>%100 pamuk materyali ile üretilmiş, Çıt çıt kapama şekliyle güvenli bir kullanım sağlar.İki tarz tek parçada;Hem gömlek hem ceket.XS-S /  M-L /  XL-2XL Beden seçeneği Mevcuttur.Ürünümüz tekli olarak satın alınabilir.</t>
+  </si>
+  <si>
+    <t>%85 pamuk, %12 polyester ve %3 spandex karışımından oluşan materyali ile konforlu bir deneyim sağlar.S-M-L-XL-2XL Beden seçeneği mevcuttur.Ürünümüz tekli olarak satın alınabilir.</t>
   </si>
 </sst>
 </file>
@@ -642,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,7 +810,7 @@
         <v>25</v>
       </c>
       <c r="F8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -855,7 +855,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
@@ -867,7 +867,7 @@
         <v>33</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="F11" t="s">
         <v>6</v>
@@ -875,19 +875,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
         <v>36</v>
       </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" t="s">
-        <v>37</v>
-      </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="F12" t="s">
         <v>6</v>
@@ -895,19 +895,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
         <v>39</v>
       </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" t="s">
-        <v>40</v>
-      </c>
       <c r="E13" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="F13" t="s">
         <v>6</v>
@@ -915,19 +915,19 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
         <v>41</v>
       </c>
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" t="s">
-        <v>42</v>
-      </c>
       <c r="E14" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="F14" t="s">
         <v>6</v>
@@ -935,19 +935,19 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" t="s">
         <v>43</v>
       </c>
-      <c r="B15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" t="s">
-        <v>44</v>
-      </c>
       <c r="E15" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="F15" t="s">
         <v>6</v>
@@ -955,19 +955,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
         <v>45</v>
       </c>
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" t="s">
-        <v>46</v>
-      </c>
       <c r="E16" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="F16" t="s">
         <v>6</v>
@@ -975,19 +975,19 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" t="s">
         <v>47</v>
       </c>
-      <c r="B17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" t="s">
-        <v>48</v>
-      </c>
       <c r="E17" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="F17" t="s">
         <v>6</v>
@@ -995,19 +995,19 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s">
         <v>49</v>
       </c>
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" t="s">
-        <v>50</v>
-      </c>
       <c r="E18" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="F18" t="s">
         <v>6</v>
@@ -1015,19 +1015,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" t="s">
         <v>51</v>
       </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" t="s">
-        <v>52</v>
-      </c>
       <c r="E19" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="F19" t="s">
         <v>6</v>
@@ -1035,19 +1035,19 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" t="s">
         <v>53</v>
       </c>
-      <c r="B20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" t="s">
-        <v>54</v>
-      </c>
       <c r="E20" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="F20" t="s">
         <v>6</v>
@@ -1055,19 +1055,19 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" t="s">
         <v>55</v>
       </c>
-      <c r="B21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" t="s">
-        <v>56</v>
-      </c>
       <c r="E21" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="F21" t="s">
         <v>6</v>
@@ -1075,7 +1075,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B22" t="s">
         <v>19</v>
@@ -1084,10 +1084,10 @@
         <v>32</v>
       </c>
       <c r="D22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E22" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="F22" t="s">
         <v>6</v>
@@ -1095,19 +1095,19 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" t="s">
         <v>60</v>
       </c>
-      <c r="B23" t="s">
-        <v>62</v>
-      </c>
       <c r="C23" t="s">
         <v>32</v>
       </c>
       <c r="D23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E23" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="F23" t="s">
         <v>6</v>
@@ -1115,19 +1115,19 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" t="s">
         <v>62</v>
       </c>
-      <c r="C24" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" t="s">
-        <v>64</v>
-      </c>
       <c r="E24" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="F24" t="s">
         <v>6</v>
@@ -1135,19 +1135,19 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C25" t="s">
         <v>32</v>
       </c>
       <c r="D25" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E25" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="F25" t="s">
         <v>6</v>
@@ -1155,19 +1155,19 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C26" t="s">
         <v>32</v>
       </c>
       <c r="D26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="F26" t="s">
         <v>6</v>
@@ -1175,19 +1175,19 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B27" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" t="s">
         <v>69</v>
       </c>
-      <c r="C27" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27" t="s">
-        <v>72</v>
-      </c>
       <c r="E27" s="3" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="F27" t="s">
         <v>6</v>
@@ -1195,19 +1195,19 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C28" t="s">
         <v>32</v>
       </c>
       <c r="D28" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="F28" t="s">
         <v>6</v>
@@ -1215,19 +1215,19 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C29" t="s">
         <v>32</v>
       </c>
       <c r="D29" t="s">
+        <v>73</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="F29" t="s">
         <v>6</v>
@@ -1235,19 +1235,19 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C30" t="s">
         <v>32</v>
       </c>
       <c r="D30" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="F30" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Katalog guncellendi - Cum 14.11.2025 11:50:33,32
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="116" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E235233-3577-47F3-86FB-3E228D889202}"/>
+  <xr:revisionPtr revIDLastSave="117" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BBDCB67-7B23-470C-B6D4-04BB9C811B88}"/>
   <bookViews>
-    <workbookView xWindow="5325" yWindow="3720" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="95">
   <si>
     <t>urun_adi</t>
   </si>
@@ -257,6 +257,54 @@
   </si>
   <si>
     <t>%85 pamuk, %12 polyester ve %3 spandex karışımından oluşan materyali ile konforlu bir deneyim sağlar.S-M-L-XL-2XL Beden seçeneği mevcuttur.Ürünümüz tekli olarak satın alınabilir.</t>
+  </si>
+  <si>
+    <t>KETENANTRASİT.jpg</t>
+  </si>
+  <si>
+    <t>360 Tl</t>
+  </si>
+  <si>
+    <t>Slim fit chino keten pantolon, pamuk ve polyester karışımından oluşan orta kalınlığa sahip kumaşı, konforlu bir kullanım vaat eder.Nefes alan kumaşı ile yaz aylarında serin tutar, terletmez.31-38 Beden seçeneği mevcuttur.Ürünümüz serili olarak satılmaktadır.</t>
+  </si>
+  <si>
+    <t>Chino Keten Pantolon Antrasit</t>
+  </si>
+  <si>
+    <t>KETENBEJ.jpg</t>
+  </si>
+  <si>
+    <t>Chino Keten Pantolon Bej</t>
+  </si>
+  <si>
+    <t>Chino Keten Pantolon Gri</t>
+  </si>
+  <si>
+    <t>KETENGRİ.jpg</t>
+  </si>
+  <si>
+    <t>Chino Keten Pantolon Mavi</t>
+  </si>
+  <si>
+    <t>KETENMAVİ.jpg</t>
+  </si>
+  <si>
+    <t>Chino Keten Pantolon Siyah</t>
+  </si>
+  <si>
+    <t>KETENSİYAH.jpg</t>
+  </si>
+  <si>
+    <t>Chino Keten Pantolon Taş</t>
+  </si>
+  <si>
+    <t>KETENTAŞ.jpg</t>
+  </si>
+  <si>
+    <t>Chino Keten Pantolon Yeşil</t>
+  </si>
+  <si>
+    <t>YEŞİLKETEN.jpg</t>
   </si>
 </sst>
 </file>
@@ -640,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1253,6 +1301,146 @@
         <v>6</v>
       </c>
     </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" t="s">
+        <v>79</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>84</v>
+      </c>
+      <c r="B32" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" t="s">
+        <v>83</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33" t="s">
+        <v>80</v>
+      </c>
+      <c r="C33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" t="s">
+        <v>86</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" t="s">
+        <v>88</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" t="s">
+        <v>90</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" t="s">
+        <v>80</v>
+      </c>
+      <c r="C36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" t="s">
+        <v>92</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" t="s">
+        <v>94</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F37" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Katalog guncellendi - Cum 14.11.2025 12:12:13,69
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="117" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BBDCB67-7B23-470C-B6D4-04BB9C811B88}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0ACB715-F6C5-4B64-860D-EF4B1DFE7CDB}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="96">
   <si>
     <t>urun_adi</t>
   </si>
@@ -85,9 +85,6 @@
     <t>BAG4.jpg</t>
   </si>
   <si>
-    <t>Erkek baggy pantolon, bol ve rahat kesimiyle öne çıkan, modern sokak stilinin vazgeçilmez parçasıdır. Kalçadan paçaya kadar geniş formu sayesinde hareket özgürlüğü sunar.Ürün içeriği 100% Pamuk.29-38  beden seçeneği mevcuttur.</t>
-  </si>
-  <si>
     <t>Baggy Koyu Mavi</t>
   </si>
   <si>
@@ -97,9 +94,6 @@
     <t>350 Tl</t>
   </si>
   <si>
-    <t>%98 pamuk içeriği ile nefes alabilen yapıda, cildinize nazik dokunuşlar sunar.Bağcıklı kapama şekliyle kişisel zevke göre ayarlama imkanı taşır.Lastikli bel detayı sayesinde  rahatlığından ödün vermez.34-46 Beden aralığı mevcuttur.</t>
-  </si>
-  <si>
     <t>Bel Paça Lastik  Pantolon Antrasit</t>
   </si>
   <si>
@@ -250,24 +244,12 @@
     <t>Eşref Gömlek Siyah</t>
   </si>
   <si>
-    <t>Polyester materyali sayesinde hafifliğiyle konforlu bir kullanım sunarken dayanıklılığından da taviz vermez.Uzun kollu oluşu soğuk havalarda ekstra koruma sağlarken çizgili deseniyle trendleri takip eder.S-M-L-XL-2XL Beden seçeneği mevcuttur.Ürünümüz serili olarak satılmaktadır.</t>
-  </si>
-  <si>
-    <t>%100 pamuk materyali ile üretilmiş, Çıt çıt kapama şekliyle güvenli bir kullanım sağlar.İki tarz tek parçada;Hem gömlek hem ceket.XS-S /  M-L /  XL-2XL Beden seçeneği Mevcuttur.Ürünümüz tekli olarak satın alınabilir.</t>
-  </si>
-  <si>
-    <t>%85 pamuk, %12 polyester ve %3 spandex karışımından oluşan materyali ile konforlu bir deneyim sağlar.S-M-L-XL-2XL Beden seçeneği mevcuttur.Ürünümüz tekli olarak satın alınabilir.</t>
-  </si>
-  <si>
     <t>KETENANTRASİT.jpg</t>
   </si>
   <si>
     <t>360 Tl</t>
   </si>
   <si>
-    <t>Slim fit chino keten pantolon, pamuk ve polyester karışımından oluşan orta kalınlığa sahip kumaşı, konforlu bir kullanım vaat eder.Nefes alan kumaşı ile yaz aylarında serin tutar, terletmez.31-38 Beden seçeneği mevcuttur.Ürünümüz serili olarak satılmaktadır.</t>
-  </si>
-  <si>
     <t>Chino Keten Pantolon Antrasit</t>
   </si>
   <si>
@@ -305,6 +287,27 @@
   </si>
   <si>
     <t>YEŞİLKETEN.jpg</t>
+  </si>
+  <si>
+    <t>Regular Fit Kot Pantolon Hein</t>
+  </si>
+  <si>
+    <t>%100 pamuk materyali ile üretilmiş, Çıt çıt kapama şekliyle güvenli bir kullanım sağlar.İki tarz tek parçada;Hem gömlek hem ceket.XS-S /  M-L /  XL-2XL Beden seçeneği Mevcuttur.Ürünümüz tekli olarak satın alınabilir.Belirtilen fiyatlar adet fiyatıdır.</t>
+  </si>
+  <si>
+    <t>Erkek baggy pantolon, bol ve rahat kesimiyle öne çıkan, modern sokak stilinin vazgeçilmez parçasıdır. Kalçadan paçaya kadar geniş formu sayesinde hareket özgürlüğü sunar.Ürün içeriği 100% Pamuk.29-38  beden seçeneği mevcuttur.Ürünümüz tekli olarak satın alınabilir.Belirtilen fiyatlar adet fiyatıdır.</t>
+  </si>
+  <si>
+    <t>%98 pamuk içeriği ile nefes alabilen yapıda, cildinize nazik dokunuşlar sunar.Bağcıklı kapama şekliyle kişisel zevke göre ayarlama imkanı taşır.Lastikli bel detayı sayesinde  rahatlığından ödün vermez.34-46 Beden aralığı mevcuttur.Ürünümüz tekli olarak satın alınabilir.Belirtilen fiyatlar adet fiyatıdır.</t>
+  </si>
+  <si>
+    <t>%85 pamuk, %12 polyester ve %3 spandex karışımından oluşan materyali ile konforlu bir deneyim sağlar.S-M-L-XL-2XL Beden seçeneği mevcuttur.Ürünümüz tekli olarak satın alınabilir.Belirtilen fiyatlar adet fiyatıdır.</t>
+  </si>
+  <si>
+    <t>Polyester materyali sayesinde hafifliğiyle konforlu bir kullanım sunarken dayanıklılığından da taviz vermez.Uzun kollu oluşu soğuk havalarda ekstra koruma sağlarken çizgili deseniyle trendleri takip eder.S-M-L-XL-2XL Beden seçeneği mevcuttur.Ürünümüz serili olarak satılmaktadır.Belirtilen fiyatlar adet fiyatıdır.</t>
+  </si>
+  <si>
+    <t>Slim fit chino keten pantolon, pamuk ve polyester karışımından oluşan orta kalınlığa sahip kumaşı, konforlu bir kullanım vaat eder.Nefes alan kumaşı ile yaz aylarında serin tutar, terletmez.31-38 Beden seçeneği mevcuttur.Ürünümüz serili olarak satılmaktadır.Belirtilen fiyatlar adet fiyatıdır.</t>
   </si>
 </sst>
 </file>
@@ -688,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,7 +738,7 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>91</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
@@ -755,7 +758,7 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>91</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
@@ -775,7 +778,7 @@
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>91</v>
       </c>
       <c r="F4" t="s">
         <v>6</v>
@@ -795,7 +798,7 @@
         <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>91</v>
       </c>
       <c r="F5" t="s">
         <v>6</v>
@@ -815,7 +818,7 @@
         <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>91</v>
       </c>
       <c r="F6" t="s">
         <v>6</v>
@@ -823,7 +826,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
@@ -832,10 +835,10 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>91</v>
       </c>
       <c r="F7" t="s">
         <v>6</v>
@@ -843,39 +846,39 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>25</v>
+        <v>92</v>
       </c>
       <c r="F8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="F9" t="s">
         <v>6</v>
@@ -883,19 +886,19 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="F10" t="s">
         <v>6</v>
@@ -903,19 +906,19 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E11" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="F11" t="s">
         <v>6</v>
@@ -923,19 +926,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
         <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="F12" t="s">
         <v>6</v>
@@ -943,19 +946,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
         <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E13" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="F13" t="s">
         <v>6</v>
@@ -963,19 +966,19 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
         <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E14" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="F14" t="s">
         <v>6</v>
@@ -983,19 +986,19 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
         <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E15" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="F15" t="s">
         <v>6</v>
@@ -1003,19 +1006,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
         <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E16" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="F16" t="s">
         <v>6</v>
@@ -1023,19 +1026,19 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
         <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E17" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="F17" t="s">
         <v>6</v>
@@ -1043,19 +1046,19 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E18" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="F18" t="s">
         <v>6</v>
@@ -1063,19 +1066,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E19" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="F19" t="s">
         <v>6</v>
@@ -1083,19 +1086,19 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E20" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="F20" t="s">
         <v>6</v>
@@ -1103,19 +1106,19 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E21" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="F21" t="s">
         <v>6</v>
@@ -1123,19 +1126,19 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B22" t="s">
         <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E22" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="F22" t="s">
         <v>6</v>
@@ -1143,19 +1146,19 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D23" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E23" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="F23" t="s">
         <v>6</v>
@@ -1163,19 +1166,19 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" t="s">
         <v>60</v>
       </c>
-      <c r="C24" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" t="s">
-        <v>62</v>
-      </c>
       <c r="E24" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="F24" t="s">
         <v>6</v>
@@ -1183,19 +1186,19 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C25" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D25" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E25" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="F25" t="s">
         <v>6</v>
@@ -1203,19 +1206,19 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C26" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="F26" t="s">
         <v>6</v>
@@ -1223,19 +1226,19 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" t="s">
         <v>67</v>
       </c>
-      <c r="C27" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27" t="s">
-        <v>69</v>
-      </c>
       <c r="E27" s="3" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="F27" t="s">
         <v>6</v>
@@ -1243,19 +1246,19 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="F28" t="s">
         <v>6</v>
@@ -1263,19 +1266,19 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B29" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C29" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D29" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="F29" t="s">
         <v>6</v>
@@ -1283,19 +1286,19 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B30" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C30" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="F30" t="s">
         <v>6</v>
@@ -1303,19 +1306,19 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B31" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C31" t="s">
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="F31" t="s">
         <v>6</v>
@@ -1323,19 +1326,19 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B32" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C32" t="s">
         <v>7</v>
       </c>
       <c r="D32" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="F32" t="s">
         <v>6</v>
@@ -1343,19 +1346,19 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B33" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" t="s">
         <v>80</v>
       </c>
-      <c r="C33" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" t="s">
-        <v>86</v>
-      </c>
       <c r="E33" s="3" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="F33" t="s">
         <v>6</v>
@@ -1363,19 +1366,19 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B34" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C34" t="s">
         <v>7</v>
       </c>
       <c r="D34" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="F34" t="s">
         <v>6</v>
@@ -1383,19 +1386,19 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B35" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C35" t="s">
         <v>7</v>
       </c>
       <c r="D35" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="F35" t="s">
         <v>6</v>
@@ -1403,19 +1406,19 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B36" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C36" t="s">
         <v>7</v>
       </c>
       <c r="D36" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="F36" t="s">
         <v>6</v>
@@ -1423,22 +1426,110 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B37" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C37" t="s">
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="F37" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Katalog guncellendi - Cum 14.11.2025 13:22:24,91
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0ACB715-F6C5-4B64-860D-EF4B1DFE7CDB}"/>
+  <xr:revisionPtr revIDLastSave="135" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C98F8ADE-F87A-440A-8668-5C7496AD0358}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="129">
   <si>
     <t>urun_adi</t>
   </si>
@@ -308,6 +308,105 @@
   </si>
   <si>
     <t>Slim fit chino keten pantolon, pamuk ve polyester karışımından oluşan orta kalınlığa sahip kumaşı, konforlu bir kullanım vaat eder.Nefes alan kumaşı ile yaz aylarında serin tutar, terletmez.31-38 Beden seçeneği mevcuttur.Ürünümüz serili olarak satılmaktadır.Belirtilen fiyatlar adet fiyatıdır.</t>
+  </si>
+  <si>
+    <t>STRAİGHTKOYU.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Straight Kot Pantolon  Koyu Mavi </t>
+  </si>
+  <si>
+    <t>450 Tl</t>
+  </si>
+  <si>
+    <t>%100 pamuklu kumaşı sayesinde gün boyu konfor sunar ve cildin nefes almasını sağlar.Normal bel kesimi ile rahat hareket etmenize olanak tanırken, düz paça tasarımı modern bir görünüm kazandırır.30-31-32-33-34-36-38-40 Beden seçeneği mevcuttur.Ürünümüz tekli olarak satın alınabilir.Belirtilen fiyatlar adet fiyatıdır.</t>
+  </si>
+  <si>
+    <t>STRAİGHTAÇIK.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Straight Kot Pantolon  Açık  Mavi </t>
+  </si>
+  <si>
+    <t>Regular Fit Kot Pantolon Seapoint</t>
+  </si>
+  <si>
+    <t>SEAPOİNT.jpg</t>
+  </si>
+  <si>
+    <t>%98 pamuk ve %2 spandex karışımı materyali sayesinde konforlu bir deneyim sunar.Regular fit kesimi ile vücut hatlarınıza uyum sağlayarak şık bir görünüm kazandırır.30-31-32-33-34-36-38-40 Beden seçeneği mevcuttur.Ürünümüz tekli olarak satın alınabilir.Belirtilen fiyatlar adet fiyatıdır.</t>
+  </si>
+  <si>
+    <t>OCEAN.jpg</t>
+  </si>
+  <si>
+    <t>Regular Fit Kot Pantolon Ocean</t>
+  </si>
+  <si>
+    <t>Regular Fit Kot Pantolon Ren</t>
+  </si>
+  <si>
+    <t>REN.jpg</t>
+  </si>
+  <si>
+    <t>Regular Fit Kot Pantolon Heinkel</t>
+  </si>
+  <si>
+    <t>HEİNKEL.jpg</t>
+  </si>
+  <si>
+    <t>HEİN.jpg</t>
+  </si>
+  <si>
+    <t>Regular Fit Kot Pantolon Hawker</t>
+  </si>
+  <si>
+    <t>HAWKER.jpg</t>
+  </si>
+  <si>
+    <t>FORİUS.jpg</t>
+  </si>
+  <si>
+    <t>Regular Fit Kot Pantolon Forius</t>
+  </si>
+  <si>
+    <t>Regular Fit Kot Pantolon Douglas</t>
+  </si>
+  <si>
+    <t>DOUGLAS.jpg</t>
+  </si>
+  <si>
+    <t>Regular Fit Kot Pantolon Angry</t>
+  </si>
+  <si>
+    <t>ANGRY.jpg</t>
+  </si>
+  <si>
+    <t>Regular Fit Kot Kanvas Pantolon Taş</t>
+  </si>
+  <si>
+    <t>KANVATAŞ.jpg</t>
+  </si>
+  <si>
+    <t>Regular Fit Kot Kanvas Pantolon Kahverengi</t>
+  </si>
+  <si>
+    <t>KANVASKAHVE.jpg</t>
+  </si>
+  <si>
+    <t>Regular Fit Kot Kanvas Pantolon Gri</t>
+  </si>
+  <si>
+    <t>KANVASGRİ.jpg</t>
+  </si>
+  <si>
+    <t>Regular Fit Kot Kanvas Pantolon Bej</t>
+  </si>
+  <si>
+    <t>KANVASBEJ.jpg</t>
+  </si>
+  <si>
+    <t>%98 pamuk ve %2 spandex karışımı materyali sayesinde konforlu bir deneyim sunar.5 cepli tasarımı ve Regular fit kesimi ile vücut hatlarınıza uyum sağlayarak şık bir görünüm kazandırır.29-30-31-32-33-34-36-38-40 Beden seçeneği mevcuttur.Ürünümüz serili olarak satılmaktadır.Belirtilen fiyatlar adet fiyatıdır.</t>
   </si>
 </sst>
 </file>
@@ -691,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1446,90 +1545,290 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>97</v>
+      </c>
+      <c r="B38" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" t="s">
+        <v>96</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" t="s">
+        <v>100</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>102</v>
+      </c>
+      <c r="B40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" t="s">
+        <v>103</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41" t="s">
+        <v>98</v>
+      </c>
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" t="s">
+        <v>105</v>
+      </c>
+      <c r="E41" t="s">
+        <v>104</v>
+      </c>
+      <c r="F41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>107</v>
+      </c>
+      <c r="B42" t="s">
+        <v>98</v>
+      </c>
+      <c r="C42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" t="s">
+        <v>108</v>
+      </c>
+      <c r="E42" t="s">
+        <v>104</v>
+      </c>
+      <c r="F42" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>109</v>
+      </c>
+      <c r="B43" t="s">
+        <v>98</v>
+      </c>
+      <c r="C43" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" t="s">
+        <v>110</v>
+      </c>
+      <c r="E43" t="s">
+        <v>104</v>
+      </c>
+      <c r="F43" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>89</v>
       </c>
-      <c r="C38" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>98</v>
+      </c>
       <c r="C44" t="s">
         <v>7</v>
       </c>
+      <c r="D44" t="s">
+        <v>111</v>
+      </c>
+      <c r="E44" t="s">
+        <v>104</v>
+      </c>
+      <c r="F44" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>112</v>
+      </c>
+      <c r="B45" t="s">
+        <v>98</v>
+      </c>
       <c r="C45" t="s">
         <v>7</v>
       </c>
+      <c r="D45" t="s">
+        <v>113</v>
+      </c>
+      <c r="E45" t="s">
+        <v>104</v>
+      </c>
+      <c r="F45" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>115</v>
+      </c>
+      <c r="B46" t="s">
+        <v>98</v>
+      </c>
       <c r="C46" t="s">
         <v>7</v>
       </c>
+      <c r="D46" t="s">
+        <v>114</v>
+      </c>
+      <c r="E46" t="s">
+        <v>104</v>
+      </c>
+      <c r="F46" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>116</v>
+      </c>
+      <c r="B47" t="s">
+        <v>98</v>
+      </c>
       <c r="C47" t="s">
         <v>7</v>
       </c>
+      <c r="D47" t="s">
+        <v>117</v>
+      </c>
+      <c r="E47" t="s">
+        <v>104</v>
+      </c>
+      <c r="F47" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>118</v>
+      </c>
+      <c r="B48" t="s">
+        <v>98</v>
+      </c>
       <c r="C48" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>119</v>
+      </c>
+      <c r="E48" t="s">
+        <v>104</v>
+      </c>
+      <c r="F48" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>120</v>
+      </c>
+      <c r="B49" t="s">
+        <v>98</v>
+      </c>
       <c r="C49" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>121</v>
+      </c>
+      <c r="E49" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>122</v>
+      </c>
+      <c r="B50" t="s">
+        <v>98</v>
+      </c>
       <c r="C50" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>123</v>
+      </c>
+      <c r="E50" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>124</v>
+      </c>
+      <c r="B51" t="s">
+        <v>98</v>
+      </c>
       <c r="C51" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>125</v>
+      </c>
+      <c r="E51" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>126</v>
+      </c>
+      <c r="B52" t="s">
+        <v>98</v>
+      </c>
       <c r="C52" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C53" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C54" t="s">
-        <v>7</v>
+      <c r="D52" t="s">
+        <v>127</v>
+      </c>
+      <c r="E52" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Katalog guncellendi - Cum 14.11.2025 13:25:21,22
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="135" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C98F8ADE-F87A-440A-8668-5C7496AD0358}"/>
+  <xr:revisionPtr revIDLastSave="137" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E9F1CFF-149D-45F1-A1B2-A6B87B98DA7C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5325" yWindow="3720" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -792,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Katalog guncellendi - Cum 14.11.2025 13:59:31,22
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="137" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E9F1CFF-149D-45F1-A1B2-A6B87B98DA7C}"/>
+  <xr:revisionPtr revIDLastSave="141" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC991FBA-9DE3-482C-89BE-F2131F816948}"/>
   <bookViews>
-    <workbookView xWindow="5325" yWindow="3720" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -793,7 +793,7 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1768,7 +1768,7 @@
         <v>120</v>
       </c>
       <c r="B49" t="s">
-        <v>98</v>
+        <v>23</v>
       </c>
       <c r="C49" t="s">
         <v>7</v>
@@ -1785,7 +1785,7 @@
         <v>122</v>
       </c>
       <c r="B50" t="s">
-        <v>98</v>
+        <v>23</v>
       </c>
       <c r="C50" t="s">
         <v>7</v>
@@ -1802,7 +1802,7 @@
         <v>124</v>
       </c>
       <c r="B51" t="s">
-        <v>98</v>
+        <v>23</v>
       </c>
       <c r="C51" t="s">
         <v>7</v>
@@ -1819,7 +1819,7 @@
         <v>126</v>
       </c>
       <c r="B52" t="s">
-        <v>98</v>
+        <v>23</v>
       </c>
       <c r="C52" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Katalog guncellendi - Cum 14.11.2025 14:29:31,47
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="141" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC991FBA-9DE3-482C-89BE-F2131F816948}"/>
+  <xr:revisionPtr revIDLastSave="160" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D980DF3C-101A-42FF-A1CA-44A938847C0B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="144">
   <si>
     <t>urun_adi</t>
   </si>
@@ -407,6 +407,51 @@
   </si>
   <si>
     <t>%98 pamuk ve %2 spandex karışımı materyali sayesinde konforlu bir deneyim sunar.5 cepli tasarımı ve Regular fit kesimi ile vücut hatlarınıza uyum sağlayarak şık bir görünüm kazandırır.29-30-31-32-33-34-36-38-40 Beden seçeneği mevcuttur.Ürünümüz serili olarak satılmaktadır.Belirtilen fiyatlar adet fiyatıdır.</t>
+  </si>
+  <si>
+    <t>Enzim SoftShell Mont Füme</t>
+  </si>
+  <si>
+    <t>600 Tl</t>
+  </si>
+  <si>
+    <t>Mont</t>
+  </si>
+  <si>
+    <t>SOFTFÜME.jpg</t>
+  </si>
+  <si>
+    <t>Su ve rüzgar geçirmez özelliği ile her türlü hava koşulunda konforlu bir kullanım sunar.Polar ve astar detayları ile ekstra sıcaklık ve konfor sağlar.S-M-L-XL-2XL-3XL Beden seçeneği mevcuttur.Ürünümüz serili olarak satılmaktadır.Belirtilen fiyatlar adet fiyatıdır.</t>
+  </si>
+  <si>
+    <t>Enzim SoftShell Mont Haki</t>
+  </si>
+  <si>
+    <t>SOFTHAKİ.jpg</t>
+  </si>
+  <si>
+    <t>Enzim SoftShell Mont Siyah</t>
+  </si>
+  <si>
+    <t>SOFTSİYAH.jpg</t>
+  </si>
+  <si>
+    <t>Slim Fit kot Pantolon Dornier</t>
+  </si>
+  <si>
+    <t>320 Tl</t>
+  </si>
+  <si>
+    <t>DORNİER.jpg</t>
+  </si>
+  <si>
+    <t>Slim Fit kot Pantolon Dove</t>
+  </si>
+  <si>
+    <t>DOVE.jpg</t>
+  </si>
+  <si>
+    <t>%98 pamuk ve %2 spandex içeriği sayesinde nefes alabilirlik ve esneklik sağlar, gün boyu konforlu bir kullanım sunar.Slim silueti vücut hatlarınıza mükemmel uyum sağlayarak şık bir profil çizer.31-32-33-34-36-38 Beden seçeneği mevcuttur.Ürünümüz tekli olarak satın alınabilir.Belirtilen fiyatlar adet fiyatıdır.</t>
   </si>
 </sst>
 </file>
@@ -790,10 +835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1763,7 +1808,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>120</v>
       </c>
@@ -1779,8 +1824,11 @@
       <c r="E49" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>122</v>
       </c>
@@ -1796,8 +1844,11 @@
       <c r="E50" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>124</v>
       </c>
@@ -1813,8 +1864,11 @@
       <c r="E51" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>126</v>
       </c>
@@ -1829,6 +1883,114 @@
       </c>
       <c r="E52" t="s">
         <v>128</v>
+      </c>
+      <c r="F52" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>129</v>
+      </c>
+      <c r="B53" t="s">
+        <v>130</v>
+      </c>
+      <c r="C53" t="s">
+        <v>131</v>
+      </c>
+      <c r="D53" t="s">
+        <v>132</v>
+      </c>
+      <c r="E53" t="s">
+        <v>133</v>
+      </c>
+      <c r="F53" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>134</v>
+      </c>
+      <c r="B54" t="s">
+        <v>130</v>
+      </c>
+      <c r="C54" t="s">
+        <v>131</v>
+      </c>
+      <c r="D54" t="s">
+        <v>135</v>
+      </c>
+      <c r="E54" t="s">
+        <v>133</v>
+      </c>
+      <c r="F54" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>136</v>
+      </c>
+      <c r="B55" t="s">
+        <v>130</v>
+      </c>
+      <c r="C55" t="s">
+        <v>131</v>
+      </c>
+      <c r="D55" t="s">
+        <v>137</v>
+      </c>
+      <c r="E55" t="s">
+        <v>133</v>
+      </c>
+      <c r="F55" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>138</v>
+      </c>
+      <c r="B56" t="s">
+        <v>139</v>
+      </c>
+      <c r="C56" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" t="s">
+        <v>140</v>
+      </c>
+      <c r="E56" t="s">
+        <v>143</v>
+      </c>
+      <c r="F56" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>141</v>
+      </c>
+      <c r="B57" t="s">
+        <v>139</v>
+      </c>
+      <c r="C57" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57" t="s">
+        <v>142</v>
+      </c>
+      <c r="E57" t="s">
+        <v>143</v>
+      </c>
+      <c r="F57" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F58" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Katalog guncellendi - Cum 14.11.2025 14:36:44,39
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="160" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D980DF3C-101A-42FF-A1CA-44A938847C0B}"/>
+  <xr:revisionPtr revIDLastSave="162" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94B96AE9-D02E-4D23-89FE-F8951FA3EB1C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="144">
   <si>
     <t>urun_adi</t>
   </si>
@@ -418,9 +418,6 @@
     <t>Mont</t>
   </si>
   <si>
-    <t>SOFTFÜME.jpg</t>
-  </si>
-  <si>
     <t>Su ve rüzgar geçirmez özelliği ile her türlü hava koşulunda konforlu bir kullanım sunar.Polar ve astar detayları ile ekstra sıcaklık ve konfor sağlar.S-M-L-XL-2XL-3XL Beden seçeneği mevcuttur.Ürünümüz serili olarak satılmaktadır.Belirtilen fiyatlar adet fiyatıdır.</t>
   </si>
   <si>
@@ -452,6 +449,9 @@
   </si>
   <si>
     <t>%98 pamuk ve %2 spandex içeriği sayesinde nefes alabilirlik ve esneklik sağlar, gün boyu konforlu bir kullanım sunar.Slim silueti vücut hatlarınıza mükemmel uyum sağlayarak şık bir profil çizer.31-32-33-34-36-38 Beden seçeneği mevcuttur.Ürünümüz tekli olarak satın alınabilir.Belirtilen fiyatlar adet fiyatıdır.</t>
+  </si>
+  <si>
+    <t>SOFTFUME.jpg</t>
   </si>
 </sst>
 </file>
@@ -835,10 +835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1899,10 +1899,10 @@
         <v>131</v>
       </c>
       <c r="D53" t="s">
+        <v>143</v>
+      </c>
+      <c r="E53" t="s">
         <v>132</v>
-      </c>
-      <c r="E53" t="s">
-        <v>133</v>
       </c>
       <c r="F53" t="s">
         <v>6</v>
@@ -1910,7 +1910,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B54" t="s">
         <v>130</v>
@@ -1919,10 +1919,10 @@
         <v>131</v>
       </c>
       <c r="D54" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E54" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F54" t="s">
         <v>6</v>
@@ -1930,7 +1930,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B55" t="s">
         <v>130</v>
@@ -1939,10 +1939,10 @@
         <v>131</v>
       </c>
       <c r="D55" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E55" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F55" t="s">
         <v>6</v>
@@ -1950,19 +1950,19 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>137</v>
+      </c>
+      <c r="B56" t="s">
         <v>138</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" t="s">
         <v>139</v>
       </c>
-      <c r="C56" t="s">
-        <v>7</v>
-      </c>
-      <c r="D56" t="s">
-        <v>140</v>
-      </c>
       <c r="E56" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F56" t="s">
         <v>6</v>
@@ -1970,26 +1970,21 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>140</v>
+      </c>
+      <c r="B57" t="s">
+        <v>138</v>
+      </c>
+      <c r="C57" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57" t="s">
         <v>141</v>
       </c>
-      <c r="B57" t="s">
-        <v>139</v>
-      </c>
-      <c r="C57" t="s">
-        <v>7</v>
-      </c>
-      <c r="D57" t="s">
+      <c r="E57" t="s">
         <v>142</v>
       </c>
-      <c r="E57" t="s">
-        <v>143</v>
-      </c>
       <c r="F57" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F58" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Katalog guncellendi - Cum 14.11.2025 15:35:14,92
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="162" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94B96AE9-D02E-4D23-89FE-F8951FA3EB1C}"/>
+  <xr:revisionPtr revIDLastSave="180" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{293C7648-9967-4F83-8CEF-E0594F34838C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="152">
   <si>
     <t>urun_adi</t>
   </si>
@@ -79,9 +79,6 @@
     <t>Baggy Kar Yıkama</t>
   </si>
   <si>
-    <t>300 Tl</t>
-  </si>
-  <si>
     <t>BAG4.jpg</t>
   </si>
   <si>
@@ -91,9 +88,6 @@
     <t>BAG5.jpg</t>
   </si>
   <si>
-    <t>350 Tl</t>
-  </si>
-  <si>
     <t>Bel Paça Lastik  Pantolon Antrasit</t>
   </si>
   <si>
@@ -196,9 +190,6 @@
     <t>Kot Gömlek Ceket Denim Blue</t>
   </si>
   <si>
-    <t>400 Tl</t>
-  </si>
-  <si>
     <t>Kot Gömlek Ceket Mavi</t>
   </si>
   <si>
@@ -217,9 +208,6 @@
     <t>Eşref Gömlek Açık Mavi</t>
   </si>
   <si>
-    <t>260 Tl</t>
-  </si>
-  <si>
     <t>Eşref Gömlek Bej</t>
   </si>
   <si>
@@ -247,9 +235,6 @@
     <t>KETENANTRASİT.jpg</t>
   </si>
   <si>
-    <t>360 Tl</t>
-  </si>
-  <si>
     <t>Chino Keten Pantolon Antrasit</t>
   </si>
   <si>
@@ -295,33 +280,15 @@
     <t>%100 pamuk materyali ile üretilmiş, Çıt çıt kapama şekliyle güvenli bir kullanım sağlar.İki tarz tek parçada;Hem gömlek hem ceket.XS-S /  M-L /  XL-2XL Beden seçeneği Mevcuttur.Ürünümüz tekli olarak satın alınabilir.Belirtilen fiyatlar adet fiyatıdır.</t>
   </si>
   <si>
-    <t>Erkek baggy pantolon, bol ve rahat kesimiyle öne çıkan, modern sokak stilinin vazgeçilmez parçasıdır. Kalçadan paçaya kadar geniş formu sayesinde hareket özgürlüğü sunar.Ürün içeriği 100% Pamuk.29-38  beden seçeneği mevcuttur.Ürünümüz tekli olarak satın alınabilir.Belirtilen fiyatlar adet fiyatıdır.</t>
-  </si>
-  <si>
-    <t>%98 pamuk içeriği ile nefes alabilen yapıda, cildinize nazik dokunuşlar sunar.Bağcıklı kapama şekliyle kişisel zevke göre ayarlama imkanı taşır.Lastikli bel detayı sayesinde  rahatlığından ödün vermez.34-46 Beden aralığı mevcuttur.Ürünümüz tekli olarak satın alınabilir.Belirtilen fiyatlar adet fiyatıdır.</t>
-  </si>
-  <si>
     <t>%85 pamuk, %12 polyester ve %3 spandex karışımından oluşan materyali ile konforlu bir deneyim sağlar.S-M-L-XL-2XL Beden seçeneği mevcuttur.Ürünümüz tekli olarak satın alınabilir.Belirtilen fiyatlar adet fiyatıdır.</t>
   </si>
   <si>
-    <t>Polyester materyali sayesinde hafifliğiyle konforlu bir kullanım sunarken dayanıklılığından da taviz vermez.Uzun kollu oluşu soğuk havalarda ekstra koruma sağlarken çizgili deseniyle trendleri takip eder.S-M-L-XL-2XL Beden seçeneği mevcuttur.Ürünümüz serili olarak satılmaktadır.Belirtilen fiyatlar adet fiyatıdır.</t>
-  </si>
-  <si>
-    <t>Slim fit chino keten pantolon, pamuk ve polyester karışımından oluşan orta kalınlığa sahip kumaşı, konforlu bir kullanım vaat eder.Nefes alan kumaşı ile yaz aylarında serin tutar, terletmez.31-38 Beden seçeneği mevcuttur.Ürünümüz serili olarak satılmaktadır.Belirtilen fiyatlar adet fiyatıdır.</t>
-  </si>
-  <si>
     <t>STRAİGHTKOYU.jpg</t>
   </si>
   <si>
     <t xml:space="preserve"> Straight Kot Pantolon  Koyu Mavi </t>
   </si>
   <si>
-    <t>450 Tl</t>
-  </si>
-  <si>
-    <t>%100 pamuklu kumaşı sayesinde gün boyu konfor sunar ve cildin nefes almasını sağlar.Normal bel kesimi ile rahat hareket etmenize olanak tanırken, düz paça tasarımı modern bir görünüm kazandırır.30-31-32-33-34-36-38-40 Beden seçeneği mevcuttur.Ürünümüz tekli olarak satın alınabilir.Belirtilen fiyatlar adet fiyatıdır.</t>
-  </si>
-  <si>
     <t>STRAİGHTAÇIK.jpg</t>
   </si>
   <si>
@@ -334,9 +301,6 @@
     <t>SEAPOİNT.jpg</t>
   </si>
   <si>
-    <t>%98 pamuk ve %2 spandex karışımı materyali sayesinde konforlu bir deneyim sunar.Regular fit kesimi ile vücut hatlarınıza uyum sağlayarak şık bir görünüm kazandırır.30-31-32-33-34-36-38-40 Beden seçeneği mevcuttur.Ürünümüz tekli olarak satın alınabilir.Belirtilen fiyatlar adet fiyatıdır.</t>
-  </si>
-  <si>
     <t>OCEAN.jpg</t>
   </si>
   <si>
@@ -373,9 +337,6 @@
     <t>Regular Fit Kot Pantolon Douglas</t>
   </si>
   <si>
-    <t>DOUGLAS.jpg</t>
-  </si>
-  <si>
     <t>Regular Fit Kot Pantolon Angry</t>
   </si>
   <si>
@@ -406,18 +367,15 @@
     <t>KANVASBEJ.jpg</t>
   </si>
   <si>
-    <t>%98 pamuk ve %2 spandex karışımı materyali sayesinde konforlu bir deneyim sunar.5 cepli tasarımı ve Regular fit kesimi ile vücut hatlarınıza uyum sağlayarak şık bir görünüm kazandırır.29-30-31-32-33-34-36-38-40 Beden seçeneği mevcuttur.Ürünümüz serili olarak satılmaktadır.Belirtilen fiyatlar adet fiyatıdır.</t>
-  </si>
-  <si>
     <t>Enzim SoftShell Mont Füme</t>
   </si>
   <si>
-    <t>600 Tl</t>
-  </si>
-  <si>
     <t>Mont</t>
   </si>
   <si>
+    <t>SOFTFÜME.jpg</t>
+  </si>
+  <si>
     <t>Su ve rüzgar geçirmez özelliği ile her türlü hava koşulunda konforlu bir kullanım sunar.Polar ve astar detayları ile ekstra sıcaklık ve konfor sağlar.S-M-L-XL-2XL-3XL Beden seçeneği mevcuttur.Ürünümüz serili olarak satılmaktadır.Belirtilen fiyatlar adet fiyatıdır.</t>
   </si>
   <si>
@@ -436,9 +394,6 @@
     <t>Slim Fit kot Pantolon Dornier</t>
   </si>
   <si>
-    <t>320 Tl</t>
-  </si>
-  <si>
     <t>DORNİER.jpg</t>
   </si>
   <si>
@@ -448,10 +403,79 @@
     <t>DOVE.jpg</t>
   </si>
   <si>
-    <t>%98 pamuk ve %2 spandex içeriği sayesinde nefes alabilirlik ve esneklik sağlar, gün boyu konforlu bir kullanım sunar.Slim silueti vücut hatlarınıza mükemmel uyum sağlayarak şık bir profil çizer.31-32-33-34-36-38 Beden seçeneği mevcuttur.Ürünümüz tekli olarak satın alınabilir.Belirtilen fiyatlar adet fiyatıdır.</t>
-  </si>
-  <si>
-    <t>SOFTFUME.jpg</t>
+    <t>Ürün içeriği 100% Pamuk.29-30-31-32-33-34-36-38  beden seçeneği mevcuttur.Ürünümüz tekli olarak satın alınabilir.Belirtilen fiyatlar adet fiyatıdır.</t>
+  </si>
+  <si>
+    <t>%98 pamuk içeriğine sahiptir..Bağcıklı kapama şekli ve lastikli bel detayı sayesinde  rahatlığından ödün vermez.34-36-38-40-42-44-46 Beden aralığı mevcuttur.Ürünümüz tekli olarak satın alınabilir.Belirtilen fiyatlar adet fiyatıdır.</t>
+  </si>
+  <si>
+    <t>Polyester materyali sayesinde hafifliğiyle konforlu bir kullanım sunarken dayanıklılığından da taviz vermez.S-M-L-XL-2XL Beden seçeneği mevcuttur.Ürünümüz serili olarak satılmaktadır.Belirtilen fiyatlar adet fiyatıdır.</t>
+  </si>
+  <si>
+    <t>Slim fit chino keten pantolon, pamuk ve polyester karışımından oluşan orta kalınlığa sahip kumaşı, konforlu bir kullanım vaat eder.31-38 Beden seçeneği mevcuttur.Ürünümüz serili olarak satılmaktadır.Belirtilen fiyatlar adet fiyatıdır.</t>
+  </si>
+  <si>
+    <t>%100 pamuklu kumaşı sayesinde gün boyu konfor sunar ve cildin nefes almasını sağlar.30-31-32-33-34-36-38-40 Beden seçeneği mevcuttur.Ürünümüz tekli olarak satın alınabilir.Belirtilen fiyatlar adet fiyatıdır.</t>
+  </si>
+  <si>
+    <t>%98 pamuk ve %2 spandex karışımı materyali sayesinde konforlu bir deneyim sunar.30-31-32-33-34-36-38-40 Beden seçeneği mevcuttur.Ürünümüz tekli olarak satın alınabilir.Belirtilen fiyatlar adet fiyatıdır.</t>
+  </si>
+  <si>
+    <t>%98 pamuk ve %2 spandex içeriği sayesinde nefes alabilirlik ve esneklik sağlar, gün boyu konforlu bir kullanım sunar.31-32-33-34-36-38 Beden seçeneği mevcuttur.Ürünümüz tekli olarak satın alınabilir.Belirtilen fiyatlar adet fiyatıdır.</t>
+  </si>
+  <si>
+    <t>350 TL</t>
+  </si>
+  <si>
+    <t>400 TL</t>
+  </si>
+  <si>
+    <t>260 TL</t>
+  </si>
+  <si>
+    <t>360 TL</t>
+  </si>
+  <si>
+    <t>450 TL</t>
+  </si>
+  <si>
+    <t>451 TL</t>
+  </si>
+  <si>
+    <t>452 TL</t>
+  </si>
+  <si>
+    <t>453 TL</t>
+  </si>
+  <si>
+    <t>454 TL</t>
+  </si>
+  <si>
+    <t>455 TL</t>
+  </si>
+  <si>
+    <t>456 TL</t>
+  </si>
+  <si>
+    <t>457 TL</t>
+  </si>
+  <si>
+    <t>458 TL</t>
+  </si>
+  <si>
+    <t>459 TL</t>
+  </si>
+  <si>
+    <t>460 TL</t>
+  </si>
+  <si>
+    <t>461 TL</t>
+  </si>
+  <si>
+    <t>462 TL</t>
+  </si>
+  <si>
+    <t>DOUGLAS.png</t>
   </si>
 </sst>
 </file>
@@ -837,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,7 +906,7 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
+        <v>127</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
@@ -902,7 +926,7 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>91</v>
+        <v>127</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
@@ -922,7 +946,7 @@
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>91</v>
+        <v>127</v>
       </c>
       <c r="F4" t="s">
         <v>6</v>
@@ -933,7 +957,7 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -942,7 +966,7 @@
         <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>91</v>
+        <v>127</v>
       </c>
       <c r="F5" t="s">
         <v>6</v>
@@ -953,16 +977,16 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
       <c r="E6" t="s">
-        <v>91</v>
+        <v>127</v>
       </c>
       <c r="F6" t="s">
         <v>6</v>
@@ -970,19 +994,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
       <c r="E7" t="s">
-        <v>91</v>
+        <v>127</v>
       </c>
       <c r="F7" t="s">
         <v>6</v>
@@ -990,39 +1014,39 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>134</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>92</v>
+        <v>128</v>
       </c>
       <c r="F8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>134</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>92</v>
+        <v>128</v>
       </c>
       <c r="F9" t="s">
         <v>6</v>
@@ -1030,19 +1054,19 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>134</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>92</v>
+        <v>128</v>
       </c>
       <c r="F10" t="s">
         <v>6</v>
@@ -1050,19 +1074,19 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F11" t="s">
         <v>6</v>
@@ -1070,19 +1094,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F12" t="s">
         <v>6</v>
@@ -1090,19 +1114,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E13" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F13" t="s">
         <v>6</v>
@@ -1110,19 +1134,19 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E14" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F14" t="s">
         <v>6</v>
@@ -1130,19 +1154,19 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E15" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F15" t="s">
         <v>6</v>
@@ -1150,19 +1174,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F16" t="s">
         <v>6</v>
@@ -1170,19 +1194,19 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F17" t="s">
         <v>6</v>
@@ -1190,19 +1214,19 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E18" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F18" t="s">
         <v>6</v>
@@ -1210,19 +1234,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E19" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F19" t="s">
         <v>6</v>
@@ -1230,19 +1254,19 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F20" t="s">
         <v>6</v>
@@ -1250,19 +1274,19 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E21" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F21" t="s">
         <v>6</v>
@@ -1270,19 +1294,19 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E22" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F22" t="s">
         <v>6</v>
@@ -1290,19 +1314,19 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>135</v>
       </c>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D23" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E23" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F23" t="s">
         <v>6</v>
@@ -1310,19 +1334,19 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>135</v>
       </c>
       <c r="C24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D24" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E24" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F24" t="s">
         <v>6</v>
@@ -1330,19 +1354,19 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B25" t="s">
-        <v>58</v>
+        <v>135</v>
       </c>
       <c r="C25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D25" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E25" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F25" t="s">
         <v>6</v>
@@ -1350,19 +1374,19 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
+        <v>136</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>94</v>
+        <v>129</v>
       </c>
       <c r="F26" t="s">
         <v>6</v>
@@ -1370,19 +1394,19 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B27" t="s">
-        <v>65</v>
+        <v>136</v>
       </c>
       <c r="C27" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D27" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>94</v>
+        <v>129</v>
       </c>
       <c r="F27" t="s">
         <v>6</v>
@@ -1390,19 +1414,19 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B28" t="s">
+        <v>136</v>
+      </c>
+      <c r="C28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" t="s">
         <v>65</v>
       </c>
-      <c r="C28" t="s">
-        <v>30</v>
-      </c>
-      <c r="D28" t="s">
-        <v>69</v>
-      </c>
       <c r="E28" s="3" t="s">
-        <v>94</v>
+        <v>129</v>
       </c>
       <c r="F28" t="s">
         <v>6</v>
@@ -1410,19 +1434,19 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B29" t="s">
-        <v>65</v>
+        <v>136</v>
       </c>
       <c r="C29" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D29" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>94</v>
+        <v>129</v>
       </c>
       <c r="F29" t="s">
         <v>6</v>
@@ -1430,19 +1454,19 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>136</v>
       </c>
       <c r="C30" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D30" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>94</v>
+        <v>129</v>
       </c>
       <c r="F30" t="s">
         <v>6</v>
@@ -1450,19 +1474,19 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B31" t="s">
-        <v>75</v>
+        <v>137</v>
       </c>
       <c r="C31" t="s">
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>94</v>
+        <v>129</v>
       </c>
       <c r="F31" t="s">
         <v>6</v>
@@ -1470,19 +1494,19 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B32" t="s">
-        <v>75</v>
+        <v>137</v>
       </c>
       <c r="C32" t="s">
         <v>7</v>
       </c>
       <c r="D32" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="F32" t="s">
         <v>6</v>
@@ -1490,19 +1514,19 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B33" t="s">
+        <v>137</v>
+      </c>
+      <c r="C33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" t="s">
         <v>75</v>
       </c>
-      <c r="C33" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" t="s">
-        <v>80</v>
-      </c>
       <c r="E33" s="3" t="s">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="F33" t="s">
         <v>6</v>
@@ -1510,19 +1534,19 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B34" t="s">
-        <v>75</v>
+        <v>137</v>
       </c>
       <c r="C34" t="s">
         <v>7</v>
       </c>
       <c r="D34" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="F34" t="s">
         <v>6</v>
@@ -1530,19 +1554,19 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B35" t="s">
-        <v>75</v>
+        <v>137</v>
       </c>
       <c r="C35" t="s">
         <v>7</v>
       </c>
       <c r="D35" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="F35" t="s">
         <v>6</v>
@@ -1550,19 +1574,19 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B36" t="s">
-        <v>75</v>
+        <v>137</v>
       </c>
       <c r="C36" t="s">
         <v>7</v>
       </c>
       <c r="D36" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="F36" t="s">
         <v>6</v>
@@ -1570,19 +1594,19 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B37" t="s">
-        <v>75</v>
+        <v>137</v>
       </c>
       <c r="C37" t="s">
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="F37" t="s">
         <v>6</v>
@@ -1590,19 +1614,19 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B38" t="s">
-        <v>23</v>
+        <v>134</v>
       </c>
       <c r="C38" t="s">
         <v>7</v>
       </c>
       <c r="D38" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>99</v>
+        <v>131</v>
       </c>
       <c r="F38" t="s">
         <v>6</v>
@@ -1610,19 +1634,19 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B39" t="s">
-        <v>23</v>
+        <v>134</v>
       </c>
       <c r="C39" t="s">
         <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>99</v>
+        <v>131</v>
       </c>
       <c r="F39" t="s">
         <v>6</v>
@@ -1630,19 +1654,19 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B40" t="s">
-        <v>98</v>
+        <v>138</v>
       </c>
       <c r="C40" t="s">
         <v>7</v>
       </c>
       <c r="D40" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="F40" t="s">
         <v>6</v>
@@ -1650,19 +1674,19 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B41" t="s">
-        <v>98</v>
+        <v>138</v>
       </c>
       <c r="C41" t="s">
         <v>7</v>
       </c>
       <c r="D41" t="s">
-        <v>105</v>
-      </c>
-      <c r="E41" t="s">
-        <v>104</v>
+        <v>93</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="F41" t="s">
         <v>6</v>
@@ -1670,19 +1694,19 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="B42" t="s">
-        <v>98</v>
+        <v>138</v>
       </c>
       <c r="C42" t="s">
         <v>7</v>
       </c>
       <c r="D42" t="s">
-        <v>108</v>
-      </c>
-      <c r="E42" t="s">
-        <v>104</v>
+        <v>96</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="F42" t="s">
         <v>6</v>
@@ -1690,19 +1714,19 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="B43" t="s">
+        <v>138</v>
+      </c>
+      <c r="C43" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" t="s">
         <v>98</v>
       </c>
-      <c r="C43" t="s">
-        <v>7</v>
-      </c>
-      <c r="D43" t="s">
-        <v>110</v>
-      </c>
-      <c r="E43" t="s">
-        <v>104</v>
+      <c r="E43" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="F43" t="s">
         <v>6</v>
@@ -1710,19 +1734,19 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B44" t="s">
-        <v>98</v>
+        <v>138</v>
       </c>
       <c r="C44" t="s">
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>111</v>
-      </c>
-      <c r="E44" t="s">
-        <v>104</v>
+        <v>99</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="F44" t="s">
         <v>6</v>
@@ -1730,19 +1754,19 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B45" t="s">
-        <v>98</v>
+        <v>138</v>
       </c>
       <c r="C45" t="s">
         <v>7</v>
       </c>
       <c r="D45" t="s">
-        <v>113</v>
-      </c>
-      <c r="E45" t="s">
-        <v>104</v>
+        <v>101</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="F45" t="s">
         <v>6</v>
@@ -1750,19 +1774,19 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="B46" t="s">
-        <v>98</v>
+        <v>139</v>
       </c>
       <c r="C46" t="s">
         <v>7</v>
       </c>
       <c r="D46" t="s">
-        <v>114</v>
-      </c>
-      <c r="E46" t="s">
-        <v>104</v>
+        <v>102</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="F46" t="s">
         <v>6</v>
@@ -1770,19 +1794,19 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="B47" t="s">
-        <v>98</v>
+        <v>140</v>
       </c>
       <c r="C47" t="s">
         <v>7</v>
       </c>
       <c r="D47" t="s">
-        <v>117</v>
-      </c>
-      <c r="E47" t="s">
-        <v>104</v>
+        <v>151</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="F47" t="s">
         <v>6</v>
@@ -1790,19 +1814,19 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="B48" t="s">
-        <v>98</v>
+        <v>141</v>
       </c>
       <c r="C48" t="s">
         <v>7</v>
       </c>
       <c r="D48" t="s">
-        <v>119</v>
-      </c>
-      <c r="E48" t="s">
-        <v>104</v>
+        <v>106</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="F48" t="s">
         <v>6</v>
@@ -1810,19 +1834,19 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="B49" t="s">
-        <v>23</v>
+        <v>142</v>
       </c>
       <c r="C49" t="s">
         <v>7</v>
       </c>
       <c r="D49" t="s">
-        <v>121</v>
-      </c>
-      <c r="E49" t="s">
-        <v>128</v>
+        <v>108</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="F49" t="s">
         <v>6</v>
@@ -1830,19 +1854,19 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="B50" t="s">
-        <v>23</v>
+        <v>143</v>
       </c>
       <c r="C50" t="s">
         <v>7</v>
       </c>
       <c r="D50" t="s">
-        <v>123</v>
-      </c>
-      <c r="E50" t="s">
-        <v>128</v>
+        <v>110</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="F50" t="s">
         <v>6</v>
@@ -1850,19 +1874,19 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="B51" t="s">
-        <v>23</v>
+        <v>144</v>
       </c>
       <c r="C51" t="s">
         <v>7</v>
       </c>
       <c r="D51" t="s">
-        <v>125</v>
-      </c>
-      <c r="E51" t="s">
-        <v>128</v>
+        <v>112</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="F51" t="s">
         <v>6</v>
@@ -1870,19 +1894,19 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="B52" t="s">
-        <v>23</v>
+        <v>145</v>
       </c>
       <c r="C52" t="s">
         <v>7</v>
       </c>
       <c r="D52" t="s">
-        <v>127</v>
-      </c>
-      <c r="E52" t="s">
-        <v>128</v>
+        <v>114</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="F52" t="s">
         <v>6</v>
@@ -1890,19 +1914,19 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="B53" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
       <c r="C53" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="D53" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="E53" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="F53" t="s">
         <v>6</v>
@@ -1910,19 +1934,19 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="B54" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="C54" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="D54" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="E54" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="F54" t="s">
         <v>6</v>
@@ -1930,19 +1954,19 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="B55" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
       <c r="C55" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="D55" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="E55" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="F55" t="s">
         <v>6</v>
@@ -1950,19 +1974,19 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B56" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="C56" t="s">
         <v>7</v>
       </c>
       <c r="D56" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="E56" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="F56" t="s">
         <v>6</v>
@@ -1970,19 +1994,19 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="B57" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="C57" t="s">
         <v>7</v>
       </c>
       <c r="D57" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="E57" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="F57" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Katalog guncellendi - Cmt 15.11.2025  8:55:29,83
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="180" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{293C7648-9967-4F83-8CEF-E0594F34838C}"/>
+  <xr:revisionPtr revIDLastSave="206" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A52253AB-9A7D-43A2-A29D-B3141F74C512}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="141">
   <si>
     <t>urun_adi</t>
   </si>
@@ -277,12 +277,6 @@
     <t>Regular Fit Kot Pantolon Hein</t>
   </si>
   <si>
-    <t>%100 pamuk materyali ile üretilmiş, Çıt çıt kapama şekliyle güvenli bir kullanım sağlar.İki tarz tek parçada;Hem gömlek hem ceket.XS-S /  M-L /  XL-2XL Beden seçeneği Mevcuttur.Ürünümüz tekli olarak satın alınabilir.Belirtilen fiyatlar adet fiyatıdır.</t>
-  </si>
-  <si>
-    <t>%85 pamuk, %12 polyester ve %3 spandex karışımından oluşan materyali ile konforlu bir deneyim sağlar.S-M-L-XL-2XL Beden seçeneği mevcuttur.Ürünümüz tekli olarak satın alınabilir.Belirtilen fiyatlar adet fiyatıdır.</t>
-  </si>
-  <si>
     <t>STRAİGHTKOYU.jpg</t>
   </si>
   <si>
@@ -409,21 +403,9 @@
     <t>%98 pamuk içeriğine sahiptir..Bağcıklı kapama şekli ve lastikli bel detayı sayesinde  rahatlığından ödün vermez.34-36-38-40-42-44-46 Beden aralığı mevcuttur.Ürünümüz tekli olarak satın alınabilir.Belirtilen fiyatlar adet fiyatıdır.</t>
   </si>
   <si>
-    <t>Polyester materyali sayesinde hafifliğiyle konforlu bir kullanım sunarken dayanıklılığından da taviz vermez.S-M-L-XL-2XL Beden seçeneği mevcuttur.Ürünümüz serili olarak satılmaktadır.Belirtilen fiyatlar adet fiyatıdır.</t>
-  </si>
-  <si>
-    <t>Slim fit chino keten pantolon, pamuk ve polyester karışımından oluşan orta kalınlığa sahip kumaşı, konforlu bir kullanım vaat eder.31-38 Beden seçeneği mevcuttur.Ürünümüz serili olarak satılmaktadır.Belirtilen fiyatlar adet fiyatıdır.</t>
-  </si>
-  <si>
     <t>%100 pamuklu kumaşı sayesinde gün boyu konfor sunar ve cildin nefes almasını sağlar.30-31-32-33-34-36-38-40 Beden seçeneği mevcuttur.Ürünümüz tekli olarak satın alınabilir.Belirtilen fiyatlar adet fiyatıdır.</t>
   </si>
   <si>
-    <t>%98 pamuk ve %2 spandex karışımı materyali sayesinde konforlu bir deneyim sunar.30-31-32-33-34-36-38-40 Beden seçeneği mevcuttur.Ürünümüz tekli olarak satın alınabilir.Belirtilen fiyatlar adet fiyatıdır.</t>
-  </si>
-  <si>
-    <t>%98 pamuk ve %2 spandex içeriği sayesinde nefes alabilirlik ve esneklik sağlar, gün boyu konforlu bir kullanım sunar.31-32-33-34-36-38 Beden seçeneği mevcuttur.Ürünümüz tekli olarak satın alınabilir.Belirtilen fiyatlar adet fiyatıdır.</t>
-  </si>
-  <si>
     <t>350 TL</t>
   </si>
   <si>
@@ -439,43 +421,28 @@
     <t>450 TL</t>
   </si>
   <si>
-    <t>451 TL</t>
-  </si>
-  <si>
-    <t>452 TL</t>
-  </si>
-  <si>
-    <t>453 TL</t>
-  </si>
-  <si>
-    <t>454 TL</t>
-  </si>
-  <si>
-    <t>455 TL</t>
-  </si>
-  <si>
-    <t>456 TL</t>
-  </si>
-  <si>
-    <t>457 TL</t>
-  </si>
-  <si>
-    <t>458 TL</t>
-  </si>
-  <si>
-    <t>459 TL</t>
-  </si>
-  <si>
-    <t>460 TL</t>
-  </si>
-  <si>
-    <t>461 TL</t>
-  </si>
-  <si>
-    <t>462 TL</t>
-  </si>
-  <si>
     <t>DOUGLAS.png</t>
+  </si>
+  <si>
+    <t>600 TL</t>
+  </si>
+  <si>
+    <t>%85 pamuk, %12 polyester ve %3 spandex.S-M-L-XL-2XL Beden seçeneği mevcuttur.Ürünümüz tekli olarak satın alınabilir.Belirtilen fiyatlar adet fiyatıdır.</t>
+  </si>
+  <si>
+    <t>%100 pamuk materyali ile üretilmiş.Hem gömlek hem ceket.XS-S /  M-L /  XL-2XL Beden seçeneği Mevcuttur.Ürünümüz tekli olarak satın alınabilir.Belirtilen fiyatlar adet fiyatıdır.</t>
+  </si>
+  <si>
+    <t>.S-M-L-XL-2XL Beden seçeneği mevcuttur.Ürünümüz serili olarak satılmaktadır.Belirtilen fiyatlar adet fiyatıdır.</t>
+  </si>
+  <si>
+    <t>Slim fit chino keten pantolon,  31-38 Beden seçeneği mevcuttur.Regular fit kalıbıda mevcuttur..Ürünümüz serili olarak satılmaktadır.Belirtilen fiyatlar adet fiyatıdır.</t>
+  </si>
+  <si>
+    <t>%98 pamuk ve %2 spandex. 30-31-32-33-34-36-38-40 Beden seçeneği mevcuttur.Ürünümüz tekli olarak satın alınabilir.Belirtilen fiyatlar adet fiyatıdır.</t>
+  </si>
+  <si>
+    <t>%98 pamuk ve %2 spandex.31-32-33-34-36-38 Beden seçeneği mevcuttur.Ürünümüz tekli olarak satın alınabilir.Belirtilen fiyatlar adet fiyatıdır.</t>
   </si>
 </sst>
 </file>
@@ -862,7 +829,7 @@
   <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+      <selection activeCell="E56" sqref="E56:E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,7 +873,7 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
@@ -926,7 +893,7 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
@@ -946,7 +913,7 @@
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F4" t="s">
         <v>6</v>
@@ -966,7 +933,7 @@
         <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F5" t="s">
         <v>6</v>
@@ -986,7 +953,7 @@
         <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F6" t="s">
         <v>6</v>
@@ -1006,7 +973,7 @@
         <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F7" t="s">
         <v>6</v>
@@ -1017,7 +984,7 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -1026,7 +993,7 @@
         <v>26</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F8" t="s">
         <v>33</v>
@@ -1037,7 +1004,7 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -1046,7 +1013,7 @@
         <v>24</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F9" t="s">
         <v>6</v>
@@ -1057,7 +1024,7 @@
         <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -1066,7 +1033,7 @@
         <v>25</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F10" t="s">
         <v>6</v>
@@ -1086,7 +1053,7 @@
         <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>86</v>
+        <v>135</v>
       </c>
       <c r="F11" t="s">
         <v>6</v>
@@ -1106,7 +1073,7 @@
         <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>86</v>
+        <v>135</v>
       </c>
       <c r="F12" t="s">
         <v>6</v>
@@ -1126,7 +1093,7 @@
         <v>35</v>
       </c>
       <c r="E13" t="s">
-        <v>86</v>
+        <v>135</v>
       </c>
       <c r="F13" t="s">
         <v>6</v>
@@ -1146,7 +1113,7 @@
         <v>37</v>
       </c>
       <c r="E14" t="s">
-        <v>86</v>
+        <v>135</v>
       </c>
       <c r="F14" t="s">
         <v>6</v>
@@ -1166,7 +1133,7 @@
         <v>39</v>
       </c>
       <c r="E15" t="s">
-        <v>86</v>
+        <v>135</v>
       </c>
       <c r="F15" t="s">
         <v>6</v>
@@ -1186,7 +1153,7 @@
         <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>86</v>
+        <v>135</v>
       </c>
       <c r="F16" t="s">
         <v>6</v>
@@ -1206,7 +1173,7 @@
         <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>86</v>
+        <v>135</v>
       </c>
       <c r="F17" t="s">
         <v>6</v>
@@ -1226,7 +1193,7 @@
         <v>45</v>
       </c>
       <c r="E18" t="s">
-        <v>86</v>
+        <v>135</v>
       </c>
       <c r="F18" t="s">
         <v>6</v>
@@ -1246,7 +1213,7 @@
         <v>47</v>
       </c>
       <c r="E19" t="s">
-        <v>86</v>
+        <v>135</v>
       </c>
       <c r="F19" t="s">
         <v>6</v>
@@ -1266,7 +1233,7 @@
         <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>86</v>
+        <v>135</v>
       </c>
       <c r="F20" t="s">
         <v>6</v>
@@ -1286,7 +1253,7 @@
         <v>51</v>
       </c>
       <c r="E21" t="s">
-        <v>86</v>
+        <v>135</v>
       </c>
       <c r="F21" t="s">
         <v>6</v>
@@ -1306,7 +1273,7 @@
         <v>52</v>
       </c>
       <c r="E22" t="s">
-        <v>86</v>
+        <v>135</v>
       </c>
       <c r="F22" t="s">
         <v>6</v>
@@ -1317,7 +1284,7 @@
         <v>55</v>
       </c>
       <c r="B23" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C23" t="s">
         <v>28</v>
@@ -1326,7 +1293,7 @@
         <v>54</v>
       </c>
       <c r="E23" t="s">
-        <v>85</v>
+        <v>136</v>
       </c>
       <c r="F23" t="s">
         <v>6</v>
@@ -1337,7 +1304,7 @@
         <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C24" t="s">
         <v>28</v>
@@ -1346,7 +1313,7 @@
         <v>57</v>
       </c>
       <c r="E24" t="s">
-        <v>85</v>
+        <v>136</v>
       </c>
       <c r="F24" t="s">
         <v>6</v>
@@ -1357,7 +1324,7 @@
         <v>58</v>
       </c>
       <c r="B25" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C25" t="s">
         <v>28</v>
@@ -1366,7 +1333,7 @@
         <v>59</v>
       </c>
       <c r="E25" t="s">
-        <v>85</v>
+        <v>136</v>
       </c>
       <c r="F25" t="s">
         <v>6</v>
@@ -1377,7 +1344,7 @@
         <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C26" t="s">
         <v>28</v>
@@ -1386,7 +1353,7 @@
         <v>60</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="F26" t="s">
         <v>6</v>
@@ -1397,7 +1364,7 @@
         <v>62</v>
       </c>
       <c r="B27" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C27" t="s">
         <v>28</v>
@@ -1406,7 +1373,7 @@
         <v>63</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="F27" t="s">
         <v>6</v>
@@ -1417,7 +1384,7 @@
         <v>64</v>
       </c>
       <c r="B28" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C28" t="s">
         <v>28</v>
@@ -1426,7 +1393,7 @@
         <v>65</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="F28" t="s">
         <v>6</v>
@@ -1437,7 +1404,7 @@
         <v>66</v>
       </c>
       <c r="B29" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C29" t="s">
         <v>28</v>
@@ -1446,7 +1413,7 @@
         <v>67</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="F29" t="s">
         <v>6</v>
@@ -1457,7 +1424,7 @@
         <v>69</v>
       </c>
       <c r="B30" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C30" t="s">
         <v>28</v>
@@ -1466,7 +1433,7 @@
         <v>68</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="F30" t="s">
         <v>6</v>
@@ -1477,7 +1444,7 @@
         <v>71</v>
       </c>
       <c r="B31" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C31" t="s">
         <v>7</v>
@@ -1486,7 +1453,7 @@
         <v>70</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="F31" t="s">
         <v>6</v>
@@ -1497,7 +1464,7 @@
         <v>73</v>
       </c>
       <c r="B32" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C32" t="s">
         <v>7</v>
@@ -1506,7 +1473,7 @@
         <v>72</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="F32" t="s">
         <v>6</v>
@@ -1517,7 +1484,7 @@
         <v>74</v>
       </c>
       <c r="B33" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C33" t="s">
         <v>7</v>
@@ -1526,7 +1493,7 @@
         <v>75</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="F33" t="s">
         <v>6</v>
@@ -1537,7 +1504,7 @@
         <v>76</v>
       </c>
       <c r="B34" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C34" t="s">
         <v>7</v>
@@ -1546,7 +1513,7 @@
         <v>77</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="F34" t="s">
         <v>6</v>
@@ -1557,7 +1524,7 @@
         <v>78</v>
       </c>
       <c r="B35" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C35" t="s">
         <v>7</v>
@@ -1566,7 +1533,7 @@
         <v>79</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="F35" t="s">
         <v>6</v>
@@ -1577,7 +1544,7 @@
         <v>80</v>
       </c>
       <c r="B36" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C36" t="s">
         <v>7</v>
@@ -1586,7 +1553,7 @@
         <v>81</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="F36" t="s">
         <v>6</v>
@@ -1597,7 +1564,7 @@
         <v>82</v>
       </c>
       <c r="B37" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C37" t="s">
         <v>7</v>
@@ -1606,7 +1573,7 @@
         <v>83</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="F37" t="s">
         <v>6</v>
@@ -1614,19 +1581,19 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B38" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C38" t="s">
         <v>7</v>
       </c>
       <c r="D38" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F38" t="s">
         <v>6</v>
@@ -1634,19 +1601,19 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B39" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C39" t="s">
         <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F39" t="s">
         <v>6</v>
@@ -1654,19 +1621,19 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B40" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C40" t="s">
         <v>7</v>
       </c>
       <c r="D40" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="F40" t="s">
         <v>6</v>
@@ -1674,19 +1641,19 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B41" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C41" t="s">
         <v>7</v>
       </c>
       <c r="D41" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="F41" t="s">
         <v>6</v>
@@ -1694,19 +1661,19 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B42" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C42" t="s">
         <v>7</v>
       </c>
       <c r="D42" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="F42" t="s">
         <v>6</v>
@@ -1714,19 +1681,19 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B43" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C43" t="s">
         <v>7</v>
       </c>
       <c r="D43" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="F43" t="s">
         <v>6</v>
@@ -1737,16 +1704,16 @@
         <v>84</v>
       </c>
       <c r="B44" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C44" t="s">
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="F44" t="s">
         <v>6</v>
@@ -1754,19 +1721,19 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B45" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C45" t="s">
         <v>7</v>
       </c>
       <c r="D45" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="F45" t="s">
         <v>6</v>
@@ -1774,19 +1741,19 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B46" t="s">
+        <v>132</v>
+      </c>
+      <c r="C46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" t="s">
+        <v>100</v>
+      </c>
+      <c r="E46" s="3" t="s">
         <v>139</v>
-      </c>
-      <c r="C46" t="s">
-        <v>7</v>
-      </c>
-      <c r="D46" t="s">
-        <v>102</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>132</v>
       </c>
       <c r="F46" t="s">
         <v>6</v>
@@ -1794,19 +1761,19 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B47" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C47" t="s">
         <v>7</v>
       </c>
       <c r="D47" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="F47" t="s">
         <v>6</v>
@@ -1814,19 +1781,19 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B48" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C48" t="s">
         <v>7</v>
       </c>
       <c r="D48" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="F48" t="s">
         <v>6</v>
@@ -1834,19 +1801,19 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B49" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="C49" t="s">
         <v>7</v>
       </c>
       <c r="D49" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="F49" t="s">
         <v>6</v>
@@ -1854,19 +1821,19 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B50" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="C50" t="s">
         <v>7</v>
       </c>
       <c r="D50" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="F50" t="s">
         <v>6</v>
@@ -1874,19 +1841,19 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B51" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="C51" t="s">
         <v>7</v>
       </c>
       <c r="D51" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="F51" t="s">
         <v>6</v>
@@ -1894,19 +1861,19 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B52" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="C52" t="s">
         <v>7</v>
       </c>
       <c r="D52" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="F52" t="s">
         <v>6</v>
@@ -1914,19 +1881,19 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>113</v>
+      </c>
+      <c r="B53" t="s">
+        <v>134</v>
+      </c>
+      <c r="C53" t="s">
+        <v>114</v>
+      </c>
+      <c r="D53" t="s">
         <v>115</v>
       </c>
-      <c r="B53" t="s">
-        <v>146</v>
-      </c>
-      <c r="C53" t="s">
+      <c r="E53" t="s">
         <v>116</v>
-      </c>
-      <c r="D53" t="s">
-        <v>117</v>
-      </c>
-      <c r="E53" t="s">
-        <v>118</v>
       </c>
       <c r="F53" t="s">
         <v>6</v>
@@ -1934,19 +1901,19 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B54" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="C54" t="s">
+        <v>114</v>
+      </c>
+      <c r="D54" t="s">
+        <v>118</v>
+      </c>
+      <c r="E54" t="s">
         <v>116</v>
-      </c>
-      <c r="D54" t="s">
-        <v>120</v>
-      </c>
-      <c r="E54" t="s">
-        <v>118</v>
       </c>
       <c r="F54" t="s">
         <v>6</v>
@@ -1954,19 +1921,19 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B55" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="C55" t="s">
+        <v>114</v>
+      </c>
+      <c r="D55" t="s">
+        <v>120</v>
+      </c>
+      <c r="E55" t="s">
         <v>116</v>
-      </c>
-      <c r="D55" t="s">
-        <v>122</v>
-      </c>
-      <c r="E55" t="s">
-        <v>118</v>
       </c>
       <c r="F55" t="s">
         <v>6</v>
@@ -1974,19 +1941,19 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B56" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="C56" t="s">
         <v>7</v>
       </c>
       <c r="D56" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E56" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="F56" t="s">
         <v>6</v>
@@ -1994,19 +1961,19 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B57" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="C57" t="s">
         <v>7</v>
       </c>
       <c r="D57" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E57" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="F57" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Katalog guncellendi - Cmt 15.11.2025  9:15:53,53
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="206" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A52253AB-9A7D-43A2-A29D-B3141F74C512}"/>
+  <xr:revisionPtr revIDLastSave="208" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E082C57A-B8BE-4A32-B144-F7AD3F6BB580}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="142">
   <si>
     <t>urun_adi</t>
   </si>
@@ -443,6 +443,9 @@
   </si>
   <si>
     <t>%98 pamuk ve %2 spandex.31-32-33-34-36-38 Beden seçeneği mevcuttur.Ürünümüz tekli olarak satın alınabilir.Belirtilen fiyatlar adet fiyatıdır.</t>
+  </si>
+  <si>
+    <t>320 TL</t>
   </si>
 </sst>
 </file>
@@ -829,7 +832,7 @@
   <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56:E57"/>
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1944,7 +1947,7 @@
         <v>121</v>
       </c>
       <c r="B56" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="C56" t="s">
         <v>7</v>
@@ -1964,7 +1967,7 @@
         <v>123</v>
       </c>
       <c r="B57" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="C57" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Katalog guncellendi - Per 20.11.2025 17:17:16,26
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="208" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E082C57A-B8BE-4A32-B144-F7AD3F6BB580}"/>
+  <xr:revisionPtr revIDLastSave="210" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F34256A-86D0-43F5-8E4E-BCDFD71FE48F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -367,9 +367,6 @@
     <t>Mont</t>
   </si>
   <si>
-    <t>SOFTFÜME.jpg</t>
-  </si>
-  <si>
     <t>Su ve rüzgar geçirmez özelliği ile her türlü hava koşulunda konforlu bir kullanım sunar.Polar ve astar detayları ile ekstra sıcaklık ve konfor sağlar.S-M-L-XL-2XL-3XL Beden seçeneği mevcuttur.Ürünümüz serili olarak satılmaktadır.Belirtilen fiyatlar adet fiyatıdır.</t>
   </si>
   <si>
@@ -446,6 +443,9 @@
   </si>
   <si>
     <t>320 TL</t>
+  </si>
+  <si>
+    <t>SOFTFÜME.jpeg</t>
   </si>
 </sst>
 </file>
@@ -832,7 +832,7 @@
   <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,7 +876,7 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
@@ -896,7 +896,7 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
@@ -916,7 +916,7 @@
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F4" t="s">
         <v>6</v>
@@ -936,7 +936,7 @@
         <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F5" t="s">
         <v>6</v>
@@ -956,7 +956,7 @@
         <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F6" t="s">
         <v>6</v>
@@ -976,7 +976,7 @@
         <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F7" t="s">
         <v>6</v>
@@ -987,7 +987,7 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -996,7 +996,7 @@
         <v>26</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F8" t="s">
         <v>33</v>
@@ -1007,7 +1007,7 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -1016,7 +1016,7 @@
         <v>24</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F9" t="s">
         <v>6</v>
@@ -1027,7 +1027,7 @@
         <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -1036,7 +1036,7 @@
         <v>25</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F10" t="s">
         <v>6</v>
@@ -1056,7 +1056,7 @@
         <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F11" t="s">
         <v>6</v>
@@ -1076,7 +1076,7 @@
         <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F12" t="s">
         <v>6</v>
@@ -1096,7 +1096,7 @@
         <v>35</v>
       </c>
       <c r="E13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F13" t="s">
         <v>6</v>
@@ -1116,7 +1116,7 @@
         <v>37</v>
       </c>
       <c r="E14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F14" t="s">
         <v>6</v>
@@ -1136,7 +1136,7 @@
         <v>39</v>
       </c>
       <c r="E15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F15" t="s">
         <v>6</v>
@@ -1156,7 +1156,7 @@
         <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F16" t="s">
         <v>6</v>
@@ -1176,7 +1176,7 @@
         <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F17" t="s">
         <v>6</v>
@@ -1196,7 +1196,7 @@
         <v>45</v>
       </c>
       <c r="E18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F18" t="s">
         <v>6</v>
@@ -1216,7 +1216,7 @@
         <v>47</v>
       </c>
       <c r="E19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F19" t="s">
         <v>6</v>
@@ -1236,7 +1236,7 @@
         <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F20" t="s">
         <v>6</v>
@@ -1256,7 +1256,7 @@
         <v>51</v>
       </c>
       <c r="E21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F21" t="s">
         <v>6</v>
@@ -1276,7 +1276,7 @@
         <v>52</v>
       </c>
       <c r="E22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F22" t="s">
         <v>6</v>
@@ -1287,7 +1287,7 @@
         <v>55</v>
       </c>
       <c r="B23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C23" t="s">
         <v>28</v>
@@ -1296,7 +1296,7 @@
         <v>54</v>
       </c>
       <c r="E23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F23" t="s">
         <v>6</v>
@@ -1307,7 +1307,7 @@
         <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C24" t="s">
         <v>28</v>
@@ -1316,7 +1316,7 @@
         <v>57</v>
       </c>
       <c r="E24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F24" t="s">
         <v>6</v>
@@ -1327,7 +1327,7 @@
         <v>58</v>
       </c>
       <c r="B25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C25" t="s">
         <v>28</v>
@@ -1336,7 +1336,7 @@
         <v>59</v>
       </c>
       <c r="E25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F25" t="s">
         <v>6</v>
@@ -1347,7 +1347,7 @@
         <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C26" t="s">
         <v>28</v>
@@ -1356,7 +1356,7 @@
         <v>60</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F26" t="s">
         <v>6</v>
@@ -1367,7 +1367,7 @@
         <v>62</v>
       </c>
       <c r="B27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C27" t="s">
         <v>28</v>
@@ -1376,7 +1376,7 @@
         <v>63</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F27" t="s">
         <v>6</v>
@@ -1387,7 +1387,7 @@
         <v>64</v>
       </c>
       <c r="B28" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C28" t="s">
         <v>28</v>
@@ -1396,7 +1396,7 @@
         <v>65</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F28" t="s">
         <v>6</v>
@@ -1407,7 +1407,7 @@
         <v>66</v>
       </c>
       <c r="B29" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C29" t="s">
         <v>28</v>
@@ -1416,7 +1416,7 @@
         <v>67</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F29" t="s">
         <v>6</v>
@@ -1427,7 +1427,7 @@
         <v>69</v>
       </c>
       <c r="B30" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C30" t="s">
         <v>28</v>
@@ -1436,7 +1436,7 @@
         <v>68</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F30" t="s">
         <v>6</v>
@@ -1447,7 +1447,7 @@
         <v>71</v>
       </c>
       <c r="B31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C31" t="s">
         <v>7</v>
@@ -1456,7 +1456,7 @@
         <v>70</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F31" t="s">
         <v>6</v>
@@ -1467,7 +1467,7 @@
         <v>73</v>
       </c>
       <c r="B32" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C32" t="s">
         <v>7</v>
@@ -1476,7 +1476,7 @@
         <v>72</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F32" t="s">
         <v>6</v>
@@ -1487,7 +1487,7 @@
         <v>74</v>
       </c>
       <c r="B33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C33" t="s">
         <v>7</v>
@@ -1496,7 +1496,7 @@
         <v>75</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F33" t="s">
         <v>6</v>
@@ -1507,7 +1507,7 @@
         <v>76</v>
       </c>
       <c r="B34" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C34" t="s">
         <v>7</v>
@@ -1516,7 +1516,7 @@
         <v>77</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F34" t="s">
         <v>6</v>
@@ -1527,7 +1527,7 @@
         <v>78</v>
       </c>
       <c r="B35" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C35" t="s">
         <v>7</v>
@@ -1536,7 +1536,7 @@
         <v>79</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F35" t="s">
         <v>6</v>
@@ -1547,7 +1547,7 @@
         <v>80</v>
       </c>
       <c r="B36" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C36" t="s">
         <v>7</v>
@@ -1556,7 +1556,7 @@
         <v>81</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F36" t="s">
         <v>6</v>
@@ -1567,7 +1567,7 @@
         <v>82</v>
       </c>
       <c r="B37" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C37" t="s">
         <v>7</v>
@@ -1576,7 +1576,7 @@
         <v>83</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F37" t="s">
         <v>6</v>
@@ -1587,7 +1587,7 @@
         <v>86</v>
       </c>
       <c r="B38" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C38" t="s">
         <v>7</v>
@@ -1596,7 +1596,7 @@
         <v>85</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F38" t="s">
         <v>6</v>
@@ -1607,7 +1607,7 @@
         <v>88</v>
       </c>
       <c r="B39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C39" t="s">
         <v>7</v>
@@ -1616,7 +1616,7 @@
         <v>87</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F39" t="s">
         <v>6</v>
@@ -1627,7 +1627,7 @@
         <v>89</v>
       </c>
       <c r="B40" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C40" t="s">
         <v>7</v>
@@ -1636,7 +1636,7 @@
         <v>90</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F40" t="s">
         <v>6</v>
@@ -1647,7 +1647,7 @@
         <v>92</v>
       </c>
       <c r="B41" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C41" t="s">
         <v>7</v>
@@ -1656,7 +1656,7 @@
         <v>91</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F41" t="s">
         <v>6</v>
@@ -1667,7 +1667,7 @@
         <v>93</v>
       </c>
       <c r="B42" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C42" t="s">
         <v>7</v>
@@ -1676,7 +1676,7 @@
         <v>94</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F42" t="s">
         <v>6</v>
@@ -1687,7 +1687,7 @@
         <v>95</v>
       </c>
       <c r="B43" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C43" t="s">
         <v>7</v>
@@ -1696,7 +1696,7 @@
         <v>96</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F43" t="s">
         <v>6</v>
@@ -1707,7 +1707,7 @@
         <v>84</v>
       </c>
       <c r="B44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C44" t="s">
         <v>7</v>
@@ -1716,7 +1716,7 @@
         <v>97</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F44" t="s">
         <v>6</v>
@@ -1727,7 +1727,7 @@
         <v>98</v>
       </c>
       <c r="B45" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C45" t="s">
         <v>7</v>
@@ -1736,7 +1736,7 @@
         <v>99</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F45" t="s">
         <v>6</v>
@@ -1747,7 +1747,7 @@
         <v>101</v>
       </c>
       <c r="B46" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C46" t="s">
         <v>7</v>
@@ -1756,7 +1756,7 @@
         <v>100</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F46" t="s">
         <v>6</v>
@@ -1767,16 +1767,16 @@
         <v>102</v>
       </c>
       <c r="B47" t="s">
+        <v>131</v>
+      </c>
+      <c r="C47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" t="s">
         <v>132</v>
       </c>
-      <c r="C47" t="s">
-        <v>7</v>
-      </c>
-      <c r="D47" t="s">
-        <v>133</v>
-      </c>
       <c r="E47" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F47" t="s">
         <v>6</v>
@@ -1787,7 +1787,7 @@
         <v>103</v>
       </c>
       <c r="B48" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C48" t="s">
         <v>7</v>
@@ -1796,7 +1796,7 @@
         <v>104</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F48" t="s">
         <v>6</v>
@@ -1807,7 +1807,7 @@
         <v>105</v>
       </c>
       <c r="B49" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C49" t="s">
         <v>7</v>
@@ -1816,7 +1816,7 @@
         <v>106</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F49" t="s">
         <v>6</v>
@@ -1827,7 +1827,7 @@
         <v>107</v>
       </c>
       <c r="B50" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C50" t="s">
         <v>7</v>
@@ -1836,7 +1836,7 @@
         <v>108</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F50" t="s">
         <v>6</v>
@@ -1847,7 +1847,7 @@
         <v>109</v>
       </c>
       <c r="B51" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C51" t="s">
         <v>7</v>
@@ -1856,7 +1856,7 @@
         <v>110</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F51" t="s">
         <v>6</v>
@@ -1867,7 +1867,7 @@
         <v>111</v>
       </c>
       <c r="B52" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C52" t="s">
         <v>7</v>
@@ -1876,7 +1876,7 @@
         <v>112</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F52" t="s">
         <v>6</v>
@@ -1887,16 +1887,16 @@
         <v>113</v>
       </c>
       <c r="B53" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C53" t="s">
         <v>114</v>
       </c>
       <c r="D53" t="s">
+        <v>141</v>
+      </c>
+      <c r="E53" t="s">
         <v>115</v>
-      </c>
-      <c r="E53" t="s">
-        <v>116</v>
       </c>
       <c r="F53" t="s">
         <v>6</v>
@@ -1904,19 +1904,19 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B54" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C54" t="s">
         <v>114</v>
       </c>
       <c r="D54" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E54" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F54" t="s">
         <v>6</v>
@@ -1924,19 +1924,19 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B55" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C55" t="s">
         <v>114</v>
       </c>
       <c r="D55" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E55" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F55" t="s">
         <v>6</v>
@@ -1944,19 +1944,19 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>120</v>
+      </c>
+      <c r="B56" t="s">
+        <v>140</v>
+      </c>
+      <c r="C56" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" t="s">
         <v>121</v>
       </c>
-      <c r="B56" t="s">
-        <v>141</v>
-      </c>
-      <c r="C56" t="s">
-        <v>7</v>
-      </c>
-      <c r="D56" t="s">
-        <v>122</v>
-      </c>
       <c r="E56" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F56" t="s">
         <v>6</v>
@@ -1964,19 +1964,19 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>122</v>
+      </c>
+      <c r="B57" t="s">
+        <v>140</v>
+      </c>
+      <c r="C57" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57" t="s">
         <v>123</v>
       </c>
-      <c r="B57" t="s">
-        <v>141</v>
-      </c>
-      <c r="C57" t="s">
-        <v>7</v>
-      </c>
-      <c r="D57" t="s">
-        <v>124</v>
-      </c>
       <c r="E57" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F57" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Katalog guncellendi - Cum 21.11.2025 13:01:48,65
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="210" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F34256A-86D0-43F5-8E4E-BCDFD71FE48F}"/>
+  <xr:revisionPtr revIDLastSave="211" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE773A6A-47E4-4886-B945-A18DDE9ACBDB}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="157">
   <si>
     <t>urun_adi</t>
   </si>
@@ -446,6 +446,51 @@
   </si>
   <si>
     <t>SOFTFÜME.jpeg</t>
+  </si>
+  <si>
+    <t>FİYESMEN 1047 MONT AÇIK YEŞİL</t>
+  </si>
+  <si>
+    <t>1300 TL</t>
+  </si>
+  <si>
+    <t>S-M-L-XL-2XL Beden seçeneği mevcuttur.Ürünümüz serili olarak satılmaktadır.Belirtilen fiyatlar adet fiyatıdır.</t>
+  </si>
+  <si>
+    <t>fiyesmen1047montaçıkyeşil.jpg</t>
+  </si>
+  <si>
+    <t>1300TL</t>
+  </si>
+  <si>
+    <t>fiyesmen1047montantrasit.jpg</t>
+  </si>
+  <si>
+    <t>FİYESMEN 1047 MONT ANTRASİT</t>
+  </si>
+  <si>
+    <t>fiyesmen1047montgri.jpg</t>
+  </si>
+  <si>
+    <t>FİYESMEN 1047 MONT GRİ</t>
+  </si>
+  <si>
+    <t>fiyesmen1047montkahverengi.jpg</t>
+  </si>
+  <si>
+    <t>FİYESMEN 1047 MONT KAHVERENGİ</t>
+  </si>
+  <si>
+    <t>fiyesmen1047montsiyah.jpg</t>
+  </si>
+  <si>
+    <t>FİYESMEN 1047 MONT SİYAH</t>
+  </si>
+  <si>
+    <t>fiyesmen1047montyeşil.jpg</t>
+  </si>
+  <si>
+    <t>FİYESMEN 1047 MONT YEŞİL</t>
   </si>
 </sst>
 </file>
@@ -829,17 +874,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I50" sqref="I50"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.28515625" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="43.28515625" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1982,6 +2027,126 @@
         <v>6</v>
       </c>
     </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>142</v>
+      </c>
+      <c r="B58" t="s">
+        <v>143</v>
+      </c>
+      <c r="C58" t="s">
+        <v>114</v>
+      </c>
+      <c r="D58" t="s">
+        <v>145</v>
+      </c>
+      <c r="E58" t="s">
+        <v>144</v>
+      </c>
+      <c r="F58" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>148</v>
+      </c>
+      <c r="B59" t="s">
+        <v>146</v>
+      </c>
+      <c r="C59" t="s">
+        <v>114</v>
+      </c>
+      <c r="D59" t="s">
+        <v>147</v>
+      </c>
+      <c r="E59" t="s">
+        <v>144</v>
+      </c>
+      <c r="F59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>150</v>
+      </c>
+      <c r="B60" t="s">
+        <v>146</v>
+      </c>
+      <c r="C60" t="s">
+        <v>114</v>
+      </c>
+      <c r="D60" t="s">
+        <v>149</v>
+      </c>
+      <c r="E60" t="s">
+        <v>144</v>
+      </c>
+      <c r="F60" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>152</v>
+      </c>
+      <c r="B61" t="s">
+        <v>146</v>
+      </c>
+      <c r="C61" t="s">
+        <v>114</v>
+      </c>
+      <c r="D61" t="s">
+        <v>151</v>
+      </c>
+      <c r="E61" t="s">
+        <v>144</v>
+      </c>
+      <c r="F61" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>154</v>
+      </c>
+      <c r="B62" t="s">
+        <v>146</v>
+      </c>
+      <c r="C62" t="s">
+        <v>114</v>
+      </c>
+      <c r="D62" t="s">
+        <v>153</v>
+      </c>
+      <c r="E62" t="s">
+        <v>144</v>
+      </c>
+      <c r="F62" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>156</v>
+      </c>
+      <c r="B63" t="s">
+        <v>146</v>
+      </c>
+      <c r="C63" t="s">
+        <v>114</v>
+      </c>
+      <c r="D63" t="s">
+        <v>155</v>
+      </c>
+      <c r="E63" t="s">
+        <v>144</v>
+      </c>
+      <c r="F63" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Katalog guncellendi - Cum 21.11.2025 13:32:01,75
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="211" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE773A6A-47E4-4886-B945-A18DDE9ACBDB}"/>
+  <xr:revisionPtr revIDLastSave="217" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A8FFCE6-991E-4EEF-93EB-64335907A432}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="187">
   <si>
     <t>urun_adi</t>
   </si>
@@ -460,9 +460,6 @@
     <t>fiyesmen1047montaçıkyeşil.jpg</t>
   </si>
   <si>
-    <t>1300TL</t>
-  </si>
-  <si>
     <t>fiyesmen1047montantrasit.jpg</t>
   </si>
   <si>
@@ -491,13 +488,109 @@
   </si>
   <si>
     <t>FİYESMEN 1047 MONT YEŞİL</t>
+  </si>
+  <si>
+    <t>DERİ MONT SİYAH</t>
+  </si>
+  <si>
+    <t>derimont.jpg</t>
+  </si>
+  <si>
+    <t>945 TL</t>
+  </si>
+  <si>
+    <t>FİYESMEN1311MONCLERMONTSİYAH.jpg</t>
+  </si>
+  <si>
+    <t>FİYESMEN 1311 MONCLER MONT SİYAH</t>
+  </si>
+  <si>
+    <t>FİYESMEN1468MONHAKİ.jpg</t>
+  </si>
+  <si>
+    <t>FİYESMEN1468MONTSİYAH.JPG</t>
+  </si>
+  <si>
+    <t>FİYESMEN 1468 MONT HAKİ</t>
+  </si>
+  <si>
+    <t>FİYESMEN 1468 MONT SİYAH</t>
+  </si>
+  <si>
+    <t>FİYESMENNOVAMONTSİYAH.jpg</t>
+  </si>
+  <si>
+    <t>FİYESMEN NOVA MONT SİYAH</t>
+  </si>
+  <si>
+    <t>1070 TL</t>
+  </si>
+  <si>
+    <t>1450 TL</t>
+  </si>
+  <si>
+    <t>kadifemont.jpg</t>
+  </si>
+  <si>
+    <t>kadifemontkahve.jpg</t>
+  </si>
+  <si>
+    <t>KADİFE MONT SİYAH</t>
+  </si>
+  <si>
+    <t>KADİFE MONT KAHVERENGİ</t>
+  </si>
+  <si>
+    <t>1150 TL</t>
+  </si>
+  <si>
+    <t>LTFMONTGRİ.jpg</t>
+  </si>
+  <si>
+    <t>LTFMONTLACİVERT.jpg</t>
+  </si>
+  <si>
+    <t>LTF ŞİŞME MONT GRİ</t>
+  </si>
+  <si>
+    <t>LTF ŞİŞME  MONT LACİVERT</t>
+  </si>
+  <si>
+    <t>outdoormont.jpg</t>
+  </si>
+  <si>
+    <t>OUTDOOR MONT SİYAH</t>
+  </si>
+  <si>
+    <t>1200 TL</t>
+  </si>
+  <si>
+    <t>1100 TL</t>
+  </si>
+  <si>
+    <t>S-M-L-XL-2XL Beden seçeneği mevcuttur.Battal beden seçeneğimiz vardır.Ürünümüz serili olarak satılmaktadır.Belirtilen fiyatlar adet fiyatıdır.</t>
+  </si>
+  <si>
+    <t>POOLDEEP3017MONTBEJ.jpg</t>
+  </si>
+  <si>
+    <t>POOLDEEP3017MONTSİYAH.jpg</t>
+  </si>
+  <si>
+    <t>POOL DEEP 3017 MONT BEJ</t>
+  </si>
+  <si>
+    <t>POOL DEEP 3017 MONT SİYAH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -528,6 +621,13 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="162"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -562,19 +662,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Virgül" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -874,10 +977,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2049,16 +2152,16 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B59" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C59" t="s">
         <v>114</v>
       </c>
       <c r="D59" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E59" t="s">
         <v>144</v>
@@ -2069,16 +2172,16 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B60" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C60" t="s">
         <v>114</v>
       </c>
       <c r="D60" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E60" t="s">
         <v>144</v>
@@ -2089,16 +2192,16 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B61" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C61" t="s">
         <v>114</v>
       </c>
       <c r="D61" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E61" t="s">
         <v>144</v>
@@ -2109,16 +2212,16 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B62" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C62" t="s">
         <v>114</v>
       </c>
       <c r="D62" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E62" t="s">
         <v>144</v>
@@ -2129,21 +2232,261 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B63" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C63" t="s">
         <v>114</v>
       </c>
       <c r="D63" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E63" t="s">
         <v>144</v>
       </c>
       <c r="F63" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>156</v>
+      </c>
+      <c r="B64" t="s">
+        <v>158</v>
+      </c>
+      <c r="C64" t="s">
+        <v>114</v>
+      </c>
+      <c r="D64" t="s">
+        <v>157</v>
+      </c>
+      <c r="E64" t="s">
+        <v>144</v>
+      </c>
+      <c r="F64" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>160</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C65" t="s">
+        <v>114</v>
+      </c>
+      <c r="D65" t="s">
+        <v>159</v>
+      </c>
+      <c r="E65" t="s">
+        <v>144</v>
+      </c>
+      <c r="F65" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>163</v>
+      </c>
+      <c r="B66" t="s">
+        <v>167</v>
+      </c>
+      <c r="C66" t="s">
+        <v>114</v>
+      </c>
+      <c r="D66" t="s">
+        <v>161</v>
+      </c>
+      <c r="E66" t="s">
+        <v>144</v>
+      </c>
+      <c r="F66" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>164</v>
+      </c>
+      <c r="B67" t="s">
+        <v>167</v>
+      </c>
+      <c r="C67" t="s">
+        <v>114</v>
+      </c>
+      <c r="D67" t="s">
+        <v>162</v>
+      </c>
+      <c r="E67" t="s">
+        <v>144</v>
+      </c>
+      <c r="F67" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>166</v>
+      </c>
+      <c r="B68" t="s">
+        <v>167</v>
+      </c>
+      <c r="C68" t="s">
+        <v>114</v>
+      </c>
+      <c r="D68" t="s">
+        <v>165</v>
+      </c>
+      <c r="E68" t="s">
+        <v>144</v>
+      </c>
+      <c r="F68" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>171</v>
+      </c>
+      <c r="B69" t="s">
+        <v>173</v>
+      </c>
+      <c r="C69" t="s">
+        <v>114</v>
+      </c>
+      <c r="D69" t="s">
+        <v>169</v>
+      </c>
+      <c r="E69" t="s">
+        <v>144</v>
+      </c>
+      <c r="F69" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>172</v>
+      </c>
+      <c r="B70" t="s">
+        <v>173</v>
+      </c>
+      <c r="C70" t="s">
+        <v>114</v>
+      </c>
+      <c r="D70" t="s">
+        <v>170</v>
+      </c>
+      <c r="E70" t="s">
+        <v>144</v>
+      </c>
+      <c r="F70" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>176</v>
+      </c>
+      <c r="B71" t="s">
+        <v>181</v>
+      </c>
+      <c r="C71" t="s">
+        <v>114</v>
+      </c>
+      <c r="D71" t="s">
+        <v>174</v>
+      </c>
+      <c r="E71" t="s">
+        <v>144</v>
+      </c>
+      <c r="F71" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>177</v>
+      </c>
+      <c r="B72" t="s">
+        <v>181</v>
+      </c>
+      <c r="C72" t="s">
+        <v>114</v>
+      </c>
+      <c r="D72" t="s">
+        <v>175</v>
+      </c>
+      <c r="E72" t="s">
+        <v>144</v>
+      </c>
+      <c r="F72" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>179</v>
+      </c>
+      <c r="B73" t="s">
+        <v>180</v>
+      </c>
+      <c r="C73" t="s">
+        <v>114</v>
+      </c>
+      <c r="D73" t="s">
+        <v>178</v>
+      </c>
+      <c r="E73" t="s">
+        <v>182</v>
+      </c>
+      <c r="F73" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>185</v>
+      </c>
+      <c r="B74" t="s">
+        <v>167</v>
+      </c>
+      <c r="C74" t="s">
+        <v>114</v>
+      </c>
+      <c r="D74" t="s">
+        <v>183</v>
+      </c>
+      <c r="E74" t="s">
+        <v>144</v>
+      </c>
+      <c r="F74" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>186</v>
+      </c>
+      <c r="B75" t="s">
+        <v>167</v>
+      </c>
+      <c r="C75" t="s">
+        <v>114</v>
+      </c>
+      <c r="D75" t="s">
+        <v>184</v>
+      </c>
+      <c r="E75" t="s">
+        <v>144</v>
+      </c>
+      <c r="F75" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Katalog guncellendi - Cum 21.11.2025 13:35:16,64
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="217" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A8FFCE6-991E-4EEF-93EB-64335907A432}"/>
+  <xr:revisionPtr revIDLastSave="219" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{333008F7-6D5D-4D7D-B73A-9FE65680ECE4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -502,15 +502,9 @@
     <t>FİYESMEN1311MONCLERMONTSİYAH.jpg</t>
   </si>
   <si>
-    <t>FİYESMEN 1311 MONCLER MONT SİYAH</t>
-  </si>
-  <si>
     <t>FİYESMEN1468MONHAKİ.jpg</t>
   </si>
   <si>
-    <t>FİYESMEN1468MONTSİYAH.JPG</t>
-  </si>
-  <si>
     <t>FİYESMEN 1468 MONT HAKİ</t>
   </si>
   <si>
@@ -581,6 +575,12 @@
   </si>
   <si>
     <t>POOL DEEP 3017 MONT SİYAH</t>
+  </si>
+  <si>
+    <t>FİYESMEN1468MONTSİYAH.jpg</t>
+  </si>
+  <si>
+    <t>FİYESMEN 1311  MONT SİYAH</t>
   </si>
 </sst>
 </file>
@@ -980,7 +980,7 @@
   <dimension ref="A1:F75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2272,10 +2272,10 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>160</v>
+        <v>186</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C65" t="s">
         <v>114</v>
@@ -2292,16 +2292,16 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B66" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C66" t="s">
         <v>114</v>
       </c>
       <c r="D66" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E66" t="s">
         <v>144</v>
@@ -2312,16 +2312,16 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B67" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C67" t="s">
         <v>114</v>
       </c>
       <c r="D67" t="s">
-        <v>162</v>
+        <v>185</v>
       </c>
       <c r="E67" t="s">
         <v>144</v>
@@ -2332,16 +2332,16 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B68" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C68" t="s">
         <v>114</v>
       </c>
       <c r="D68" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E68" t="s">
         <v>144</v>
@@ -2352,16 +2352,16 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>169</v>
+      </c>
+      <c r="B69" t="s">
         <v>171</v>
-      </c>
-      <c r="B69" t="s">
-        <v>173</v>
       </c>
       <c r="C69" t="s">
         <v>114</v>
       </c>
       <c r="D69" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E69" t="s">
         <v>144</v>
@@ -2372,16 +2372,16 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B70" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C70" t="s">
         <v>114</v>
       </c>
       <c r="D70" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E70" t="s">
         <v>144</v>
@@ -2392,16 +2392,16 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B71" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C71" t="s">
         <v>114</v>
       </c>
       <c r="D71" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E71" t="s">
         <v>144</v>
@@ -2412,16 +2412,16 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B72" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C72" t="s">
         <v>114</v>
       </c>
       <c r="D72" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E72" t="s">
         <v>144</v>
@@ -2432,19 +2432,19 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B73" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C73" t="s">
         <v>114</v>
       </c>
       <c r="D73" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E73" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F73" t="s">
         <v>6</v>
@@ -2452,16 +2452,16 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B74" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C74" t="s">
         <v>114</v>
       </c>
       <c r="D74" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E74" t="s">
         <v>144</v>
@@ -2472,16 +2472,16 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B75" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C75" t="s">
         <v>114</v>
       </c>
       <c r="D75" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E75" t="s">
         <v>144</v>

</xml_diff>

<commit_message>
Katalog guncellendi - Pzt 24.11.2025 15:40:47,11
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="219" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{333008F7-6D5D-4D7D-B73A-9FE65680ECE4}"/>
+  <xr:revisionPtr revIDLastSave="220" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{383AA9B4-145C-4F41-BB96-9634E8A52E01}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="196">
   <si>
     <t>urun_adi</t>
   </si>
@@ -581,6 +581,33 @@
   </si>
   <si>
     <t>FİYESMEN 1311  MONT SİYAH</t>
+  </si>
+  <si>
+    <t>YELEK</t>
+  </si>
+  <si>
+    <t>5020HAKİ.jpg</t>
+  </si>
+  <si>
+    <t>ŞİŞME YELEK 5020 SOFT HAKİ</t>
+  </si>
+  <si>
+    <t>5020KAHVERENGİ.jpg</t>
+  </si>
+  <si>
+    <t>ŞİŞME YELEK 5020 SOFT  KAHVERENGİ</t>
+  </si>
+  <si>
+    <t>5020LACİVERT.jpg</t>
+  </si>
+  <si>
+    <t>ŞİŞME YELEK 5020 SOFT LACİVERT</t>
+  </si>
+  <si>
+    <t>5020SİYAH.jpg</t>
+  </si>
+  <si>
+    <t>ŞİŞME YELEK 5020 SOFT SİYAH</t>
   </si>
 </sst>
 </file>
@@ -977,10 +1004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2490,6 +2517,86 @@
         <v>6</v>
       </c>
     </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>189</v>
+      </c>
+      <c r="B76" t="s">
+        <v>128</v>
+      </c>
+      <c r="C76" t="s">
+        <v>187</v>
+      </c>
+      <c r="D76" t="s">
+        <v>188</v>
+      </c>
+      <c r="E76" t="s">
+        <v>144</v>
+      </c>
+      <c r="F76" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>191</v>
+      </c>
+      <c r="B77" t="s">
+        <v>128</v>
+      </c>
+      <c r="C77" t="s">
+        <v>187</v>
+      </c>
+      <c r="D77" t="s">
+        <v>190</v>
+      </c>
+      <c r="E77" t="s">
+        <v>144</v>
+      </c>
+      <c r="F77" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>193</v>
+      </c>
+      <c r="B78" t="s">
+        <v>128</v>
+      </c>
+      <c r="C78" t="s">
+        <v>187</v>
+      </c>
+      <c r="D78" t="s">
+        <v>192</v>
+      </c>
+      <c r="E78" t="s">
+        <v>144</v>
+      </c>
+      <c r="F78" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>195</v>
+      </c>
+      <c r="B79" t="s">
+        <v>128</v>
+      </c>
+      <c r="C79" t="s">
+        <v>187</v>
+      </c>
+      <c r="D79" t="s">
+        <v>194</v>
+      </c>
+      <c r="E79" t="s">
+        <v>144</v>
+      </c>
+      <c r="F79" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Katalog guncellendi - Pzt 24.11.2025 16:07:50,44
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="220" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{383AA9B4-145C-4F41-BB96-9634E8A52E01}"/>
+  <xr:revisionPtr revIDLastSave="224" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81DC3C61-8918-4DE8-8C37-D91234001B98}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -589,25 +589,25 @@
     <t>5020HAKİ.jpg</t>
   </si>
   <si>
-    <t>ŞİŞME YELEK 5020 SOFT HAKİ</t>
-  </si>
-  <si>
     <t>5020KAHVERENGİ.jpg</t>
   </si>
   <si>
-    <t>ŞİŞME YELEK 5020 SOFT  KAHVERENGİ</t>
-  </si>
-  <si>
     <t>5020LACİVERT.jpg</t>
   </si>
   <si>
-    <t>ŞİŞME YELEK 5020 SOFT LACİVERT</t>
-  </si>
-  <si>
     <t>5020SİYAH.jpg</t>
   </si>
   <si>
-    <t>ŞİŞME YELEK 5020 SOFT SİYAH</t>
+    <t>ŞİŞME YELEK 5010 SOFT HAKİ</t>
+  </si>
+  <si>
+    <t>ŞİŞME YELEK 5010 SOFT  KAHVERENGİ</t>
+  </si>
+  <si>
+    <t>ŞİŞME YELEK 5010 SOFT LACİVERT</t>
+  </si>
+  <si>
+    <t>ŞİŞME YELEK 5010 SOFT SİYAH</t>
   </si>
 </sst>
 </file>
@@ -1007,7 +1007,7 @@
   <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2519,7 +2519,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B76" t="s">
         <v>128</v>
@@ -2539,7 +2539,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B77" t="s">
         <v>128</v>
@@ -2548,7 +2548,7 @@
         <v>187</v>
       </c>
       <c r="D77" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E77" t="s">
         <v>144</v>
@@ -2559,7 +2559,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B78" t="s">
         <v>128</v>
@@ -2568,7 +2568,7 @@
         <v>187</v>
       </c>
       <c r="D78" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E78" t="s">
         <v>144</v>
@@ -2588,7 +2588,7 @@
         <v>187</v>
       </c>
       <c r="D79" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E79" t="s">
         <v>144</v>

</xml_diff>

<commit_message>
Katalog guncellendi - Pzt 24.11.2025 16:09:21,55
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="224" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81DC3C61-8918-4DE8-8C37-D91234001B98}"/>
+  <xr:revisionPtr revIDLastSave="226" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD7AE7DB-37EF-4581-834D-7F18B660487B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -583,9 +583,6 @@
     <t>FİYESMEN 1311  MONT SİYAH</t>
   </si>
   <si>
-    <t>YELEK</t>
-  </si>
-  <si>
     <t>5020HAKİ.jpg</t>
   </si>
   <si>
@@ -608,6 +605,9 @@
   </si>
   <si>
     <t>ŞİŞME YELEK 5010 SOFT SİYAH</t>
+  </si>
+  <si>
+    <t>Yelek</t>
   </si>
 </sst>
 </file>
@@ -1007,7 +1007,7 @@
   <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2519,16 +2519,16 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B76" t="s">
         <v>128</v>
       </c>
       <c r="C76" t="s">
+        <v>195</v>
+      </c>
+      <c r="D76" t="s">
         <v>187</v>
-      </c>
-      <c r="D76" t="s">
-        <v>188</v>
       </c>
       <c r="E76" t="s">
         <v>144</v>
@@ -2539,16 +2539,16 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B77" t="s">
         <v>128</v>
       </c>
       <c r="C77" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="D77" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E77" t="s">
         <v>144</v>
@@ -2559,16 +2559,16 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B78" t="s">
         <v>128</v>
       </c>
       <c r="C78" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="D78" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E78" t="s">
         <v>144</v>
@@ -2579,16 +2579,16 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B79" t="s">
         <v>128</v>
       </c>
       <c r="C79" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="D79" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E79" t="s">
         <v>144</v>

</xml_diff>

<commit_message>
Katalog guncellendi - Pzt 24.11.2025 16:21:53,79
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="226" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD7AE7DB-37EF-4581-834D-7F18B660487B}"/>
+  <xr:revisionPtr revIDLastSave="227" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8F8BD0E-5E15-4CC6-A8E5-47A9CF05455C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="207">
   <si>
     <t>urun_adi</t>
   </si>
@@ -608,6 +608,39 @@
   </si>
   <si>
     <t>Yelek</t>
+  </si>
+  <si>
+    <t>ŞİŞME YELEK 5020 NOVA KREM</t>
+  </si>
+  <si>
+    <t>500 TL</t>
+  </si>
+  <si>
+    <t>5020 NOVA YELEK KREM.jpg</t>
+  </si>
+  <si>
+    <t>5020novayelekbej.jpg</t>
+  </si>
+  <si>
+    <t>ŞİŞME YELEK 5020 NOVA BEJ</t>
+  </si>
+  <si>
+    <t>ŞİŞME YELEK 5020 NOVA KAHVERENGİ</t>
+  </si>
+  <si>
+    <t>5020NOVAYELEKKAHVERENGİ.jpg</t>
+  </si>
+  <si>
+    <t>ŞİŞME YELEK 5020 NOVA SİYAH</t>
+  </si>
+  <si>
+    <t>5020novayeleksiyah.jpg</t>
+  </si>
+  <si>
+    <t>5020NOVAYELEKTAŞ.jpg</t>
+  </si>
+  <si>
+    <t>ŞİŞME YELEK 5020 NOVA TAŞ</t>
   </si>
 </sst>
 </file>
@@ -1004,10 +1037,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D79" sqref="D79"/>
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2597,6 +2630,106 @@
         <v>6</v>
       </c>
     </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>196</v>
+      </c>
+      <c r="B80" t="s">
+        <v>197</v>
+      </c>
+      <c r="C80" t="s">
+        <v>195</v>
+      </c>
+      <c r="D80" t="s">
+        <v>198</v>
+      </c>
+      <c r="E80" t="s">
+        <v>144</v>
+      </c>
+      <c r="F80" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>200</v>
+      </c>
+      <c r="B81" t="s">
+        <v>197</v>
+      </c>
+      <c r="C81" t="s">
+        <v>195</v>
+      </c>
+      <c r="D81" t="s">
+        <v>199</v>
+      </c>
+      <c r="E81" t="s">
+        <v>144</v>
+      </c>
+      <c r="F81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>201</v>
+      </c>
+      <c r="B82" t="s">
+        <v>197</v>
+      </c>
+      <c r="C82" t="s">
+        <v>195</v>
+      </c>
+      <c r="D82" t="s">
+        <v>202</v>
+      </c>
+      <c r="E82" t="s">
+        <v>144</v>
+      </c>
+      <c r="F82" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>203</v>
+      </c>
+      <c r="B83" t="s">
+        <v>197</v>
+      </c>
+      <c r="C83" t="s">
+        <v>195</v>
+      </c>
+      <c r="D83" t="s">
+        <v>204</v>
+      </c>
+      <c r="E83" t="s">
+        <v>144</v>
+      </c>
+      <c r="F83" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>206</v>
+      </c>
+      <c r="B84" t="s">
+        <v>197</v>
+      </c>
+      <c r="C84" t="s">
+        <v>195</v>
+      </c>
+      <c r="D84" t="s">
+        <v>205</v>
+      </c>
+      <c r="E84" t="s">
+        <v>144</v>
+      </c>
+      <c r="F84" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Katalog guncellendi - Pzt 24.11.2025 16:36:06,92
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="227" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8F8BD0E-5E15-4CC6-A8E5-47A9CF05455C}"/>
+  <xr:revisionPtr revIDLastSave="228" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DABF13E-BD54-4D6B-B181-3DE0382C64DF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="215">
   <si>
     <t>urun_adi</t>
   </si>
@@ -641,6 +641,30 @@
   </si>
   <si>
     <t>ŞİŞME YELEK 5020 NOVA TAŞ</t>
+  </si>
+  <si>
+    <t>5010yelekkahverengi.jpg</t>
+  </si>
+  <si>
+    <t>5010yelekkrem.jpg</t>
+  </si>
+  <si>
+    <t>5010yeleksiyah.jpg</t>
+  </si>
+  <si>
+    <t>5010yelektaş.jpg</t>
+  </si>
+  <si>
+    <t>ŞİŞME YELEK 5010 YELEK KAHVERENGİ</t>
+  </si>
+  <si>
+    <t>ŞİŞME YELEK 5010 YELEK KREM</t>
+  </si>
+  <si>
+    <t>ŞİŞME YELEK 5010 YELEK SİYAH</t>
+  </si>
+  <si>
+    <t>ŞİŞME YELEK 5010 YELEKTAŞ</t>
   </si>
 </sst>
 </file>
@@ -1037,10 +1061,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F84"/>
+  <dimension ref="A1:F88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="H87" sqref="H87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2730,6 +2754,86 @@
         <v>6</v>
       </c>
     </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>211</v>
+      </c>
+      <c r="B85" t="s">
+        <v>197</v>
+      </c>
+      <c r="C85" t="s">
+        <v>195</v>
+      </c>
+      <c r="D85" t="s">
+        <v>207</v>
+      </c>
+      <c r="E85" t="s">
+        <v>144</v>
+      </c>
+      <c r="F85" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>212</v>
+      </c>
+      <c r="B86" t="s">
+        <v>197</v>
+      </c>
+      <c r="C86" t="s">
+        <v>195</v>
+      </c>
+      <c r="D86" t="s">
+        <v>208</v>
+      </c>
+      <c r="E86" t="s">
+        <v>144</v>
+      </c>
+      <c r="F86" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>213</v>
+      </c>
+      <c r="B87" t="s">
+        <v>197</v>
+      </c>
+      <c r="C87" t="s">
+        <v>195</v>
+      </c>
+      <c r="D87" t="s">
+        <v>209</v>
+      </c>
+      <c r="E87" t="s">
+        <v>144</v>
+      </c>
+      <c r="F87" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>214</v>
+      </c>
+      <c r="B88" t="s">
+        <v>197</v>
+      </c>
+      <c r="C88" t="s">
+        <v>195</v>
+      </c>
+      <c r="D88" t="s">
+        <v>210</v>
+      </c>
+      <c r="E88" t="s">
+        <v>144</v>
+      </c>
+      <c r="F88" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Katalog guncellendi - Pzt 24.11.2025 18:05:45,99
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sival\OneDrive\Desktop\SIVAL_GIYIM_KATALOG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="228" documentId="13_ncr:1_{C7CFE14E-4BC4-4266-90A5-F125D9DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DABF13E-BD54-4D6B-B181-3DE0382C64DF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="216">
   <si>
     <t>urun_adi</t>
   </si>
@@ -665,6 +665,9 @@
   </si>
   <si>
     <t>ŞİŞME YELEK 5010 YELEKTAŞ</t>
+  </si>
+  <si>
+    <t>S-M-L-XL-2XL-3XL Beden seçeneği mevcuttur.Ürünümüz serili olarak satılmaktadır.Belirtilen fiyatlar adet fiyatıdır.</t>
   </si>
 </sst>
 </file>
@@ -1064,7 +1067,7 @@
   <dimension ref="A1:F88"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="H87" sqref="H87"/>
+      <selection activeCell="E88" sqref="E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2588,7 +2591,7 @@
         <v>187</v>
       </c>
       <c r="E76" t="s">
-        <v>144</v>
+        <v>215</v>
       </c>
       <c r="F76" t="s">
         <v>6</v>
@@ -2608,7 +2611,7 @@
         <v>188</v>
       </c>
       <c r="E77" t="s">
-        <v>144</v>
+        <v>215</v>
       </c>
       <c r="F77" t="s">
         <v>6</v>
@@ -2628,7 +2631,7 @@
         <v>189</v>
       </c>
       <c r="E78" t="s">
-        <v>144</v>
+        <v>215</v>
       </c>
       <c r="F78" t="s">
         <v>6</v>
@@ -2648,7 +2651,7 @@
         <v>190</v>
       </c>
       <c r="E79" t="s">
-        <v>144</v>
+        <v>215</v>
       </c>
       <c r="F79" t="s">
         <v>6</v>
@@ -2668,7 +2671,7 @@
         <v>198</v>
       </c>
       <c r="E80" t="s">
-        <v>144</v>
+        <v>215</v>
       </c>
       <c r="F80" t="s">
         <v>6</v>
@@ -2688,7 +2691,7 @@
         <v>199</v>
       </c>
       <c r="E81" t="s">
-        <v>144</v>
+        <v>215</v>
       </c>
       <c r="F81" t="s">
         <v>6</v>
@@ -2708,7 +2711,7 @@
         <v>202</v>
       </c>
       <c r="E82" t="s">
-        <v>144</v>
+        <v>215</v>
       </c>
       <c r="F82" t="s">
         <v>6</v>
@@ -2728,7 +2731,7 @@
         <v>204</v>
       </c>
       <c r="E83" t="s">
-        <v>144</v>
+        <v>215</v>
       </c>
       <c r="F83" t="s">
         <v>6</v>
@@ -2748,7 +2751,7 @@
         <v>205</v>
       </c>
       <c r="E84" t="s">
-        <v>144</v>
+        <v>215</v>
       </c>
       <c r="F84" t="s">
         <v>6</v>
@@ -2768,7 +2771,7 @@
         <v>207</v>
       </c>
       <c r="E85" t="s">
-        <v>144</v>
+        <v>215</v>
       </c>
       <c r="F85" t="s">
         <v>6</v>
@@ -2788,7 +2791,7 @@
         <v>208</v>
       </c>
       <c r="E86" t="s">
-        <v>144</v>
+        <v>215</v>
       </c>
       <c r="F86" t="s">
         <v>6</v>
@@ -2808,7 +2811,7 @@
         <v>209</v>
       </c>
       <c r="E87" t="s">
-        <v>144</v>
+        <v>215</v>
       </c>
       <c r="F87" t="s">
         <v>6</v>
@@ -2828,7 +2831,7 @@
         <v>210</v>
       </c>
       <c r="E88" t="s">
-        <v>144</v>
+        <v>215</v>
       </c>
       <c r="F88" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Katalog guncellendi - Sal 25.11.2025 10:53:13,17
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sival\OneDrive\Desktop\SIVAL_GIYIM_KATALOG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F875AA8-6ECA-4F6F-9CA0-6DF37409FCB5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="231">
   <si>
     <t>urun_adi</t>
   </si>
@@ -668,6 +668,51 @@
   </si>
   <si>
     <t>S-M-L-XL-2XL-3XL Beden seçeneği mevcuttur.Ürünümüz serili olarak satılmaktadır.Belirtilen fiyatlar adet fiyatıdır.</t>
+  </si>
+  <si>
+    <t>ERKEK NUBUK CEKET TABA</t>
+  </si>
+  <si>
+    <t>440 TL</t>
+  </si>
+  <si>
+    <t>Ceket</t>
+  </si>
+  <si>
+    <t>TABANUBUK.jpg</t>
+  </si>
+  <si>
+    <t>S-M-L-XL-2XL Beden seçeneği mevcuttur.Dilerseniz battal beden mevcuttur.Ürünümüz serili olarak satılmaktadır.Belirtilen fiyatlar adet fiyatıdır.</t>
+  </si>
+  <si>
+    <t>GRİNUBUK.jpg</t>
+  </si>
+  <si>
+    <t>ERKEK NUBUK CEKET GRİ</t>
+  </si>
+  <si>
+    <t>HAKİNUBUK.jpg</t>
+  </si>
+  <si>
+    <t>ERKEK NUBUK CEKET HAKİ</t>
+  </si>
+  <si>
+    <t>KAHVERENGİNUBUK.jpg</t>
+  </si>
+  <si>
+    <t>ERKEK NUBUK CEKET KAHVERENGİ</t>
+  </si>
+  <si>
+    <t>LACİVERTNUBUK.jpg</t>
+  </si>
+  <si>
+    <t>ERKEK NUBUK CEKET LACİVERT</t>
+  </si>
+  <si>
+    <t>SİYAHNUBUK.jpg</t>
+  </si>
+  <si>
+    <t>ERKEK NUBUK CEKET SİYAH</t>
   </si>
 </sst>
 </file>
@@ -1064,10 +1109,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F88"/>
+  <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="E88" sqref="E88"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="E94" sqref="E94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2837,6 +2882,126 @@
         <v>6</v>
       </c>
     </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>216</v>
+      </c>
+      <c r="B89" t="s">
+        <v>217</v>
+      </c>
+      <c r="C89" t="s">
+        <v>218</v>
+      </c>
+      <c r="D89" t="s">
+        <v>219</v>
+      </c>
+      <c r="E89" t="s">
+        <v>220</v>
+      </c>
+      <c r="F89" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>222</v>
+      </c>
+      <c r="B90" t="s">
+        <v>217</v>
+      </c>
+      <c r="C90" t="s">
+        <v>218</v>
+      </c>
+      <c r="D90" t="s">
+        <v>221</v>
+      </c>
+      <c r="E90" t="s">
+        <v>220</v>
+      </c>
+      <c r="F90" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>224</v>
+      </c>
+      <c r="B91" t="s">
+        <v>217</v>
+      </c>
+      <c r="C91" t="s">
+        <v>218</v>
+      </c>
+      <c r="D91" t="s">
+        <v>223</v>
+      </c>
+      <c r="E91" t="s">
+        <v>220</v>
+      </c>
+      <c r="F91" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>226</v>
+      </c>
+      <c r="B92" t="s">
+        <v>217</v>
+      </c>
+      <c r="C92" t="s">
+        <v>218</v>
+      </c>
+      <c r="D92" t="s">
+        <v>225</v>
+      </c>
+      <c r="E92" t="s">
+        <v>220</v>
+      </c>
+      <c r="F92" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>228</v>
+      </c>
+      <c r="B93" t="s">
+        <v>217</v>
+      </c>
+      <c r="C93" t="s">
+        <v>218</v>
+      </c>
+      <c r="D93" t="s">
+        <v>227</v>
+      </c>
+      <c r="E93" t="s">
+        <v>220</v>
+      </c>
+      <c r="F93" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>230</v>
+      </c>
+      <c r="B94" t="s">
+        <v>217</v>
+      </c>
+      <c r="C94" t="s">
+        <v>218</v>
+      </c>
+      <c r="D94" t="s">
+        <v>229</v>
+      </c>
+      <c r="E94" t="s">
+        <v>220</v>
+      </c>
+      <c r="F94" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Katalog guncellendi - Sal 25.11.2025 11:01:35,94
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F875AA8-6ECA-4F6F-9CA0-6DF37409FCB5}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A354F69-C2CD-4463-8BB3-68314514F610}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="237">
   <si>
     <t>urun_adi</t>
   </si>
@@ -713,6 +713,24 @@
   </si>
   <si>
     <t>ERKEK NUBUK CEKET SİYAH</t>
+  </si>
+  <si>
+    <t>YAKALINUBUKSİYAH.jpg</t>
+  </si>
+  <si>
+    <t>ERKEK YAKALI NUBUK CEKET SİYAH</t>
+  </si>
+  <si>
+    <t>YAKALINUBUKGRİ.jpg</t>
+  </si>
+  <si>
+    <t>ERKEK YAKALI NUBUK CEKET GRİ</t>
+  </si>
+  <si>
+    <t>YAKALINUBUKLACİ.jpg</t>
+  </si>
+  <si>
+    <t>ERKEK YAKALI NUBUK CEKET LACİVERT</t>
   </si>
 </sst>
 </file>
@@ -1109,10 +1127,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F94"/>
+  <dimension ref="A1:F97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="E94" sqref="E94"/>
+      <selection activeCell="I92" sqref="I92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3002,6 +3020,66 @@
         <v>6</v>
       </c>
     </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>232</v>
+      </c>
+      <c r="B95" t="s">
+        <v>217</v>
+      </c>
+      <c r="C95" t="s">
+        <v>218</v>
+      </c>
+      <c r="D95" t="s">
+        <v>231</v>
+      </c>
+      <c r="E95" t="s">
+        <v>144</v>
+      </c>
+      <c r="F95" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>234</v>
+      </c>
+      <c r="B96" t="s">
+        <v>217</v>
+      </c>
+      <c r="C96" t="s">
+        <v>218</v>
+      </c>
+      <c r="D96" t="s">
+        <v>233</v>
+      </c>
+      <c r="E96" t="s">
+        <v>144</v>
+      </c>
+      <c r="F96" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>236</v>
+      </c>
+      <c r="B97" t="s">
+        <v>217</v>
+      </c>
+      <c r="C97" t="s">
+        <v>218</v>
+      </c>
+      <c r="D97" t="s">
+        <v>235</v>
+      </c>
+      <c r="E97" t="s">
+        <v>144</v>
+      </c>
+      <c r="F97" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Katalog guncellendi - Sal 25.11.2025 11:07:01,09
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A354F69-C2CD-4463-8BB3-68314514F610}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9F23855-E94A-4965-9F71-74AA140AAD08}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="241">
   <si>
     <t>urun_adi</t>
   </si>
@@ -731,6 +731,18 @@
   </si>
   <si>
     <t>ERKEK YAKALI NUBUK CEKET LACİVERT</t>
+  </si>
+  <si>
+    <t>ERKEK KAPİTONE CEKET</t>
+  </si>
+  <si>
+    <t>kapitone3.jpg</t>
+  </si>
+  <si>
+    <t>kapitone2.jpg</t>
+  </si>
+  <si>
+    <t>kapitone1.jpg</t>
   </si>
 </sst>
 </file>
@@ -1127,10 +1139,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F97"/>
+  <dimension ref="A1:F100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="I92" sqref="I92"/>
+      <selection activeCell="E99" sqref="E99:E100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3080,6 +3092,66 @@
         <v>6</v>
       </c>
     </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>237</v>
+      </c>
+      <c r="B98" t="s">
+        <v>128</v>
+      </c>
+      <c r="C98" t="s">
+        <v>218</v>
+      </c>
+      <c r="D98" t="s">
+        <v>238</v>
+      </c>
+      <c r="E98" t="s">
+        <v>144</v>
+      </c>
+      <c r="F98" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>237</v>
+      </c>
+      <c r="B99" t="s">
+        <v>128</v>
+      </c>
+      <c r="C99" t="s">
+        <v>218</v>
+      </c>
+      <c r="D99" t="s">
+        <v>239</v>
+      </c>
+      <c r="E99" t="s">
+        <v>144</v>
+      </c>
+      <c r="F99" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>237</v>
+      </c>
+      <c r="B100" t="s">
+        <v>128</v>
+      </c>
+      <c r="C100" t="s">
+        <v>218</v>
+      </c>
+      <c r="D100" t="s">
+        <v>240</v>
+      </c>
+      <c r="E100" t="s">
+        <v>144</v>
+      </c>
+      <c r="F100" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Katalog guncellendi - Çar 26.11.2025 12:08:54,83
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9F23855-E94A-4965-9F71-74AA140AAD08}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{651CFBEF-6974-4EFE-8D4C-FCADDAE07A9B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="249">
   <si>
     <t>urun_adi</t>
   </si>
@@ -743,6 +743,30 @@
   </si>
   <si>
     <t>kapitone1.jpg</t>
+  </si>
+  <si>
+    <t>ŞİŞME YELEK 2053 SAVMOD SİYAH</t>
+  </si>
+  <si>
+    <t>420 TL</t>
+  </si>
+  <si>
+    <t>savmod.jpg</t>
+  </si>
+  <si>
+    <t>ŞİŞME YELEK   3004 ALARA DERİ YELEK SİYAH</t>
+  </si>
+  <si>
+    <t>ŞİŞME YELEK   3004 ALARA DERİ YELEK HAKİ</t>
+  </si>
+  <si>
+    <t>590 TL</t>
+  </si>
+  <si>
+    <t>deriyelek.jpg</t>
+  </si>
+  <si>
+    <t>deriyelekhaki.jpg</t>
   </si>
 </sst>
 </file>
@@ -1139,10 +1163,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F100"/>
+  <dimension ref="A1:F103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="E99" sqref="E99:E100"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="D104" sqref="D104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3152,6 +3176,66 @@
         <v>6</v>
       </c>
     </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>241</v>
+      </c>
+      <c r="B101" t="s">
+        <v>242</v>
+      </c>
+      <c r="C101" t="s">
+        <v>195</v>
+      </c>
+      <c r="D101" t="s">
+        <v>243</v>
+      </c>
+      <c r="E101" t="s">
+        <v>215</v>
+      </c>
+      <c r="F101" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>244</v>
+      </c>
+      <c r="B102" t="s">
+        <v>246</v>
+      </c>
+      <c r="C102" t="s">
+        <v>195</v>
+      </c>
+      <c r="D102" t="s">
+        <v>247</v>
+      </c>
+      <c r="E102" t="s">
+        <v>215</v>
+      </c>
+      <c r="F102" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>245</v>
+      </c>
+      <c r="B103" t="s">
+        <v>246</v>
+      </c>
+      <c r="C103" t="s">
+        <v>195</v>
+      </c>
+      <c r="D103" t="s">
+        <v>248</v>
+      </c>
+      <c r="E103" t="s">
+        <v>215</v>
+      </c>
+      <c r="F103" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Katalog guncellendi - Çar 26.11.2025 12:51:17,51
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{651CFBEF-6974-4EFE-8D4C-FCADDAE07A9B}"/>
+  <xr:revisionPtr revIDLastSave="85" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F469F30B-487D-4452-93CB-DD95C8C4DE9B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="254">
   <si>
     <t>urun_adi</t>
   </si>
@@ -664,9 +664,6 @@
     <t>ŞİŞME YELEK 5010 YELEK SİYAH</t>
   </si>
   <si>
-    <t>ŞİŞME YELEK 5010 YELEKTAŞ</t>
-  </si>
-  <si>
     <t>S-M-L-XL-2XL-3XL Beden seçeneği mevcuttur.Ürünümüz serili olarak satılmaktadır.Belirtilen fiyatlar adet fiyatıdır.</t>
   </si>
   <si>
@@ -754,12 +751,6 @@
     <t>savmod.jpg</t>
   </si>
   <si>
-    <t>ŞİŞME YELEK   3004 ALARA DERİ YELEK SİYAH</t>
-  </si>
-  <si>
-    <t>ŞİŞME YELEK   3004 ALARA DERİ YELEK HAKİ</t>
-  </si>
-  <si>
     <t>590 TL</t>
   </si>
   <si>
@@ -767,6 +758,30 @@
   </si>
   <si>
     <t>deriyelekhaki.jpg</t>
+  </si>
+  <si>
+    <t>ŞİŞME YELEK 5010 YELEK TAŞ</t>
+  </si>
+  <si>
+    <t>ŞİŞME YELEK   3004 ALARA  YELEK SİYAH</t>
+  </si>
+  <si>
+    <t>ŞİŞME YELEK   3004 ALARA  YELEK HAKİ</t>
+  </si>
+  <si>
+    <t>ERKEK ŞİŞME YELEK 5431 HAKİ</t>
+  </si>
+  <si>
+    <t>ERKEK ŞİŞME YELEK 5431 SİYAH</t>
+  </si>
+  <si>
+    <t>575 TL</t>
+  </si>
+  <si>
+    <t>erkek yelek5431.jpg</t>
+  </si>
+  <si>
+    <t>erkekyeleksiyah.jpg</t>
   </si>
 </sst>
 </file>
@@ -1163,10 +1178,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F103"/>
+  <dimension ref="A1:F105"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="D104" sqref="D104"/>
+      <selection activeCell="E108" sqref="E108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2690,7 +2705,7 @@
         <v>187</v>
       </c>
       <c r="E76" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F76" t="s">
         <v>6</v>
@@ -2710,7 +2725,7 @@
         <v>188</v>
       </c>
       <c r="E77" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F77" t="s">
         <v>6</v>
@@ -2730,7 +2745,7 @@
         <v>189</v>
       </c>
       <c r="E78" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F78" t="s">
         <v>6</v>
@@ -2750,7 +2765,7 @@
         <v>190</v>
       </c>
       <c r="E79" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F79" t="s">
         <v>6</v>
@@ -2770,7 +2785,7 @@
         <v>198</v>
       </c>
       <c r="E80" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F80" t="s">
         <v>6</v>
@@ -2790,7 +2805,7 @@
         <v>199</v>
       </c>
       <c r="E81" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F81" t="s">
         <v>6</v>
@@ -2810,7 +2825,7 @@
         <v>202</v>
       </c>
       <c r="E82" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F82" t="s">
         <v>6</v>
@@ -2830,7 +2845,7 @@
         <v>204</v>
       </c>
       <c r="E83" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F83" t="s">
         <v>6</v>
@@ -2850,7 +2865,7 @@
         <v>205</v>
       </c>
       <c r="E84" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F84" t="s">
         <v>6</v>
@@ -2870,7 +2885,7 @@
         <v>207</v>
       </c>
       <c r="E85" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F85" t="s">
         <v>6</v>
@@ -2890,7 +2905,7 @@
         <v>208</v>
       </c>
       <c r="E86" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F86" t="s">
         <v>6</v>
@@ -2910,7 +2925,7 @@
         <v>209</v>
       </c>
       <c r="E87" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F87" t="s">
         <v>6</v>
@@ -2918,7 +2933,7 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>214</v>
+        <v>246</v>
       </c>
       <c r="B88" t="s">
         <v>197</v>
@@ -2930,7 +2945,7 @@
         <v>210</v>
       </c>
       <c r="E88" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F88" t="s">
         <v>6</v>
@@ -2938,19 +2953,19 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>215</v>
+      </c>
+      <c r="B89" t="s">
         <v>216</v>
       </c>
-      <c r="B89" t="s">
+      <c r="C89" t="s">
         <v>217</v>
       </c>
-      <c r="C89" t="s">
+      <c r="D89" t="s">
         <v>218</v>
       </c>
-      <c r="D89" t="s">
+      <c r="E89" t="s">
         <v>219</v>
-      </c>
-      <c r="E89" t="s">
-        <v>220</v>
       </c>
       <c r="F89" t="s">
         <v>6</v>
@@ -2958,19 +2973,19 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B90" t="s">
+        <v>216</v>
+      </c>
+      <c r="C90" t="s">
         <v>217</v>
       </c>
-      <c r="C90" t="s">
-        <v>218</v>
-      </c>
       <c r="D90" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E90" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F90" t="s">
         <v>6</v>
@@ -2978,19 +2993,19 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B91" t="s">
+        <v>216</v>
+      </c>
+      <c r="C91" t="s">
         <v>217</v>
       </c>
-      <c r="C91" t="s">
-        <v>218</v>
-      </c>
       <c r="D91" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E91" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F91" t="s">
         <v>6</v>
@@ -2998,19 +3013,19 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B92" t="s">
+        <v>216</v>
+      </c>
+      <c r="C92" t="s">
         <v>217</v>
       </c>
-      <c r="C92" t="s">
-        <v>218</v>
-      </c>
       <c r="D92" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E92" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F92" t="s">
         <v>6</v>
@@ -3018,19 +3033,19 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B93" t="s">
+        <v>216</v>
+      </c>
+      <c r="C93" t="s">
         <v>217</v>
       </c>
-      <c r="C93" t="s">
-        <v>218</v>
-      </c>
       <c r="D93" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E93" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F93" t="s">
         <v>6</v>
@@ -3038,19 +3053,19 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B94" t="s">
+        <v>216</v>
+      </c>
+      <c r="C94" t="s">
         <v>217</v>
       </c>
-      <c r="C94" t="s">
-        <v>218</v>
-      </c>
       <c r="D94" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E94" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F94" t="s">
         <v>6</v>
@@ -3058,16 +3073,16 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B95" t="s">
+        <v>216</v>
+      </c>
+      <c r="C95" t="s">
         <v>217</v>
       </c>
-      <c r="C95" t="s">
-        <v>218</v>
-      </c>
       <c r="D95" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E95" t="s">
         <v>144</v>
@@ -3078,16 +3093,16 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B96" t="s">
+        <v>216</v>
+      </c>
+      <c r="C96" t="s">
         <v>217</v>
       </c>
-      <c r="C96" t="s">
-        <v>218</v>
-      </c>
       <c r="D96" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E96" t="s">
         <v>144</v>
@@ -3098,16 +3113,16 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B97" t="s">
+        <v>216</v>
+      </c>
+      <c r="C97" t="s">
         <v>217</v>
       </c>
-      <c r="C97" t="s">
-        <v>218</v>
-      </c>
       <c r="D97" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E97" t="s">
         <v>144</v>
@@ -3118,16 +3133,16 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B98" t="s">
         <v>128</v>
       </c>
       <c r="C98" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D98" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E98" t="s">
         <v>144</v>
@@ -3138,16 +3153,16 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B99" t="s">
         <v>128</v>
       </c>
       <c r="C99" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D99" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E99" t="s">
         <v>144</v>
@@ -3158,16 +3173,16 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B100" t="s">
         <v>128</v>
       </c>
       <c r="C100" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D100" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E100" t="s">
         <v>144</v>
@@ -3178,19 +3193,19 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
+        <v>240</v>
+      </c>
+      <c r="B101" t="s">
         <v>241</v>
-      </c>
-      <c r="B101" t="s">
-        <v>242</v>
       </c>
       <c r="C101" t="s">
         <v>195</v>
       </c>
       <c r="D101" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E101" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F101" t="s">
         <v>6</v>
@@ -3198,19 +3213,19 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="B102" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C102" t="s">
         <v>195</v>
       </c>
       <c r="D102" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E102" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F102" t="s">
         <v>6</v>
@@ -3218,21 +3233,61 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B103" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C103" t="s">
         <v>195</v>
       </c>
       <c r="D103" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E103" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F103" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>249</v>
+      </c>
+      <c r="B104" t="s">
+        <v>251</v>
+      </c>
+      <c r="C104" t="s">
+        <v>195</v>
+      </c>
+      <c r="D104" t="s">
+        <v>252</v>
+      </c>
+      <c r="E104" t="s">
+        <v>214</v>
+      </c>
+      <c r="F104" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>250</v>
+      </c>
+      <c r="B105" t="s">
+        <v>251</v>
+      </c>
+      <c r="C105" t="s">
+        <v>195</v>
+      </c>
+      <c r="D105" t="s">
+        <v>253</v>
+      </c>
+      <c r="E105" t="s">
+        <v>214</v>
+      </c>
+      <c r="F105" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Katalog guncellendi - Per 27.11.2025 10:34:41,30
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F469F30B-487D-4452-93CB-DD95C8C4DE9B}"/>
+  <xr:revisionPtr revIDLastSave="109" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB48942C-B9FF-4126-9DE5-4C97ECEC72DE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="264">
   <si>
     <t>urun_adi</t>
   </si>
@@ -782,6 +782,36 @@
   </si>
   <si>
     <t>erkekyeleksiyah.jpg</t>
+  </si>
+  <si>
+    <t>280 TL</t>
+  </si>
+  <si>
+    <t>Sweat</t>
+  </si>
+  <si>
+    <t>MASTİF3050SİY.jpg</t>
+  </si>
+  <si>
+    <t>MASTİF 3050  3 İP SWEATSHİRT SİYAH</t>
+  </si>
+  <si>
+    <t>MASTİF3050MAVİ.jpg</t>
+  </si>
+  <si>
+    <t>MASTİF 3050  3 İP SWEATSHİRT MAVİ</t>
+  </si>
+  <si>
+    <t>MASTİF3050LACİ.jpg</t>
+  </si>
+  <si>
+    <t>MASTİF 3050  3 İP SWEATSHİRT LACİVERT</t>
+  </si>
+  <si>
+    <t>MASTİF3050SUYEŞ.jpg</t>
+  </si>
+  <si>
+    <t>MASTİF 3050  3 İP SWEATSHİRT SU YEŞİLİ</t>
   </si>
 </sst>
 </file>
@@ -1178,10 +1208,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F105"/>
+  <dimension ref="A1:F109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="E108" sqref="E108"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="E102" sqref="E102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3291,6 +3321,86 @@
         <v>6</v>
       </c>
     </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>257</v>
+      </c>
+      <c r="B106" t="s">
+        <v>254</v>
+      </c>
+      <c r="C106" t="s">
+        <v>255</v>
+      </c>
+      <c r="D106" t="s">
+        <v>256</v>
+      </c>
+      <c r="E106" t="s">
+        <v>214</v>
+      </c>
+      <c r="F106" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>259</v>
+      </c>
+      <c r="B107" t="s">
+        <v>254</v>
+      </c>
+      <c r="C107" t="s">
+        <v>255</v>
+      </c>
+      <c r="D107" t="s">
+        <v>258</v>
+      </c>
+      <c r="E107" t="s">
+        <v>214</v>
+      </c>
+      <c r="F107" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>261</v>
+      </c>
+      <c r="B108" t="s">
+        <v>254</v>
+      </c>
+      <c r="C108" t="s">
+        <v>255</v>
+      </c>
+      <c r="D108" t="s">
+        <v>260</v>
+      </c>
+      <c r="E108" t="s">
+        <v>214</v>
+      </c>
+      <c r="F108" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>263</v>
+      </c>
+      <c r="B109" t="s">
+        <v>254</v>
+      </c>
+      <c r="C109" t="s">
+        <v>255</v>
+      </c>
+      <c r="D109" t="s">
+        <v>262</v>
+      </c>
+      <c r="E109" t="s">
+        <v>214</v>
+      </c>
+      <c r="F109" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Katalog guncellendi - Per 27.11.2025 10:52:59,17
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -1210,8 +1210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="E102" sqref="E102"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="I108" sqref="I108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Katalog guncellendi - Per 27.11.2025 10:54:45,08
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="109" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB48942C-B9FF-4126-9DE5-4C97ECEC72DE}"/>
+  <xr:revisionPtr revIDLastSave="111" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{975FCBEF-F1CA-4FF0-A5BD-93C6C7059E1B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="265">
   <si>
     <t>urun_adi</t>
   </si>
@@ -812,6 +812,9 @@
   </si>
   <si>
     <t>MASTİF 3050  3 İP SWEATSHİRT SU YEŞİLİ</t>
+  </si>
+  <si>
+    <t>S-M-L-XL-2XL  Beden seçeneği mevcuttur.Ürünümüz serili olarak satılmaktadır.Belirtilen fiyatlar adet fiyatıdır.</t>
   </si>
 </sst>
 </file>
@@ -1211,7 +1214,7 @@
   <dimension ref="A1:F109"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="I108" sqref="I108"/>
+      <selection activeCell="E111" sqref="E111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3335,7 +3338,7 @@
         <v>256</v>
       </c>
       <c r="E106" t="s">
-        <v>214</v>
+        <v>264</v>
       </c>
       <c r="F106" t="s">
         <v>33</v>
@@ -3355,7 +3358,7 @@
         <v>258</v>
       </c>
       <c r="E107" t="s">
-        <v>214</v>
+        <v>264</v>
       </c>
       <c r="F107" t="s">
         <v>33</v>
@@ -3375,7 +3378,7 @@
         <v>260</v>
       </c>
       <c r="E108" t="s">
-        <v>214</v>
+        <v>264</v>
       </c>
       <c r="F108" t="s">
         <v>33</v>
@@ -3395,7 +3398,7 @@
         <v>262</v>
       </c>
       <c r="E109" t="s">
-        <v>214</v>
+        <v>264</v>
       </c>
       <c r="F109" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
Katalog guncellendi - Per 27.11.2025 11:13:03,64
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="111" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{975FCBEF-F1CA-4FF0-A5BD-93C6C7059E1B}"/>
+  <xr:revisionPtr revIDLastSave="112" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78BBD766-A53B-4FA6-81E6-36869966712D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="276">
   <si>
     <t>urun_adi</t>
   </si>
@@ -815,6 +815,39 @@
   </si>
   <si>
     <t>S-M-L-XL-2XL  Beden seçeneği mevcuttur.Ürünümüz serili olarak satılmaktadır.Belirtilen fiyatlar adet fiyatıdır.</t>
+  </si>
+  <si>
+    <t>BOLD BROTHERS 6011 YARIM FERMUAR SWEAT BEYAZ</t>
+  </si>
+  <si>
+    <t>bold6011beyaz.jpg</t>
+  </si>
+  <si>
+    <t>BOLD BROTHERS 6011 YARIM FERMUAR SWEAT LACİVERT</t>
+  </si>
+  <si>
+    <t>bold6011laci.jpg</t>
+  </si>
+  <si>
+    <t>BOLD BROTHERS 6011 YARIM FERMUAR SWEAT MAVİ</t>
+  </si>
+  <si>
+    <t>bold6011mavi.jpg</t>
+  </si>
+  <si>
+    <t>BOLD BROTHERS 6011 YARIM FERMUAR SWEAT SİYAH</t>
+  </si>
+  <si>
+    <t>bold6011siyahj.pg</t>
+  </si>
+  <si>
+    <t>BOLD BROTHERS 6011 YARIM FERMUAR SWEAT YEŞİL</t>
+  </si>
+  <si>
+    <t>bold6011yeşil.jpg</t>
+  </si>
+  <si>
+    <t>400 Ttl</t>
   </si>
 </sst>
 </file>
@@ -1211,15 +1244,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F109"/>
+  <dimension ref="A1:F114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="E111" sqref="E111"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" customWidth="1"/>
+    <col min="1" max="1" width="52.28515625" customWidth="1"/>
     <col min="4" max="4" width="43.28515625" customWidth="1"/>
     <col min="5" max="5" width="22.7109375" customWidth="1"/>
   </cols>
@@ -3341,7 +3374,7 @@
         <v>264</v>
       </c>
       <c r="F106" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
@@ -3361,7 +3394,7 @@
         <v>264</v>
       </c>
       <c r="F107" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
@@ -3381,7 +3414,7 @@
         <v>264</v>
       </c>
       <c r="F108" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
@@ -3401,7 +3434,107 @@
         <v>264</v>
       </c>
       <c r="F109" t="s">
-        <v>33</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>265</v>
+      </c>
+      <c r="B110" t="s">
+        <v>275</v>
+      </c>
+      <c r="C110" t="s">
+        <v>255</v>
+      </c>
+      <c r="D110" t="s">
+        <v>266</v>
+      </c>
+      <c r="E110" t="s">
+        <v>264</v>
+      </c>
+      <c r="F110" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>267</v>
+      </c>
+      <c r="B111" t="s">
+        <v>275</v>
+      </c>
+      <c r="C111" t="s">
+        <v>255</v>
+      </c>
+      <c r="D111" t="s">
+        <v>268</v>
+      </c>
+      <c r="E111" t="s">
+        <v>264</v>
+      </c>
+      <c r="F111" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>269</v>
+      </c>
+      <c r="B112" t="s">
+        <v>275</v>
+      </c>
+      <c r="C112" t="s">
+        <v>255</v>
+      </c>
+      <c r="D112" t="s">
+        <v>270</v>
+      </c>
+      <c r="E112" t="s">
+        <v>264</v>
+      </c>
+      <c r="F112" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>271</v>
+      </c>
+      <c r="B113" t="s">
+        <v>275</v>
+      </c>
+      <c r="C113" t="s">
+        <v>255</v>
+      </c>
+      <c r="D113" t="s">
+        <v>272</v>
+      </c>
+      <c r="E113" t="s">
+        <v>264</v>
+      </c>
+      <c r="F113" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>273</v>
+      </c>
+      <c r="B114" t="s">
+        <v>275</v>
+      </c>
+      <c r="C114" t="s">
+        <v>255</v>
+      </c>
+      <c r="D114" t="s">
+        <v>274</v>
+      </c>
+      <c r="E114" t="s">
+        <v>264</v>
+      </c>
+      <c r="F114" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Katalog guncellendi - Per 27.11.2025 11:15:01,59
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="112" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78BBD766-A53B-4FA6-81E6-36869966712D}"/>
+  <xr:revisionPtr revIDLastSave="113" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D917CA32-3F01-4A96-BCE3-6B31758F2CAC}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -838,9 +838,6 @@
     <t>BOLD BROTHERS 6011 YARIM FERMUAR SWEAT SİYAH</t>
   </si>
   <si>
-    <t>bold6011siyahj.pg</t>
-  </si>
-  <si>
     <t>BOLD BROTHERS 6011 YARIM FERMUAR SWEAT YEŞİL</t>
   </si>
   <si>
@@ -848,6 +845,9 @@
   </si>
   <si>
     <t>400 Ttl</t>
+  </si>
+  <si>
+    <t>bold6011siyahj.jpg</t>
   </si>
 </sst>
 </file>
@@ -1246,8 +1246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B114" sqref="B114"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="D107" sqref="D107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3442,7 +3442,7 @@
         <v>265</v>
       </c>
       <c r="B110" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C110" t="s">
         <v>255</v>
@@ -3462,7 +3462,7 @@
         <v>267</v>
       </c>
       <c r="B111" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C111" t="s">
         <v>255</v>
@@ -3482,7 +3482,7 @@
         <v>269</v>
       </c>
       <c r="B112" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C112" t="s">
         <v>255</v>
@@ -3502,13 +3502,13 @@
         <v>271</v>
       </c>
       <c r="B113" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C113" t="s">
         <v>255</v>
       </c>
       <c r="D113" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="E113" t="s">
         <v>264</v>
@@ -3519,16 +3519,16 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B114" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C114" t="s">
         <v>255</v>
       </c>
       <c r="D114" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E114" t="s">
         <v>264</v>

</xml_diff>

<commit_message>
Katalog guncellendi - Per 27.11.2025 11:18:02,20
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="113" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D917CA32-3F01-4A96-BCE3-6B31758F2CAC}"/>
+  <xr:revisionPtr revIDLastSave="123" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4095393-7028-4F7A-A326-E338AE05A880}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="275">
   <si>
     <t>urun_adi</t>
   </si>
@@ -842,9 +842,6 @@
   </si>
   <si>
     <t>bold6011yeşil.jpg</t>
-  </si>
-  <si>
-    <t>400 Ttl</t>
   </si>
   <si>
     <t>bold6011siyahj.jpg</t>
@@ -1246,8 +1243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="D107" sqref="D107"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="B118" sqref="B118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3442,7 +3439,7 @@
         <v>265</v>
       </c>
       <c r="B110" t="s">
-        <v>274</v>
+        <v>128</v>
       </c>
       <c r="C110" t="s">
         <v>255</v>
@@ -3462,7 +3459,7 @@
         <v>267</v>
       </c>
       <c r="B111" t="s">
-        <v>274</v>
+        <v>128</v>
       </c>
       <c r="C111" t="s">
         <v>255</v>
@@ -3482,7 +3479,7 @@
         <v>269</v>
       </c>
       <c r="B112" t="s">
-        <v>274</v>
+        <v>128</v>
       </c>
       <c r="C112" t="s">
         <v>255</v>
@@ -3502,13 +3499,13 @@
         <v>271</v>
       </c>
       <c r="B113" t="s">
-        <v>274</v>
+        <v>128</v>
       </c>
       <c r="C113" t="s">
         <v>255</v>
       </c>
       <c r="D113" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E113" t="s">
         <v>264</v>
@@ -3522,7 +3519,7 @@
         <v>272</v>
       </c>
       <c r="B114" t="s">
-        <v>274</v>
+        <v>128</v>
       </c>
       <c r="C114" t="s">
         <v>255</v>

</xml_diff>

<commit_message>
Katalog guncellendi - Per 27.11.2025 11:20:05,44
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="123" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4095393-7028-4F7A-A326-E338AE05A880}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B85529F-B081-4806-8E48-F77C2729D707}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -844,7 +844,7 @@
     <t>bold6011yeşil.jpg</t>
   </si>
   <si>
-    <t>bold6011siyahj.jpg</t>
+    <t>bold6011siyah.jpg</t>
   </si>
 </sst>
 </file>
@@ -1244,7 +1244,7 @@
   <dimension ref="A1:F114"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B118" sqref="B118"/>
+      <selection activeCell="D114" sqref="D114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Katalog guncellendi - Per 27.11.2025 11:29:11,88
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="125" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B85529F-B081-4806-8E48-F77C2729D707}"/>
+  <xr:revisionPtr revIDLastSave="147" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDB38BF1-5269-41D1-B205-9B4873751B46}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="283">
   <si>
     <t>urun_adi</t>
   </si>
@@ -845,6 +845,30 @@
   </si>
   <si>
     <t>bold6011siyah.jpg</t>
+  </si>
+  <si>
+    <t>475 TL</t>
+  </si>
+  <si>
+    <t>S-M-L-XL  Beden seçeneği mevcuttur.Ürünümüz serili olarak satılmaktadır.Belirtilen fiyatlar adet fiyatıdır.</t>
+  </si>
+  <si>
+    <t>BOLD BROTHERS 6033 KAŞE GÖMLEK GRİ</t>
+  </si>
+  <si>
+    <t>BOLD BROTHERS 6033 KAŞE GÖMLEK YEŞİL</t>
+  </si>
+  <si>
+    <t>BOLD BROTHERS 6033 KAŞE GÖMLEK LACİVERT</t>
+  </si>
+  <si>
+    <t>KAŞEGÖMLEKLACİ.jpg</t>
+  </si>
+  <si>
+    <t>KAŞEGÖMLEKGRİ.jpg</t>
+  </si>
+  <si>
+    <t>KAŞEGÖMLEKYEŞİL.jpg</t>
   </si>
 </sst>
 </file>
@@ -1241,10 +1265,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F114"/>
+  <dimension ref="A1:F117"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="D114" sqref="D114"/>
+      <selection activeCell="B126" sqref="B126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3534,6 +3558,66 @@
         <v>6</v>
       </c>
     </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>279</v>
+      </c>
+      <c r="B115" t="s">
+        <v>275</v>
+      </c>
+      <c r="C115" t="s">
+        <v>28</v>
+      </c>
+      <c r="D115" t="s">
+        <v>280</v>
+      </c>
+      <c r="E115" t="s">
+        <v>276</v>
+      </c>
+      <c r="F115" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>277</v>
+      </c>
+      <c r="B116" t="s">
+        <v>275</v>
+      </c>
+      <c r="C116" t="s">
+        <v>28</v>
+      </c>
+      <c r="D116" t="s">
+        <v>281</v>
+      </c>
+      <c r="E116" t="s">
+        <v>276</v>
+      </c>
+      <c r="F116" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>278</v>
+      </c>
+      <c r="B117" t="s">
+        <v>275</v>
+      </c>
+      <c r="C117" t="s">
+        <v>28</v>
+      </c>
+      <c r="D117" t="s">
+        <v>282</v>
+      </c>
+      <c r="E117" t="s">
+        <v>276</v>
+      </c>
+      <c r="F117" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Katalog guncellendi - Per 27.11.2025 11:32:27,02
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="147" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDB38BF1-5269-41D1-B205-9B4873751B46}"/>
+  <xr:revisionPtr revIDLastSave="150" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BEB9CA2-3622-4317-AE98-A091CA88B94D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="284">
   <si>
     <t>urun_adi</t>
   </si>
@@ -869,6 +869,9 @@
   </si>
   <si>
     <t>KAŞEGÖMLEKYEŞİL.jpg</t>
+  </si>
+  <si>
+    <t>Yok</t>
   </si>
 </sst>
 </file>
@@ -1267,8 +1270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B126" sqref="B126"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2675,7 +2678,7 @@
         <v>144</v>
       </c>
       <c r="F70" t="s">
-        <v>6</v>
+        <v>283</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -2695,7 +2698,7 @@
         <v>144</v>
       </c>
       <c r="F71" t="s">
-        <v>6</v>
+        <v>283</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -2735,7 +2738,7 @@
         <v>180</v>
       </c>
       <c r="F73" t="s">
-        <v>6</v>
+        <v>283</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Katalog guncellendi - Per 27.11.2025 18:11:40,00
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="150" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BEB9CA2-3622-4317-AE98-A091CA88B94D}"/>
+  <xr:revisionPtr revIDLastSave="151" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFD1627D-EE7E-490E-A3AC-58B41BB99EA8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1271,7 +1271,7 @@
   <dimension ref="A1:F117"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="F70" sqref="F70"/>
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2738,7 +2738,7 @@
         <v>180</v>
       </c>
       <c r="F73" t="s">
-        <v>283</v>
+        <v>6</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Katalog guncellendi - Cum 28.11.2025 10:54:43,78
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="151" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFD1627D-EE7E-490E-A3AC-58B41BB99EA8}"/>
+  <xr:revisionPtr revIDLastSave="152" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF2C9AE0-C4A1-4D62-B407-F0B7B2E4F430}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1270,8 +1270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1518,7 +1518,7 @@
         <v>134</v>
       </c>
       <c r="F12" t="s">
-        <v>6</v>
+        <v>283</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Katalog guncellendi - Cmt 29.11.2025 10:44:30,20
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="152" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF2C9AE0-C4A1-4D62-B407-F0B7B2E4F430}"/>
+  <xr:revisionPtr revIDLastSave="156" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5B79EE3-861E-4417-91C5-AB61488FC768}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="301">
   <si>
     <t>urun_adi</t>
   </si>
@@ -872,6 +872,57 @@
   </si>
   <si>
     <t>Yok</t>
+  </si>
+  <si>
+    <t>195 TL</t>
+  </si>
+  <si>
+    <t>KAZAK</t>
+  </si>
+  <si>
+    <t>SELANİKKOYUMAVİ.jpg</t>
+  </si>
+  <si>
+    <t>SELANİK GÖMLEK YAKA KAZAK KOYU MAVİ</t>
+  </si>
+  <si>
+    <t>SELANİK GÖMLEK YAKA KAZAK GRİ</t>
+  </si>
+  <si>
+    <t>SELANİK GÖMLEK YAKA KAZAK SİYAH</t>
+  </si>
+  <si>
+    <t>SELANİKSİYAH.jpg</t>
+  </si>
+  <si>
+    <t>SELANİKGRİ.jpg</t>
+  </si>
+  <si>
+    <t>SELANİK GÖMLEK YAKA KAZAK KOYU YEŞİL</t>
+  </si>
+  <si>
+    <t>SELANİKKOYUYEŞİLjpg</t>
+  </si>
+  <si>
+    <t>SELANİKMAVİ.jpg</t>
+  </si>
+  <si>
+    <t>SELANİK GÖMLEK YAKA KAZAK MAVİ</t>
+  </si>
+  <si>
+    <t>SELANİK GÖMLEK YAKA KAZAK BEJ</t>
+  </si>
+  <si>
+    <t>SELANİKBEJ.jpg</t>
+  </si>
+  <si>
+    <t>SELANİK GÖMLEK YAKA KAZAK YEŞİL</t>
+  </si>
+  <si>
+    <t>SELANİKYEŞİL.jpg</t>
+  </si>
+  <si>
+    <t>M-L-XL-2XL  Beden seçeneği mevcuttur.Ürünümüz serili olarak satılmaktadır.Belirtilen fiyatlar adet fiyatıdır.</t>
   </si>
 </sst>
 </file>
@@ -1268,10 +1319,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F117"/>
+  <dimension ref="A1:F124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="E125" sqref="E125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3621,6 +3672,146 @@
         <v>6</v>
       </c>
     </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>287</v>
+      </c>
+      <c r="B118" t="s">
+        <v>284</v>
+      </c>
+      <c r="C118" t="s">
+        <v>285</v>
+      </c>
+      <c r="D118" t="s">
+        <v>286</v>
+      </c>
+      <c r="E118" t="s">
+        <v>300</v>
+      </c>
+      <c r="F118" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>288</v>
+      </c>
+      <c r="B119" t="s">
+        <v>284</v>
+      </c>
+      <c r="C119" t="s">
+        <v>285</v>
+      </c>
+      <c r="D119" t="s">
+        <v>291</v>
+      </c>
+      <c r="E119" t="s">
+        <v>300</v>
+      </c>
+      <c r="F119" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>289</v>
+      </c>
+      <c r="B120" t="s">
+        <v>284</v>
+      </c>
+      <c r="C120" t="s">
+        <v>285</v>
+      </c>
+      <c r="D120" t="s">
+        <v>290</v>
+      </c>
+      <c r="E120" t="s">
+        <v>300</v>
+      </c>
+      <c r="F120" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>292</v>
+      </c>
+      <c r="B121" t="s">
+        <v>284</v>
+      </c>
+      <c r="C121" t="s">
+        <v>285</v>
+      </c>
+      <c r="D121" t="s">
+        <v>293</v>
+      </c>
+      <c r="E121" t="s">
+        <v>300</v>
+      </c>
+      <c r="F121" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>295</v>
+      </c>
+      <c r="B122" t="s">
+        <v>284</v>
+      </c>
+      <c r="C122" t="s">
+        <v>285</v>
+      </c>
+      <c r="D122" t="s">
+        <v>294</v>
+      </c>
+      <c r="E122" t="s">
+        <v>300</v>
+      </c>
+      <c r="F122" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>296</v>
+      </c>
+      <c r="B123" t="s">
+        <v>284</v>
+      </c>
+      <c r="C123" t="s">
+        <v>285</v>
+      </c>
+      <c r="D123" t="s">
+        <v>297</v>
+      </c>
+      <c r="E123" t="s">
+        <v>300</v>
+      </c>
+      <c r="F123" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>298</v>
+      </c>
+      <c r="B124" t="s">
+        <v>284</v>
+      </c>
+      <c r="C124" t="s">
+        <v>285</v>
+      </c>
+      <c r="D124" t="s">
+        <v>299</v>
+      </c>
+      <c r="E124" t="s">
+        <v>300</v>
+      </c>
+      <c r="F124" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Katalog guncellendi - Cmt 29.11.2025 10:47:17,10
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="156" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5B79EE3-861E-4417-91C5-AB61488FC768}"/>
+  <xr:revisionPtr revIDLastSave="159" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8EF58338-A703-4CE3-B10C-E43AD7E836E9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -877,9 +877,6 @@
     <t>195 TL</t>
   </si>
   <si>
-    <t>KAZAK</t>
-  </si>
-  <si>
     <t>SELANİKKOYUMAVİ.jpg</t>
   </si>
   <si>
@@ -901,9 +898,6 @@
     <t>SELANİK GÖMLEK YAKA KAZAK KOYU YEŞİL</t>
   </si>
   <si>
-    <t>SELANİKKOYUYEŞİLjpg</t>
-  </si>
-  <si>
     <t>SELANİKMAVİ.jpg</t>
   </si>
   <si>
@@ -923,6 +917,12 @@
   </si>
   <si>
     <t>M-L-XL-2XL  Beden seçeneği mevcuttur.Ürünümüz serili olarak satılmaktadır.Belirtilen fiyatlar adet fiyatıdır.</t>
+  </si>
+  <si>
+    <t>SELANİKKOYUYEŞİL.jpg</t>
+  </si>
+  <si>
+    <t>Kazak</t>
   </si>
 </sst>
 </file>
@@ -1322,7 +1322,7 @@
   <dimension ref="A1:F124"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="E125" sqref="E125"/>
+      <selection activeCell="C118" sqref="C118:C124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3674,19 +3674,19 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B118" t="s">
         <v>284</v>
       </c>
       <c r="C118" t="s">
+        <v>300</v>
+      </c>
+      <c r="D118" t="s">
         <v>285</v>
       </c>
-      <c r="D118" t="s">
-        <v>286</v>
-      </c>
       <c r="E118" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F118" t="s">
         <v>6</v>
@@ -3694,19 +3694,19 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B119" t="s">
         <v>284</v>
       </c>
       <c r="C119" t="s">
-        <v>285</v>
+        <v>300</v>
       </c>
       <c r="D119" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E119" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F119" t="s">
         <v>6</v>
@@ -3714,19 +3714,19 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B120" t="s">
         <v>284</v>
       </c>
       <c r="C120" t="s">
-        <v>285</v>
+        <v>300</v>
       </c>
       <c r="D120" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E120" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F120" t="s">
         <v>6</v>
@@ -3734,19 +3734,19 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B121" t="s">
         <v>284</v>
       </c>
       <c r="C121" t="s">
-        <v>285</v>
+        <v>300</v>
       </c>
       <c r="D121" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="E121" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F121" t="s">
         <v>6</v>
@@ -3754,19 +3754,19 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B122" t="s">
         <v>284</v>
       </c>
       <c r="C122" t="s">
-        <v>285</v>
+        <v>300</v>
       </c>
       <c r="D122" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E122" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F122" t="s">
         <v>6</v>
@@ -3774,19 +3774,19 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B123" t="s">
         <v>284</v>
       </c>
       <c r="C123" t="s">
-        <v>285</v>
+        <v>300</v>
       </c>
       <c r="D123" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E123" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F123" t="s">
         <v>6</v>
@@ -3794,19 +3794,19 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B124" t="s">
         <v>284</v>
       </c>
       <c r="C124" t="s">
-        <v>285</v>
+        <v>300</v>
       </c>
       <c r="D124" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E124" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F124" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Katalog guncellendi - Per 04.12.2025 12:02:47,87
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/SIVAL_GIYIM_KATALOG/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/CEREN-PC/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="159" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8EF58338-A703-4CE3-B10C-E43AD7E836E9}"/>
+  <xr:revisionPtr revIDLastSave="165" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CD4944B-66C6-483A-9F4F-A4645C9C3C0A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -400,9 +400,6 @@
     <t>%98 pamuk içeriğine sahiptir..Bağcıklı kapama şekli ve lastikli bel detayı sayesinde  rahatlığından ödün vermez.34-36-38-40-42-44-46 Beden aralığı mevcuttur.Ürünümüz tekli olarak satın alınabilir.Belirtilen fiyatlar adet fiyatıdır.</t>
   </si>
   <si>
-    <t>%100 pamuklu kumaşı sayesinde gün boyu konfor sunar ve cildin nefes almasını sağlar.30-31-32-33-34-36-38-40 Beden seçeneği mevcuttur.Ürünümüz tekli olarak satın alınabilir.Belirtilen fiyatlar adet fiyatıdır.</t>
-  </si>
-  <si>
     <t>350 TL</t>
   </si>
   <si>
@@ -923,6 +920,9 @@
   </si>
   <si>
     <t>Kazak</t>
+  </si>
+  <si>
+    <t>%98 pamuk ve %2 spandex. 30-31-32-33-34-36-38-40 Beden seçeneği mevcuttur.Belirtilen fiyatlar adet fiyatıdır.</t>
   </si>
 </sst>
 </file>
@@ -1321,8 +1321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="C118" sqref="C118:C124"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38:E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1477,7 +1477,7 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -1497,7 +1497,7 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -1517,7 +1517,7 @@
         <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -1546,7 +1546,7 @@
         <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F11" t="s">
         <v>6</v>
@@ -1566,10 +1566,10 @@
         <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F12" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1586,7 +1586,7 @@
         <v>35</v>
       </c>
       <c r="E13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F13" t="s">
         <v>6</v>
@@ -1606,7 +1606,7 @@
         <v>37</v>
       </c>
       <c r="E14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F14" t="s">
         <v>6</v>
@@ -1626,7 +1626,7 @@
         <v>39</v>
       </c>
       <c r="E15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F15" t="s">
         <v>6</v>
@@ -1646,7 +1646,7 @@
         <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F16" t="s">
         <v>6</v>
@@ -1666,7 +1666,7 @@
         <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F17" t="s">
         <v>6</v>
@@ -1686,7 +1686,7 @@
         <v>45</v>
       </c>
       <c r="E18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F18" t="s">
         <v>6</v>
@@ -1706,7 +1706,7 @@
         <v>47</v>
       </c>
       <c r="E19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F19" t="s">
         <v>6</v>
@@ -1726,7 +1726,7 @@
         <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F20" t="s">
         <v>6</v>
@@ -1746,7 +1746,7 @@
         <v>51</v>
       </c>
       <c r="E21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F21" t="s">
         <v>6</v>
@@ -1766,7 +1766,7 @@
         <v>52</v>
       </c>
       <c r="E22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F22" t="s">
         <v>6</v>
@@ -1777,7 +1777,7 @@
         <v>55</v>
       </c>
       <c r="B23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C23" t="s">
         <v>28</v>
@@ -1786,7 +1786,7 @@
         <v>54</v>
       </c>
       <c r="E23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F23" t="s">
         <v>6</v>
@@ -1797,7 +1797,7 @@
         <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C24" t="s">
         <v>28</v>
@@ -1806,7 +1806,7 @@
         <v>57</v>
       </c>
       <c r="E24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F24" t="s">
         <v>6</v>
@@ -1817,7 +1817,7 @@
         <v>58</v>
       </c>
       <c r="B25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C25" t="s">
         <v>28</v>
@@ -1826,7 +1826,7 @@
         <v>59</v>
       </c>
       <c r="E25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F25" t="s">
         <v>6</v>
@@ -1837,7 +1837,7 @@
         <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C26" t="s">
         <v>28</v>
@@ -1846,7 +1846,7 @@
         <v>60</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F26" t="s">
         <v>6</v>
@@ -1857,7 +1857,7 @@
         <v>62</v>
       </c>
       <c r="B27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C27" t="s">
         <v>28</v>
@@ -1866,7 +1866,7 @@
         <v>63</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F27" t="s">
         <v>6</v>
@@ -1877,7 +1877,7 @@
         <v>64</v>
       </c>
       <c r="B28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C28" t="s">
         <v>28</v>
@@ -1886,7 +1886,7 @@
         <v>65</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F28" t="s">
         <v>6</v>
@@ -1897,7 +1897,7 @@
         <v>66</v>
       </c>
       <c r="B29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C29" t="s">
         <v>28</v>
@@ -1906,7 +1906,7 @@
         <v>67</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F29" t="s">
         <v>6</v>
@@ -1917,7 +1917,7 @@
         <v>69</v>
       </c>
       <c r="B30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C30" t="s">
         <v>28</v>
@@ -1926,7 +1926,7 @@
         <v>68</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F30" t="s">
         <v>6</v>
@@ -1937,7 +1937,7 @@
         <v>71</v>
       </c>
       <c r="B31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C31" t="s">
         <v>7</v>
@@ -1946,7 +1946,7 @@
         <v>70</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F31" t="s">
         <v>6</v>
@@ -1957,7 +1957,7 @@
         <v>73</v>
       </c>
       <c r="B32" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C32" t="s">
         <v>7</v>
@@ -1966,7 +1966,7 @@
         <v>72</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F32" t="s">
         <v>6</v>
@@ -1977,7 +1977,7 @@
         <v>74</v>
       </c>
       <c r="B33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C33" t="s">
         <v>7</v>
@@ -1986,7 +1986,7 @@
         <v>75</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F33" t="s">
         <v>6</v>
@@ -1997,7 +1997,7 @@
         <v>76</v>
       </c>
       <c r="B34" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C34" t="s">
         <v>7</v>
@@ -2006,7 +2006,7 @@
         <v>77</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F34" t="s">
         <v>6</v>
@@ -2017,7 +2017,7 @@
         <v>78</v>
       </c>
       <c r="B35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C35" t="s">
         <v>7</v>
@@ -2026,7 +2026,7 @@
         <v>79</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F35" t="s">
         <v>6</v>
@@ -2037,7 +2037,7 @@
         <v>80</v>
       </c>
       <c r="B36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C36" t="s">
         <v>7</v>
@@ -2046,7 +2046,7 @@
         <v>81</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F36" t="s">
         <v>6</v>
@@ -2057,7 +2057,7 @@
         <v>82</v>
       </c>
       <c r="B37" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C37" t="s">
         <v>7</v>
@@ -2066,7 +2066,7 @@
         <v>83</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F37" t="s">
         <v>6</v>
@@ -2077,7 +2077,7 @@
         <v>86</v>
       </c>
       <c r="B38" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C38" t="s">
         <v>7</v>
@@ -2086,7 +2086,7 @@
         <v>85</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>126</v>
+        <v>300</v>
       </c>
       <c r="F38" t="s">
         <v>6</v>
@@ -2097,7 +2097,7 @@
         <v>88</v>
       </c>
       <c r="B39" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C39" t="s">
         <v>7</v>
@@ -2106,7 +2106,7 @@
         <v>87</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>126</v>
+        <v>300</v>
       </c>
       <c r="F39" t="s">
         <v>6</v>
@@ -2117,7 +2117,7 @@
         <v>89</v>
       </c>
       <c r="B40" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C40" t="s">
         <v>7</v>
@@ -2126,7 +2126,7 @@
         <v>90</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>138</v>
+        <v>300</v>
       </c>
       <c r="F40" t="s">
         <v>6</v>
@@ -2137,7 +2137,7 @@
         <v>92</v>
       </c>
       <c r="B41" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C41" t="s">
         <v>7</v>
@@ -2146,7 +2146,7 @@
         <v>91</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>138</v>
+        <v>300</v>
       </c>
       <c r="F41" t="s">
         <v>6</v>
@@ -2157,7 +2157,7 @@
         <v>93</v>
       </c>
       <c r="B42" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C42" t="s">
         <v>7</v>
@@ -2166,7 +2166,7 @@
         <v>94</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>138</v>
+        <v>300</v>
       </c>
       <c r="F42" t="s">
         <v>6</v>
@@ -2177,7 +2177,7 @@
         <v>95</v>
       </c>
       <c r="B43" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C43" t="s">
         <v>7</v>
@@ -2186,7 +2186,7 @@
         <v>96</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>138</v>
+        <v>300</v>
       </c>
       <c r="F43" t="s">
         <v>6</v>
@@ -2197,7 +2197,7 @@
         <v>84</v>
       </c>
       <c r="B44" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C44" t="s">
         <v>7</v>
@@ -2206,7 +2206,7 @@
         <v>97</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>138</v>
+        <v>300</v>
       </c>
       <c r="F44" t="s">
         <v>6</v>
@@ -2217,7 +2217,7 @@
         <v>98</v>
       </c>
       <c r="B45" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C45" t="s">
         <v>7</v>
@@ -2226,7 +2226,7 @@
         <v>99</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>138</v>
+        <v>300</v>
       </c>
       <c r="F45" t="s">
         <v>6</v>
@@ -2237,7 +2237,7 @@
         <v>101</v>
       </c>
       <c r="B46" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C46" t="s">
         <v>7</v>
@@ -2246,7 +2246,7 @@
         <v>100</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>138</v>
+        <v>300</v>
       </c>
       <c r="F46" t="s">
         <v>6</v>
@@ -2257,16 +2257,16 @@
         <v>102</v>
       </c>
       <c r="B47" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C47" t="s">
         <v>7</v>
       </c>
       <c r="D47" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>138</v>
+        <v>300</v>
       </c>
       <c r="F47" t="s">
         <v>6</v>
@@ -2277,7 +2277,7 @@
         <v>103</v>
       </c>
       <c r="B48" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C48" t="s">
         <v>7</v>
@@ -2286,7 +2286,7 @@
         <v>104</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>138</v>
+        <v>300</v>
       </c>
       <c r="F48" t="s">
         <v>6</v>
@@ -2297,7 +2297,7 @@
         <v>105</v>
       </c>
       <c r="B49" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C49" t="s">
         <v>7</v>
@@ -2306,7 +2306,7 @@
         <v>106</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F49" t="s">
         <v>6</v>
@@ -2317,7 +2317,7 @@
         <v>107</v>
       </c>
       <c r="B50" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C50" t="s">
         <v>7</v>
@@ -2326,7 +2326,7 @@
         <v>108</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F50" t="s">
         <v>6</v>
@@ -2337,7 +2337,7 @@
         <v>109</v>
       </c>
       <c r="B51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C51" t="s">
         <v>7</v>
@@ -2346,7 +2346,7 @@
         <v>110</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F51" t="s">
         <v>6</v>
@@ -2357,7 +2357,7 @@
         <v>111</v>
       </c>
       <c r="B52" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C52" t="s">
         <v>7</v>
@@ -2366,7 +2366,7 @@
         <v>112</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F52" t="s">
         <v>6</v>
@@ -2377,13 +2377,13 @@
         <v>113</v>
       </c>
       <c r="B53" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C53" t="s">
         <v>114</v>
       </c>
       <c r="D53" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E53" t="s">
         <v>115</v>
@@ -2397,7 +2397,7 @@
         <v>116</v>
       </c>
       <c r="B54" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C54" t="s">
         <v>114</v>
@@ -2417,7 +2417,7 @@
         <v>118</v>
       </c>
       <c r="B55" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C55" t="s">
         <v>114</v>
@@ -2437,7 +2437,7 @@
         <v>120</v>
       </c>
       <c r="B56" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C56" t="s">
         <v>7</v>
@@ -2446,7 +2446,7 @@
         <v>121</v>
       </c>
       <c r="E56" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F56" t="s">
         <v>6</v>
@@ -2457,7 +2457,7 @@
         <v>122</v>
       </c>
       <c r="B57" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C57" t="s">
         <v>7</v>
@@ -2466,7 +2466,7 @@
         <v>123</v>
       </c>
       <c r="E57" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F57" t="s">
         <v>6</v>
@@ -2474,19 +2474,19 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>141</v>
+      </c>
+      <c r="B58" t="s">
         <v>142</v>
-      </c>
-      <c r="B58" t="s">
-        <v>143</v>
       </c>
       <c r="C58" t="s">
         <v>114</v>
       </c>
       <c r="D58" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E58" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F58" t="s">
         <v>6</v>
@@ -2494,19 +2494,19 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B59" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C59" t="s">
         <v>114</v>
       </c>
       <c r="D59" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E59" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F59" t="s">
         <v>6</v>
@@ -2514,19 +2514,19 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B60" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C60" t="s">
         <v>114</v>
       </c>
       <c r="D60" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E60" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F60" t="s">
         <v>6</v>
@@ -2534,19 +2534,19 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B61" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C61" t="s">
         <v>114</v>
       </c>
       <c r="D61" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E61" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F61" t="s">
         <v>6</v>
@@ -2554,19 +2554,19 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B62" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C62" t="s">
         <v>114</v>
       </c>
       <c r="D62" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E62" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F62" t="s">
         <v>6</v>
@@ -2574,19 +2574,19 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B63" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C63" t="s">
         <v>114</v>
       </c>
       <c r="D63" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E63" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F63" t="s">
         <v>6</v>
@@ -2594,19 +2594,19 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B64" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C64" t="s">
         <v>114</v>
       </c>
       <c r="D64" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E64" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F64" t="s">
         <v>6</v>
@@ -2614,19 +2614,19 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C65" t="s">
         <v>114</v>
       </c>
       <c r="D65" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E65" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F65" t="s">
         <v>6</v>
@@ -2634,19 +2634,19 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B66" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C66" t="s">
         <v>114</v>
       </c>
       <c r="D66" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E66" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F66" t="s">
         <v>6</v>
@@ -2654,19 +2654,19 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B67" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C67" t="s">
         <v>114</v>
       </c>
       <c r="D67" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E67" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F67" t="s">
         <v>6</v>
@@ -2674,19 +2674,19 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>163</v>
+      </c>
+      <c r="B68" t="s">
         <v>164</v>
-      </c>
-      <c r="B68" t="s">
-        <v>165</v>
       </c>
       <c r="C68" t="s">
         <v>114</v>
       </c>
       <c r="D68" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E68" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F68" t="s">
         <v>6</v>
@@ -2694,19 +2694,19 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B69" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C69" t="s">
         <v>114</v>
       </c>
       <c r="D69" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E69" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F69" t="s">
         <v>6</v>
@@ -2714,59 +2714,59 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>169</v>
+      </c>
+      <c r="B70" t="s">
         <v>170</v>
-      </c>
-      <c r="B70" t="s">
-        <v>171</v>
       </c>
       <c r="C70" t="s">
         <v>114</v>
       </c>
       <c r="D70" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E70" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F70" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B71" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C71" t="s">
         <v>114</v>
       </c>
       <c r="D71" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E71" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F71" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B72" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C72" t="s">
         <v>114</v>
       </c>
       <c r="D72" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E72" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F72" t="s">
         <v>6</v>
@@ -2774,19 +2774,19 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>176</v>
+      </c>
+      <c r="B73" t="s">
         <v>177</v>
-      </c>
-      <c r="B73" t="s">
-        <v>178</v>
       </c>
       <c r="C73" t="s">
         <v>114</v>
       </c>
       <c r="D73" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E73" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F73" t="s">
         <v>6</v>
@@ -2794,19 +2794,19 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B74" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C74" t="s">
         <v>114</v>
       </c>
       <c r="D74" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E74" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F74" t="s">
         <v>6</v>
@@ -2814,19 +2814,19 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B75" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C75" t="s">
         <v>114</v>
       </c>
       <c r="D75" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E75" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F75" t="s">
         <v>6</v>
@@ -2834,19 +2834,19 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B76" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C76" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D76" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E76" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F76" t="s">
         <v>6</v>
@@ -2854,19 +2854,19 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B77" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C77" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D77" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E77" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F77" t="s">
         <v>6</v>
@@ -2874,19 +2874,19 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B78" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C78" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D78" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E78" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F78" t="s">
         <v>6</v>
@@ -2894,19 +2894,19 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>193</v>
+      </c>
+      <c r="B79" t="s">
+        <v>127</v>
+      </c>
+      <c r="C79" t="s">
         <v>194</v>
       </c>
-      <c r="B79" t="s">
-        <v>128</v>
-      </c>
-      <c r="C79" t="s">
-        <v>195</v>
-      </c>
       <c r="D79" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E79" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F79" t="s">
         <v>6</v>
@@ -2914,19 +2914,19 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>195</v>
+      </c>
+      <c r="B80" t="s">
         <v>196</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C80" t="s">
+        <v>194</v>
+      </c>
+      <c r="D80" t="s">
         <v>197</v>
       </c>
-      <c r="C80" t="s">
-        <v>195</v>
-      </c>
-      <c r="D80" t="s">
-        <v>198</v>
-      </c>
       <c r="E80" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F80" t="s">
         <v>6</v>
@@ -2934,19 +2934,19 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B81" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C81" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D81" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E81" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F81" t="s">
         <v>6</v>
@@ -2954,19 +2954,19 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>200</v>
+      </c>
+      <c r="B82" t="s">
+        <v>196</v>
+      </c>
+      <c r="C82" t="s">
+        <v>194</v>
+      </c>
+      <c r="D82" t="s">
         <v>201</v>
       </c>
-      <c r="B82" t="s">
-        <v>197</v>
-      </c>
-      <c r="C82" t="s">
-        <v>195</v>
-      </c>
-      <c r="D82" t="s">
-        <v>202</v>
-      </c>
       <c r="E82" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F82" t="s">
         <v>6</v>
@@ -2974,19 +2974,19 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>202</v>
+      </c>
+      <c r="B83" t="s">
+        <v>196</v>
+      </c>
+      <c r="C83" t="s">
+        <v>194</v>
+      </c>
+      <c r="D83" t="s">
         <v>203</v>
       </c>
-      <c r="B83" t="s">
-        <v>197</v>
-      </c>
-      <c r="C83" t="s">
-        <v>195</v>
-      </c>
-      <c r="D83" t="s">
-        <v>204</v>
-      </c>
       <c r="E83" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F83" t="s">
         <v>6</v>
@@ -2994,19 +2994,19 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B84" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C84" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D84" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E84" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F84" t="s">
         <v>6</v>
@@ -3014,19 +3014,19 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B85" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C85" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D85" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E85" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F85" t="s">
         <v>6</v>
@@ -3034,19 +3034,19 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B86" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C86" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D86" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E86" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F86" t="s">
         <v>6</v>
@@ -3054,19 +3054,19 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>212</v>
+      </c>
+      <c r="B87" t="s">
+        <v>196</v>
+      </c>
+      <c r="C87" t="s">
+        <v>194</v>
+      </c>
+      <c r="D87" t="s">
+        <v>208</v>
+      </c>
+      <c r="E87" t="s">
         <v>213</v>
-      </c>
-      <c r="B87" t="s">
-        <v>197</v>
-      </c>
-      <c r="C87" t="s">
-        <v>195</v>
-      </c>
-      <c r="D87" t="s">
-        <v>209</v>
-      </c>
-      <c r="E87" t="s">
-        <v>214</v>
       </c>
       <c r="F87" t="s">
         <v>6</v>
@@ -3074,19 +3074,19 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B88" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C88" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D88" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E88" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F88" t="s">
         <v>6</v>
@@ -3094,19 +3094,19 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>214</v>
+      </c>
+      <c r="B89" t="s">
         <v>215</v>
       </c>
-      <c r="B89" t="s">
+      <c r="C89" t="s">
         <v>216</v>
       </c>
-      <c r="C89" t="s">
+      <c r="D89" t="s">
         <v>217</v>
       </c>
-      <c r="D89" t="s">
+      <c r="E89" t="s">
         <v>218</v>
-      </c>
-      <c r="E89" t="s">
-        <v>219</v>
       </c>
       <c r="F89" t="s">
         <v>6</v>
@@ -3114,19 +3114,19 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B90" t="s">
+        <v>215</v>
+      </c>
+      <c r="C90" t="s">
         <v>216</v>
       </c>
-      <c r="C90" t="s">
-        <v>217</v>
-      </c>
       <c r="D90" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E90" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F90" t="s">
         <v>6</v>
@@ -3134,19 +3134,19 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B91" t="s">
+        <v>215</v>
+      </c>
+      <c r="C91" t="s">
         <v>216</v>
       </c>
-      <c r="C91" t="s">
-        <v>217</v>
-      </c>
       <c r="D91" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E91" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F91" t="s">
         <v>6</v>
@@ -3154,19 +3154,19 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B92" t="s">
+        <v>215</v>
+      </c>
+      <c r="C92" t="s">
         <v>216</v>
       </c>
-      <c r="C92" t="s">
-        <v>217</v>
-      </c>
       <c r="D92" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E92" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F92" t="s">
         <v>6</v>
@@ -3174,19 +3174,19 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B93" t="s">
+        <v>215</v>
+      </c>
+      <c r="C93" t="s">
         <v>216</v>
       </c>
-      <c r="C93" t="s">
-        <v>217</v>
-      </c>
       <c r="D93" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E93" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F93" t="s">
         <v>6</v>
@@ -3194,19 +3194,19 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B94" t="s">
+        <v>215</v>
+      </c>
+      <c r="C94" t="s">
         <v>216</v>
       </c>
-      <c r="C94" t="s">
-        <v>217</v>
-      </c>
       <c r="D94" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E94" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F94" t="s">
         <v>6</v>
@@ -3214,19 +3214,19 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B95" t="s">
+        <v>215</v>
+      </c>
+      <c r="C95" t="s">
         <v>216</v>
       </c>
-      <c r="C95" t="s">
-        <v>217</v>
-      </c>
       <c r="D95" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E95" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F95" t="s">
         <v>6</v>
@@ -3234,19 +3234,19 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B96" t="s">
+        <v>215</v>
+      </c>
+      <c r="C96" t="s">
         <v>216</v>
       </c>
-      <c r="C96" t="s">
-        <v>217</v>
-      </c>
       <c r="D96" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E96" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F96" t="s">
         <v>6</v>
@@ -3254,19 +3254,19 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B97" t="s">
+        <v>215</v>
+      </c>
+      <c r="C97" t="s">
         <v>216</v>
       </c>
-      <c r="C97" t="s">
-        <v>217</v>
-      </c>
       <c r="D97" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E97" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F97" t="s">
         <v>6</v>
@@ -3274,19 +3274,19 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
+        <v>235</v>
+      </c>
+      <c r="B98" t="s">
+        <v>127</v>
+      </c>
+      <c r="C98" t="s">
+        <v>216</v>
+      </c>
+      <c r="D98" t="s">
         <v>236</v>
       </c>
-      <c r="B98" t="s">
-        <v>128</v>
-      </c>
-      <c r="C98" t="s">
-        <v>217</v>
-      </c>
-      <c r="D98" t="s">
-        <v>237</v>
-      </c>
       <c r="E98" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F98" t="s">
         <v>6</v>
@@ -3294,19 +3294,19 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B99" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C99" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D99" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E99" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F99" t="s">
         <v>6</v>
@@ -3314,19 +3314,19 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B100" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C100" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D100" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E100" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F100" t="s">
         <v>6</v>
@@ -3334,19 +3334,19 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
+        <v>239</v>
+      </c>
+      <c r="B101" t="s">
         <v>240</v>
       </c>
-      <c r="B101" t="s">
+      <c r="C101" t="s">
+        <v>194</v>
+      </c>
+      <c r="D101" t="s">
         <v>241</v>
       </c>
-      <c r="C101" t="s">
-        <v>195</v>
-      </c>
-      <c r="D101" t="s">
-        <v>242</v>
-      </c>
       <c r="E101" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F101" t="s">
         <v>6</v>
@@ -3354,19 +3354,19 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B102" t="s">
+        <v>242</v>
+      </c>
+      <c r="C102" t="s">
+        <v>194</v>
+      </c>
+      <c r="D102" t="s">
         <v>243</v>
       </c>
-      <c r="C102" t="s">
-        <v>195</v>
-      </c>
-      <c r="D102" t="s">
-        <v>244</v>
-      </c>
       <c r="E102" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F102" t="s">
         <v>6</v>
@@ -3374,19 +3374,19 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B103" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C103" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D103" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E103" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F103" t="s">
         <v>6</v>
@@ -3394,19 +3394,19 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B104" t="s">
+        <v>250</v>
+      </c>
+      <c r="C104" t="s">
+        <v>194</v>
+      </c>
+      <c r="D104" t="s">
         <v>251</v>
       </c>
-      <c r="C104" t="s">
-        <v>195</v>
-      </c>
-      <c r="D104" t="s">
-        <v>252</v>
-      </c>
       <c r="E104" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F104" t="s">
         <v>6</v>
@@ -3414,19 +3414,19 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
+        <v>249</v>
+      </c>
+      <c r="B105" t="s">
         <v>250</v>
       </c>
-      <c r="B105" t="s">
-        <v>251</v>
-      </c>
       <c r="C105" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D105" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E105" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F105" t="s">
         <v>6</v>
@@ -3434,19 +3434,19 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B106" t="s">
+        <v>253</v>
+      </c>
+      <c r="C106" t="s">
         <v>254</v>
       </c>
-      <c r="C106" t="s">
+      <c r="D106" t="s">
         <v>255</v>
       </c>
-      <c r="D106" t="s">
-        <v>256</v>
-      </c>
       <c r="E106" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F106" t="s">
         <v>6</v>
@@ -3454,19 +3454,19 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B107" t="s">
+        <v>253</v>
+      </c>
+      <c r="C107" t="s">
         <v>254</v>
       </c>
-      <c r="C107" t="s">
-        <v>255</v>
-      </c>
       <c r="D107" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E107" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F107" t="s">
         <v>6</v>
@@ -3474,19 +3474,19 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B108" t="s">
+        <v>253</v>
+      </c>
+      <c r="C108" t="s">
         <v>254</v>
       </c>
-      <c r="C108" t="s">
-        <v>255</v>
-      </c>
       <c r="D108" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E108" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F108" t="s">
         <v>6</v>
@@ -3494,19 +3494,19 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
+        <v>262</v>
+      </c>
+      <c r="B109" t="s">
+        <v>253</v>
+      </c>
+      <c r="C109" t="s">
+        <v>254</v>
+      </c>
+      <c r="D109" t="s">
+        <v>261</v>
+      </c>
+      <c r="E109" t="s">
         <v>263</v>
-      </c>
-      <c r="B109" t="s">
-        <v>254</v>
-      </c>
-      <c r="C109" t="s">
-        <v>255</v>
-      </c>
-      <c r="D109" t="s">
-        <v>262</v>
-      </c>
-      <c r="E109" t="s">
-        <v>264</v>
       </c>
       <c r="F109" t="s">
         <v>6</v>
@@ -3514,19 +3514,19 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
+        <v>264</v>
+      </c>
+      <c r="B110" t="s">
+        <v>127</v>
+      </c>
+      <c r="C110" t="s">
+        <v>254</v>
+      </c>
+      <c r="D110" t="s">
         <v>265</v>
       </c>
-      <c r="B110" t="s">
-        <v>128</v>
-      </c>
-      <c r="C110" t="s">
-        <v>255</v>
-      </c>
-      <c r="D110" t="s">
-        <v>266</v>
-      </c>
       <c r="E110" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F110" t="s">
         <v>6</v>
@@ -3534,19 +3534,19 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
+        <v>266</v>
+      </c>
+      <c r="B111" t="s">
+        <v>127</v>
+      </c>
+      <c r="C111" t="s">
+        <v>254</v>
+      </c>
+      <c r="D111" t="s">
         <v>267</v>
       </c>
-      <c r="B111" t="s">
-        <v>128</v>
-      </c>
-      <c r="C111" t="s">
-        <v>255</v>
-      </c>
-      <c r="D111" t="s">
-        <v>268</v>
-      </c>
       <c r="E111" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F111" t="s">
         <v>6</v>
@@ -3554,19 +3554,19 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
+        <v>268</v>
+      </c>
+      <c r="B112" t="s">
+        <v>127</v>
+      </c>
+      <c r="C112" t="s">
+        <v>254</v>
+      </c>
+      <c r="D112" t="s">
         <v>269</v>
       </c>
-      <c r="B112" t="s">
-        <v>128</v>
-      </c>
-      <c r="C112" t="s">
-        <v>255</v>
-      </c>
-      <c r="D112" t="s">
-        <v>270</v>
-      </c>
       <c r="E112" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F112" t="s">
         <v>6</v>
@@ -3574,19 +3574,19 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B113" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C113" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D113" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E113" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F113" t="s">
         <v>6</v>
@@ -3594,19 +3594,19 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
+        <v>271</v>
+      </c>
+      <c r="B114" t="s">
+        <v>127</v>
+      </c>
+      <c r="C114" t="s">
+        <v>254</v>
+      </c>
+      <c r="D114" t="s">
         <v>272</v>
       </c>
-      <c r="B114" t="s">
-        <v>128</v>
-      </c>
-      <c r="C114" t="s">
-        <v>255</v>
-      </c>
-      <c r="D114" t="s">
-        <v>273</v>
-      </c>
       <c r="E114" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F114" t="s">
         <v>6</v>
@@ -3614,19 +3614,19 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B115" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C115" t="s">
         <v>28</v>
       </c>
       <c r="D115" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E115" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F115" t="s">
         <v>6</v>
@@ -3634,19 +3634,19 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B116" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C116" t="s">
         <v>28</v>
       </c>
       <c r="D116" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E116" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F116" t="s">
         <v>6</v>
@@ -3654,19 +3654,19 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B117" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C117" t="s">
         <v>28</v>
       </c>
       <c r="D117" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E117" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F117" t="s">
         <v>6</v>
@@ -3674,19 +3674,19 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B118" t="s">
+        <v>283</v>
+      </c>
+      <c r="C118" t="s">
+        <v>299</v>
+      </c>
+      <c r="D118" t="s">
         <v>284</v>
       </c>
-      <c r="C118" t="s">
-        <v>300</v>
-      </c>
-      <c r="D118" t="s">
-        <v>285</v>
-      </c>
       <c r="E118" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F118" t="s">
         <v>6</v>
@@ -3694,19 +3694,19 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B119" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C119" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D119" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E119" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F119" t="s">
         <v>6</v>
@@ -3714,19 +3714,19 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
+        <v>287</v>
+      </c>
+      <c r="B120" t="s">
+        <v>283</v>
+      </c>
+      <c r="C120" t="s">
+        <v>299</v>
+      </c>
+      <c r="D120" t="s">
         <v>288</v>
       </c>
-      <c r="B120" t="s">
-        <v>284</v>
-      </c>
-      <c r="C120" t="s">
-        <v>300</v>
-      </c>
-      <c r="D120" t="s">
-        <v>289</v>
-      </c>
       <c r="E120" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F120" t="s">
         <v>6</v>
@@ -3734,19 +3734,19 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B121" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C121" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D121" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E121" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F121" t="s">
         <v>6</v>
@@ -3754,19 +3754,19 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B122" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C122" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D122" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E122" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F122" t="s">
         <v>6</v>
@@ -3774,19 +3774,19 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
+        <v>293</v>
+      </c>
+      <c r="B123" t="s">
+        <v>283</v>
+      </c>
+      <c r="C123" t="s">
+        <v>299</v>
+      </c>
+      <c r="D123" t="s">
         <v>294</v>
       </c>
-      <c r="B123" t="s">
-        <v>284</v>
-      </c>
-      <c r="C123" t="s">
-        <v>300</v>
-      </c>
-      <c r="D123" t="s">
-        <v>295</v>
-      </c>
       <c r="E123" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F123" t="s">
         <v>6</v>
@@ -3794,19 +3794,19 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
+        <v>295</v>
+      </c>
+      <c r="B124" t="s">
+        <v>283</v>
+      </c>
+      <c r="C124" t="s">
+        <v>299</v>
+      </c>
+      <c r="D124" t="s">
         <v>296</v>
       </c>
-      <c r="B124" t="s">
-        <v>284</v>
-      </c>
-      <c r="C124" t="s">
-        <v>300</v>
-      </c>
-      <c r="D124" t="s">
+      <c r="E124" t="s">
         <v>297</v>
-      </c>
-      <c r="E124" t="s">
-        <v>298</v>
       </c>
       <c r="F124" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Katalog guncellendi - 16.01.2026  8:03:24,23
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/CEREN-PC/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="165" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CD4944B-66C6-483A-9F4F-A4645C9C3C0A}"/>
+  <xr:revisionPtr revIDLastSave="193" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69924C6F-ED12-49FF-8430-69450AEF3F4F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="302">
   <si>
     <t>urun_adi</t>
   </si>
@@ -409,12 +409,6 @@
     <t>260 TL</t>
   </si>
   <si>
-    <t>360 TL</t>
-  </si>
-  <si>
-    <t>450 TL</t>
-  </si>
-  <si>
     <t>DOUGLAS.png</t>
   </si>
   <si>
@@ -923,6 +917,15 @@
   </si>
   <si>
     <t>%98 pamuk ve %2 spandex. 30-31-32-33-34-36-38-40 Beden seçeneği mevcuttur.Belirtilen fiyatlar adet fiyatıdır.</t>
+  </si>
+  <si>
+    <t>425 TL</t>
+  </si>
+  <si>
+    <t>500TL</t>
+  </si>
+  <si>
+    <t>yok</t>
   </si>
 </sst>
 </file>
@@ -1321,8 +1324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38:E48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1409,7 +1412,7 @@
         <v>124</v>
       </c>
       <c r="F4" t="s">
-        <v>6</v>
+        <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1546,7 +1549,7 @@
         <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F11" t="s">
         <v>6</v>
@@ -1566,10 +1569,10 @@
         <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F12" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1586,7 +1589,7 @@
         <v>35</v>
       </c>
       <c r="E13" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F13" t="s">
         <v>6</v>
@@ -1606,7 +1609,7 @@
         <v>37</v>
       </c>
       <c r="E14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F14" t="s">
         <v>6</v>
@@ -1626,7 +1629,7 @@
         <v>39</v>
       </c>
       <c r="E15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F15" t="s">
         <v>6</v>
@@ -1646,7 +1649,7 @@
         <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F16" t="s">
         <v>6</v>
@@ -1666,7 +1669,7 @@
         <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F17" t="s">
         <v>6</v>
@@ -1686,7 +1689,7 @@
         <v>45</v>
       </c>
       <c r="E18" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F18" t="s">
         <v>6</v>
@@ -1706,7 +1709,7 @@
         <v>47</v>
       </c>
       <c r="E19" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F19" t="s">
         <v>6</v>
@@ -1726,7 +1729,7 @@
         <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F20" t="s">
         <v>6</v>
@@ -1746,7 +1749,7 @@
         <v>51</v>
       </c>
       <c r="E21" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F21" t="s">
         <v>6</v>
@@ -1766,7 +1769,7 @@
         <v>52</v>
       </c>
       <c r="E22" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F22" t="s">
         <v>6</v>
@@ -1786,7 +1789,7 @@
         <v>54</v>
       </c>
       <c r="E23" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F23" t="s">
         <v>6</v>
@@ -1806,7 +1809,7 @@
         <v>57</v>
       </c>
       <c r="E24" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F24" t="s">
         <v>6</v>
@@ -1826,7 +1829,7 @@
         <v>59</v>
       </c>
       <c r="E25" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F25" t="s">
         <v>6</v>
@@ -1846,7 +1849,7 @@
         <v>60</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F26" t="s">
         <v>6</v>
@@ -1866,7 +1869,7 @@
         <v>63</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F27" t="s">
         <v>6</v>
@@ -1886,7 +1889,7 @@
         <v>65</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F28" t="s">
         <v>6</v>
@@ -1906,7 +1909,7 @@
         <v>67</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F29" t="s">
         <v>6</v>
@@ -1926,7 +1929,7 @@
         <v>68</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F30" t="s">
         <v>6</v>
@@ -1937,7 +1940,7 @@
         <v>71</v>
       </c>
       <c r="B31" t="s">
-        <v>129</v>
+        <v>299</v>
       </c>
       <c r="C31" t="s">
         <v>7</v>
@@ -1946,7 +1949,7 @@
         <v>70</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F31" t="s">
         <v>6</v>
@@ -1957,7 +1960,7 @@
         <v>73</v>
       </c>
       <c r="B32" t="s">
-        <v>129</v>
+        <v>299</v>
       </c>
       <c r="C32" t="s">
         <v>7</v>
@@ -1966,7 +1969,7 @@
         <v>72</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F32" t="s">
         <v>6</v>
@@ -1977,7 +1980,7 @@
         <v>74</v>
       </c>
       <c r="B33" t="s">
-        <v>129</v>
+        <v>299</v>
       </c>
       <c r="C33" t="s">
         <v>7</v>
@@ -1986,7 +1989,7 @@
         <v>75</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F33" t="s">
         <v>6</v>
@@ -1997,7 +2000,7 @@
         <v>76</v>
       </c>
       <c r="B34" t="s">
-        <v>129</v>
+        <v>299</v>
       </c>
       <c r="C34" t="s">
         <v>7</v>
@@ -2006,7 +2009,7 @@
         <v>77</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F34" t="s">
         <v>6</v>
@@ -2017,7 +2020,7 @@
         <v>78</v>
       </c>
       <c r="B35" t="s">
-        <v>129</v>
+        <v>299</v>
       </c>
       <c r="C35" t="s">
         <v>7</v>
@@ -2026,7 +2029,7 @@
         <v>79</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F35" t="s">
         <v>6</v>
@@ -2037,7 +2040,7 @@
         <v>80</v>
       </c>
       <c r="B36" t="s">
-        <v>129</v>
+        <v>299</v>
       </c>
       <c r="C36" t="s">
         <v>7</v>
@@ -2046,7 +2049,7 @@
         <v>81</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F36" t="s">
         <v>6</v>
@@ -2057,7 +2060,7 @@
         <v>82</v>
       </c>
       <c r="B37" t="s">
-        <v>129</v>
+        <v>299</v>
       </c>
       <c r="C37" t="s">
         <v>7</v>
@@ -2066,7 +2069,7 @@
         <v>83</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F37" t="s">
         <v>6</v>
@@ -2086,7 +2089,7 @@
         <v>85</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F38" t="s">
         <v>6</v>
@@ -2106,7 +2109,7 @@
         <v>87</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F39" t="s">
         <v>6</v>
@@ -2117,7 +2120,7 @@
         <v>89</v>
       </c>
       <c r="B40" t="s">
-        <v>130</v>
+        <v>300</v>
       </c>
       <c r="C40" t="s">
         <v>7</v>
@@ -2126,7 +2129,7 @@
         <v>90</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F40" t="s">
         <v>6</v>
@@ -2137,7 +2140,7 @@
         <v>92</v>
       </c>
       <c r="B41" t="s">
-        <v>130</v>
+        <v>300</v>
       </c>
       <c r="C41" t="s">
         <v>7</v>
@@ -2146,7 +2149,7 @@
         <v>91</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F41" t="s">
         <v>6</v>
@@ -2157,7 +2160,7 @@
         <v>93</v>
       </c>
       <c r="B42" t="s">
-        <v>130</v>
+        <v>300</v>
       </c>
       <c r="C42" t="s">
         <v>7</v>
@@ -2166,7 +2169,7 @@
         <v>94</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F42" t="s">
         <v>6</v>
@@ -2177,7 +2180,7 @@
         <v>95</v>
       </c>
       <c r="B43" t="s">
-        <v>130</v>
+        <v>300</v>
       </c>
       <c r="C43" t="s">
         <v>7</v>
@@ -2186,7 +2189,7 @@
         <v>96</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F43" t="s">
         <v>6</v>
@@ -2197,7 +2200,7 @@
         <v>84</v>
       </c>
       <c r="B44" t="s">
-        <v>130</v>
+        <v>300</v>
       </c>
       <c r="C44" t="s">
         <v>7</v>
@@ -2206,7 +2209,7 @@
         <v>97</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F44" t="s">
         <v>6</v>
@@ -2217,7 +2220,7 @@
         <v>98</v>
       </c>
       <c r="B45" t="s">
-        <v>130</v>
+        <v>300</v>
       </c>
       <c r="C45" t="s">
         <v>7</v>
@@ -2226,7 +2229,7 @@
         <v>99</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F45" t="s">
         <v>6</v>
@@ -2237,7 +2240,7 @@
         <v>101</v>
       </c>
       <c r="B46" t="s">
-        <v>130</v>
+        <v>300</v>
       </c>
       <c r="C46" t="s">
         <v>7</v>
@@ -2246,7 +2249,7 @@
         <v>100</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F46" t="s">
         <v>6</v>
@@ -2257,16 +2260,16 @@
         <v>102</v>
       </c>
       <c r="B47" t="s">
-        <v>130</v>
+        <v>300</v>
       </c>
       <c r="C47" t="s">
         <v>7</v>
       </c>
       <c r="D47" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F47" t="s">
         <v>6</v>
@@ -2277,7 +2280,7 @@
         <v>103</v>
       </c>
       <c r="B48" t="s">
-        <v>130</v>
+        <v>300</v>
       </c>
       <c r="C48" t="s">
         <v>7</v>
@@ -2286,7 +2289,7 @@
         <v>104</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F48" t="s">
         <v>6</v>
@@ -2306,7 +2309,7 @@
         <v>106</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F49" t="s">
         <v>6</v>
@@ -2326,7 +2329,7 @@
         <v>108</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F50" t="s">
         <v>6</v>
@@ -2346,7 +2349,7 @@
         <v>110</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F51" t="s">
         <v>6</v>
@@ -2366,7 +2369,7 @@
         <v>112</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F52" t="s">
         <v>6</v>
@@ -2377,13 +2380,13 @@
         <v>113</v>
       </c>
       <c r="B53" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C53" t="s">
         <v>114</v>
       </c>
       <c r="D53" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E53" t="s">
         <v>115</v>
@@ -2397,7 +2400,7 @@
         <v>116</v>
       </c>
       <c r="B54" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C54" t="s">
         <v>114</v>
@@ -2417,7 +2420,7 @@
         <v>118</v>
       </c>
       <c r="B55" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C55" t="s">
         <v>114</v>
@@ -2437,7 +2440,7 @@
         <v>120</v>
       </c>
       <c r="B56" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C56" t="s">
         <v>7</v>
@@ -2446,7 +2449,7 @@
         <v>121</v>
       </c>
       <c r="E56" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F56" t="s">
         <v>6</v>
@@ -2457,7 +2460,7 @@
         <v>122</v>
       </c>
       <c r="B57" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C57" t="s">
         <v>7</v>
@@ -2466,7 +2469,7 @@
         <v>123</v>
       </c>
       <c r="E57" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F57" t="s">
         <v>6</v>
@@ -2474,219 +2477,219 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B58" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C58" t="s">
         <v>114</v>
       </c>
       <c r="D58" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E58" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F58" t="s">
-        <v>6</v>
+        <v>280</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B59" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C59" t="s">
         <v>114</v>
       </c>
       <c r="D59" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E59" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F59" t="s">
-        <v>6</v>
+        <v>280</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B60" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C60" t="s">
         <v>114</v>
       </c>
       <c r="D60" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E60" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F60" t="s">
-        <v>6</v>
+        <v>280</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B61" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C61" t="s">
         <v>114</v>
       </c>
       <c r="D61" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E61" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F61" t="s">
-        <v>6</v>
+        <v>280</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B62" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C62" t="s">
         <v>114</v>
       </c>
       <c r="D62" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E62" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F62" t="s">
-        <v>6</v>
+        <v>280</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B63" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C63" t="s">
         <v>114</v>
       </c>
       <c r="D63" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E63" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F63" t="s">
-        <v>6</v>
+        <v>280</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>153</v>
+      </c>
+      <c r="B64" t="s">
         <v>155</v>
-      </c>
-      <c r="B64" t="s">
-        <v>157</v>
       </c>
       <c r="C64" t="s">
         <v>114</v>
       </c>
       <c r="D64" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E64" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F64" t="s">
-        <v>6</v>
+        <v>280</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C65" t="s">
         <v>114</v>
       </c>
       <c r="D65" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E65" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F65" t="s">
-        <v>6</v>
+        <v>280</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B66" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C66" t="s">
         <v>114</v>
       </c>
       <c r="D66" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E66" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F66" t="s">
-        <v>6</v>
+        <v>280</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B67" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C67" t="s">
         <v>114</v>
       </c>
       <c r="D67" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E67" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F67" t="s">
-        <v>6</v>
+        <v>280</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B68" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C68" t="s">
         <v>114</v>
       </c>
       <c r="D68" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E68" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F68" t="s">
         <v>6</v>
@@ -2694,119 +2697,119 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>166</v>
+      </c>
+      <c r="B69" t="s">
         <v>168</v>
-      </c>
-      <c r="B69" t="s">
-        <v>170</v>
       </c>
       <c r="C69" t="s">
         <v>114</v>
       </c>
       <c r="D69" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E69" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F69" t="s">
-        <v>6</v>
+        <v>280</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B70" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C70" t="s">
         <v>114</v>
       </c>
       <c r="D70" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E70" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F70" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B71" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C71" t="s">
         <v>114</v>
       </c>
       <c r="D71" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E71" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F71" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B72" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C72" t="s">
         <v>114</v>
       </c>
       <c r="D72" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E72" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F72" t="s">
-        <v>6</v>
+        <v>280</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B73" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C73" t="s">
         <v>114</v>
       </c>
       <c r="D73" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E73" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F73" t="s">
-        <v>6</v>
+        <v>280</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B74" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C74" t="s">
         <v>114</v>
       </c>
       <c r="D74" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E74" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F74" t="s">
         <v>6</v>
@@ -2814,19 +2817,19 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B75" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C75" t="s">
         <v>114</v>
       </c>
       <c r="D75" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E75" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F75" t="s">
         <v>6</v>
@@ -2834,19 +2837,19 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B76" t="s">
         <v>127</v>
       </c>
       <c r="C76" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D76" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E76" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F76" t="s">
         <v>6</v>
@@ -2854,19 +2857,19 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B77" t="s">
         <v>127</v>
       </c>
       <c r="C77" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D77" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E77" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F77" t="s">
         <v>6</v>
@@ -2874,19 +2877,19 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B78" t="s">
         <v>127</v>
       </c>
       <c r="C78" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D78" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E78" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F78" t="s">
         <v>6</v>
@@ -2894,19 +2897,19 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B79" t="s">
         <v>127</v>
       </c>
       <c r="C79" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D79" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E79" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F79" t="s">
         <v>6</v>
@@ -2914,19 +2917,19 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>193</v>
+      </c>
+      <c r="B80" t="s">
+        <v>194</v>
+      </c>
+      <c r="C80" t="s">
+        <v>192</v>
+      </c>
+      <c r="D80" t="s">
         <v>195</v>
       </c>
-      <c r="B80" t="s">
-        <v>196</v>
-      </c>
-      <c r="C80" t="s">
-        <v>194</v>
-      </c>
-      <c r="D80" t="s">
-        <v>197</v>
-      </c>
       <c r="E80" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F80" t="s">
         <v>6</v>
@@ -2934,19 +2937,19 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B81" t="s">
+        <v>194</v>
+      </c>
+      <c r="C81" t="s">
+        <v>192</v>
+      </c>
+      <c r="D81" t="s">
         <v>196</v>
       </c>
-      <c r="C81" t="s">
-        <v>194</v>
-      </c>
-      <c r="D81" t="s">
-        <v>198</v>
-      </c>
       <c r="E81" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F81" t="s">
         <v>6</v>
@@ -2954,19 +2957,19 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B82" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C82" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D82" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E82" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F82" t="s">
         <v>6</v>
@@ -2974,19 +2977,19 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B83" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C83" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D83" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E83" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F83" t="s">
         <v>6</v>
@@ -2994,19 +2997,19 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B84" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C84" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D84" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E84" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F84" t="s">
         <v>6</v>
@@ -3014,19 +3017,19 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B85" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C85" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D85" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E85" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F85" t="s">
         <v>6</v>
@@ -3034,19 +3037,19 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
+        <v>209</v>
+      </c>
+      <c r="B86" t="s">
+        <v>194</v>
+      </c>
+      <c r="C86" t="s">
+        <v>192</v>
+      </c>
+      <c r="D86" t="s">
+        <v>205</v>
+      </c>
+      <c r="E86" t="s">
         <v>211</v>
-      </c>
-      <c r="B86" t="s">
-        <v>196</v>
-      </c>
-      <c r="C86" t="s">
-        <v>194</v>
-      </c>
-      <c r="D86" t="s">
-        <v>207</v>
-      </c>
-      <c r="E86" t="s">
-        <v>213</v>
       </c>
       <c r="F86" t="s">
         <v>6</v>
@@ -3054,19 +3057,19 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B87" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C87" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D87" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E87" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F87" t="s">
         <v>6</v>
@@ -3074,19 +3077,19 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B88" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C88" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D88" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E88" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F88" t="s">
         <v>6</v>
@@ -3094,19 +3097,19 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>212</v>
+      </c>
+      <c r="B89" t="s">
+        <v>213</v>
+      </c>
+      <c r="C89" t="s">
         <v>214</v>
       </c>
-      <c r="B89" t="s">
+      <c r="D89" t="s">
         <v>215</v>
       </c>
-      <c r="C89" t="s">
+      <c r="E89" t="s">
         <v>216</v>
-      </c>
-      <c r="D89" t="s">
-        <v>217</v>
-      </c>
-      <c r="E89" t="s">
-        <v>218</v>
       </c>
       <c r="F89" t="s">
         <v>6</v>
@@ -3114,19 +3117,19 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B90" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C90" t="s">
+        <v>214</v>
+      </c>
+      <c r="D90" t="s">
+        <v>217</v>
+      </c>
+      <c r="E90" t="s">
         <v>216</v>
-      </c>
-      <c r="D90" t="s">
-        <v>219</v>
-      </c>
-      <c r="E90" t="s">
-        <v>218</v>
       </c>
       <c r="F90" t="s">
         <v>6</v>
@@ -3134,19 +3137,19 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B91" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C91" t="s">
+        <v>214</v>
+      </c>
+      <c r="D91" t="s">
+        <v>219</v>
+      </c>
+      <c r="E91" t="s">
         <v>216</v>
-      </c>
-      <c r="D91" t="s">
-        <v>221</v>
-      </c>
-      <c r="E91" t="s">
-        <v>218</v>
       </c>
       <c r="F91" t="s">
         <v>6</v>
@@ -3154,19 +3157,19 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B92" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C92" t="s">
+        <v>214</v>
+      </c>
+      <c r="D92" t="s">
+        <v>221</v>
+      </c>
+      <c r="E92" t="s">
         <v>216</v>
-      </c>
-      <c r="D92" t="s">
-        <v>223</v>
-      </c>
-      <c r="E92" t="s">
-        <v>218</v>
       </c>
       <c r="F92" t="s">
         <v>6</v>
@@ -3174,19 +3177,19 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B93" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C93" t="s">
+        <v>214</v>
+      </c>
+      <c r="D93" t="s">
+        <v>223</v>
+      </c>
+      <c r="E93" t="s">
         <v>216</v>
-      </c>
-      <c r="D93" t="s">
-        <v>225</v>
-      </c>
-      <c r="E93" t="s">
-        <v>218</v>
       </c>
       <c r="F93" t="s">
         <v>6</v>
@@ -3194,19 +3197,19 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B94" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C94" t="s">
+        <v>214</v>
+      </c>
+      <c r="D94" t="s">
+        <v>225</v>
+      </c>
+      <c r="E94" t="s">
         <v>216</v>
-      </c>
-      <c r="D94" t="s">
-        <v>227</v>
-      </c>
-      <c r="E94" t="s">
-        <v>218</v>
       </c>
       <c r="F94" t="s">
         <v>6</v>
@@ -3214,19 +3217,19 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B95" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C95" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D95" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E95" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F95" t="s">
         <v>6</v>
@@ -3234,19 +3237,19 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B96" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C96" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D96" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E96" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F96" t="s">
         <v>6</v>
@@ -3254,19 +3257,19 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B97" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C97" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D97" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E97" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F97" t="s">
         <v>6</v>
@@ -3274,19 +3277,19 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B98" t="s">
         <v>127</v>
       </c>
       <c r="C98" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D98" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E98" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F98" t="s">
         <v>6</v>
@@ -3294,19 +3297,19 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B99" t="s">
         <v>127</v>
       </c>
       <c r="C99" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D99" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E99" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F99" t="s">
         <v>6</v>
@@ -3314,19 +3317,19 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B100" t="s">
         <v>127</v>
       </c>
       <c r="C100" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D100" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E100" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F100" t="s">
         <v>6</v>
@@ -3334,19 +3337,19 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
+        <v>237</v>
+      </c>
+      <c r="B101" t="s">
+        <v>238</v>
+      </c>
+      <c r="C101" t="s">
+        <v>192</v>
+      </c>
+      <c r="D101" t="s">
         <v>239</v>
       </c>
-      <c r="B101" t="s">
-        <v>240</v>
-      </c>
-      <c r="C101" t="s">
-        <v>194</v>
-      </c>
-      <c r="D101" t="s">
-        <v>241</v>
-      </c>
       <c r="E101" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F101" t="s">
         <v>6</v>
@@ -3354,19 +3357,19 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B102" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C102" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D102" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E102" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F102" t="s">
         <v>6</v>
@@ -3374,19 +3377,19 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B103" t="s">
+        <v>240</v>
+      </c>
+      <c r="C103" t="s">
+        <v>192</v>
+      </c>
+      <c r="D103" t="s">
         <v>242</v>
       </c>
-      <c r="C103" t="s">
-        <v>194</v>
-      </c>
-      <c r="D103" t="s">
-        <v>244</v>
-      </c>
       <c r="E103" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F103" t="s">
         <v>6</v>
@@ -3394,19 +3397,19 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
+        <v>246</v>
+      </c>
+      <c r="B104" t="s">
         <v>248</v>
       </c>
-      <c r="B104" t="s">
-        <v>250</v>
-      </c>
       <c r="C104" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D104" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E104" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F104" t="s">
         <v>6</v>
@@ -3414,19 +3417,19 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B105" t="s">
+        <v>248</v>
+      </c>
+      <c r="C105" t="s">
+        <v>192</v>
+      </c>
+      <c r="D105" t="s">
         <v>250</v>
       </c>
-      <c r="C105" t="s">
-        <v>194</v>
-      </c>
-      <c r="D105" t="s">
-        <v>252</v>
-      </c>
       <c r="E105" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F105" t="s">
         <v>6</v>
@@ -3434,19 +3437,19 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B106" t="s">
+        <v>251</v>
+      </c>
+      <c r="C106" t="s">
+        <v>252</v>
+      </c>
+      <c r="D106" t="s">
         <v>253</v>
       </c>
-      <c r="C106" t="s">
-        <v>254</v>
-      </c>
-      <c r="D106" t="s">
-        <v>255</v>
-      </c>
       <c r="E106" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F106" t="s">
         <v>6</v>
@@ -3454,19 +3457,19 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B107" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C107" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D107" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E107" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F107" t="s">
         <v>6</v>
@@ -3474,19 +3477,19 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B108" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C108" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D108" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E108" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F108" t="s">
         <v>6</v>
@@ -3494,19 +3497,19 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B109" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C109" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D109" t="s">
+        <v>259</v>
+      </c>
+      <c r="E109" t="s">
         <v>261</v>
-      </c>
-      <c r="E109" t="s">
-        <v>263</v>
       </c>
       <c r="F109" t="s">
         <v>6</v>
@@ -3514,19 +3517,19 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B110" t="s">
         <v>127</v>
       </c>
       <c r="C110" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D110" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E110" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F110" t="s">
         <v>6</v>
@@ -3534,19 +3537,19 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B111" t="s">
         <v>127</v>
       </c>
       <c r="C111" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D111" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E111" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F111" t="s">
         <v>6</v>
@@ -3554,19 +3557,19 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B112" t="s">
         <v>127</v>
       </c>
       <c r="C112" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D112" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E112" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F112" t="s">
         <v>6</v>
@@ -3574,19 +3577,19 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B113" t="s">
         <v>127</v>
       </c>
       <c r="C113" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D113" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E113" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F113" t="s">
         <v>6</v>
@@ -3594,19 +3597,19 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B114" t="s">
         <v>127</v>
       </c>
       <c r="C114" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D114" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E114" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F114" t="s">
         <v>6</v>
@@ -3614,19 +3617,19 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B115" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C115" t="s">
         <v>28</v>
       </c>
       <c r="D115" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E115" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F115" t="s">
         <v>6</v>
@@ -3634,19 +3637,19 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B116" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C116" t="s">
         <v>28</v>
       </c>
       <c r="D116" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E116" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F116" t="s">
         <v>6</v>
@@ -3654,19 +3657,19 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B117" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C117" t="s">
         <v>28</v>
       </c>
       <c r="D117" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E117" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F117" t="s">
         <v>6</v>
@@ -3674,19 +3677,19 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B118" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C118" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D118" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E118" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F118" t="s">
         <v>6</v>
@@ -3694,19 +3697,19 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B119" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C119" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D119" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E119" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F119" t="s">
         <v>6</v>
@@ -3714,19 +3717,19 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B120" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C120" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D120" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E120" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F120" t="s">
         <v>6</v>
@@ -3734,19 +3737,19 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B121" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C121" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D121" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E121" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F121" t="s">
         <v>6</v>
@@ -3754,19 +3757,19 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B122" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C122" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D122" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E122" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F122" t="s">
         <v>6</v>
@@ -3774,19 +3777,19 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B123" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C123" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D123" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E123" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F123" t="s">
         <v>6</v>
@@ -3794,19 +3797,19 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
+        <v>293</v>
+      </c>
+      <c r="B124" t="s">
+        <v>281</v>
+      </c>
+      <c r="C124" t="s">
+        <v>297</v>
+      </c>
+      <c r="D124" t="s">
+        <v>294</v>
+      </c>
+      <c r="E124" t="s">
         <v>295</v>
-      </c>
-      <c r="B124" t="s">
-        <v>283</v>
-      </c>
-      <c r="C124" t="s">
-        <v>299</v>
-      </c>
-      <c r="D124" t="s">
-        <v>296</v>
-      </c>
-      <c r="E124" t="s">
-        <v>297</v>
       </c>
       <c r="F124" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Katalog guncellendi - 16.01.2026 11:18:57,51
</commit_message>
<xml_diff>
--- a/urunler.xlsx
+++ b/urunler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49dd5535ee0ab452/Desktop/CEREN-PC/SIVAL_GIYIM_KATALOG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="193" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69924C6F-ED12-49FF-8430-69450AEF3F4F}"/>
+  <xr:revisionPtr revIDLastSave="194" documentId="13_ncr:1_{CCE8B614-DB69-4334-AC06-D714AC841E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B541A64-EA0F-4DCC-A056-87AD91AE2D16}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="321">
   <si>
     <t>urun_adi</t>
   </si>
@@ -926,6 +926,63 @@
   </si>
   <si>
     <t>yok</t>
+  </si>
+  <si>
+    <t>246.jpg</t>
+  </si>
+  <si>
+    <t>STRAİGHT FİT 246</t>
+  </si>
+  <si>
+    <t>450 TL</t>
+  </si>
+  <si>
+    <t>32-33-34-36-38-40 Beden seçeneği mevcuttur.Ürünümüz serili olarak satılmaktadır.Belirtilen fiyatlar adet fiyatıdır.</t>
+  </si>
+  <si>
+    <t>VAR</t>
+  </si>
+  <si>
+    <t>STRAİGHT FİT 246/3</t>
+  </si>
+  <si>
+    <t>246-3.jpg</t>
+  </si>
+  <si>
+    <t>STRAİGHT FİT 246/4</t>
+  </si>
+  <si>
+    <t>246-4.jpg</t>
+  </si>
+  <si>
+    <t>STRAİGHT FİT 243/1</t>
+  </si>
+  <si>
+    <t>243-1.jpg</t>
+  </si>
+  <si>
+    <t>STRAİGHT FİT 246/2</t>
+  </si>
+  <si>
+    <t>246-2.jpg</t>
+  </si>
+  <si>
+    <t>STRAİGHT FİT 243/4</t>
+  </si>
+  <si>
+    <t>243-4.jpg</t>
+  </si>
+  <si>
+    <t>STRAİGHT FİT 243/5</t>
+  </si>
+  <si>
+    <t>243-5.jpg</t>
+  </si>
+  <si>
+    <t>STRAİGHT FİT 243/2</t>
+  </si>
+  <si>
+    <t>243-2.jpg</t>
   </si>
 </sst>
 </file>
@@ -1322,10 +1379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F124"/>
+  <dimension ref="A1:F132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="D140" sqref="D140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3815,6 +3872,166 @@
         <v>6</v>
       </c>
     </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>303</v>
+      </c>
+      <c r="B125" t="s">
+        <v>304</v>
+      </c>
+      <c r="C125" t="s">
+        <v>7</v>
+      </c>
+      <c r="D125" t="s">
+        <v>302</v>
+      </c>
+      <c r="E125" t="s">
+        <v>305</v>
+      </c>
+      <c r="F125" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>307</v>
+      </c>
+      <c r="B126" t="s">
+        <v>304</v>
+      </c>
+      <c r="C126" t="s">
+        <v>7</v>
+      </c>
+      <c r="D126" t="s">
+        <v>308</v>
+      </c>
+      <c r="E126" t="s">
+        <v>305</v>
+      </c>
+      <c r="F126" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>309</v>
+      </c>
+      <c r="B127" t="s">
+        <v>304</v>
+      </c>
+      <c r="C127" t="s">
+        <v>7</v>
+      </c>
+      <c r="D127" t="s">
+        <v>310</v>
+      </c>
+      <c r="E127" t="s">
+        <v>305</v>
+      </c>
+      <c r="F127" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>311</v>
+      </c>
+      <c r="B128" t="s">
+        <v>304</v>
+      </c>
+      <c r="C128" t="s">
+        <v>7</v>
+      </c>
+      <c r="D128" t="s">
+        <v>312</v>
+      </c>
+      <c r="E128" t="s">
+        <v>305</v>
+      </c>
+      <c r="F128" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>313</v>
+      </c>
+      <c r="B129" t="s">
+        <v>304</v>
+      </c>
+      <c r="C129" t="s">
+        <v>7</v>
+      </c>
+      <c r="D129" t="s">
+        <v>314</v>
+      </c>
+      <c r="E129" t="s">
+        <v>305</v>
+      </c>
+      <c r="F129" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>315</v>
+      </c>
+      <c r="B130" t="s">
+        <v>304</v>
+      </c>
+      <c r="C130" t="s">
+        <v>7</v>
+      </c>
+      <c r="D130" t="s">
+        <v>316</v>
+      </c>
+      <c r="E130" t="s">
+        <v>305</v>
+      </c>
+      <c r="F130" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>317</v>
+      </c>
+      <c r="B131" t="s">
+        <v>304</v>
+      </c>
+      <c r="C131" t="s">
+        <v>7</v>
+      </c>
+      <c r="D131" t="s">
+        <v>318</v>
+      </c>
+      <c r="E131" t="s">
+        <v>305</v>
+      </c>
+      <c r="F131" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>319</v>
+      </c>
+      <c r="B132" t="s">
+        <v>304</v>
+      </c>
+      <c r="C132" t="s">
+        <v>7</v>
+      </c>
+      <c r="D132" t="s">
+        <v>320</v>
+      </c>
+      <c r="E132" t="s">
+        <v>305</v>
+      </c>
+      <c r="F132" t="s">
+        <v>306</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>